<commit_message>
Add screenshot w/ name, add delete files on exit, add test cases, create multiple testclasses
</commit_message>
<xml_diff>
--- a/Test_Cases.xlsx
+++ b/Test_Cases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vivike\Desktop\autotesting\vizsgaremeknew\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFDE46E2-369E-4D94-8B89-6D7AE4E570AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98520605-6F0D-49DD-8B1F-1846B192B7B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34260" yWindow="2910" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="tesztesetek (test case)" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="598" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="604" uniqueCount="156">
   <si>
     <t>Azonosító (ID)</t>
   </si>
@@ -468,9 +468,6 @@
     <t>Profil törlése után nem lehetséges bejelentkezni a törölttel megegyező adatokkal</t>
   </si>
   <si>
-    <t>Az oldalon konzisztens a heading-ek szövegstílusa, betűtípusa</t>
-  </si>
-  <si>
     <t>Betűtípus a headingeknél megegyezik az oldalon</t>
   </si>
   <si>
@@ -534,9 +531,6 @@
     <t>Profil törlése ellenőrzése</t>
   </si>
   <si>
-    <t>Heading szövegstílus ellenőrzése</t>
-  </si>
-  <si>
     <t>TC20</t>
   </si>
   <si>
@@ -555,22 +549,51 @@
     <t>TC25</t>
   </si>
   <si>
-    <t>Kép ellenőrzése</t>
+    <t>h2 Heading szövegstílus ellenőrzése</t>
   </si>
   <si>
-    <t>Képek ellenőrzése a felületen</t>
+    <t>Az oldalon konzisztens a  h2 heading-ek szövegstílusa, betűtípusa</t>
   </si>
   <si>
-    <t xml:space="preserve">1. Navigálj a portioUrl oldalra
+    <t>Keskeny nézet ellenőrzés</t>
+  </si>
+  <si>
+    <t>Profil módosítása</t>
+  </si>
+  <si>
+    <t>Képek ellenőrzése a Work oldalon</t>
+  </si>
+  <si>
+    <t>Képek ellenőrzése</t>
+  </si>
+  <si>
+    <t>4 db .png fájl konzisztens a bejegyzések címével</t>
+  </si>
+  <si>
+    <t>4 db .png fájl
+CaseStudyOne.png
+EventAppCaseStudy.png
+RecipeAppUxStudy.png
+UXCaseStudyforAgricultureApp.png</t>
+  </si>
+  <si>
+    <t>1. Navigálj a portioUrl oldalra
 2. Sikeres regisztráció
 3. Sikeres bejelentkezés
-4. </t>
+4. H2 headingek ellenőrzése</t>
   </si>
   <si>
-    <t>.img fájl</t>
+    <t>1. Navigálj a portioUrl oldalra
+2. Sikeres regisztráció
+3. Sikeres bejelentkezés
+4. Work gomb megnyomása
+5. Bejegyzésekhez társított képek ellenőrzése</t>
   </si>
   <si>
-    <t>.img fájl lementve sajátgépre</t>
+    <t>Keskeny nézetben a navBar hamburger menüre vált</t>
+  </si>
+  <si>
+    <t>képernyő méret = 980x540px</t>
   </si>
 </sst>
 </file>
@@ -2460,8 +2483,8 @@
   <dimension ref="A1:Y1008"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H22" sqref="H22"/>
+      <pane ySplit="1" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1"/>
@@ -2473,7 +2496,7 @@
     <col min="5" max="5" width="10.75" style="2" customWidth="1"/>
     <col min="6" max="6" width="11.75" customWidth="1"/>
     <col min="7" max="7" width="23.25" customWidth="1"/>
-    <col min="8" max="8" width="23" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="28" customWidth="1"/>
     <col min="9" max="9" width="25.375" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="32" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="16.25" customWidth="1"/>
@@ -2583,7 +2606,7 @@
         <v>14</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>55</v>
@@ -2630,7 +2653,7 @@
         <v>15</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>56</v>
@@ -2677,7 +2700,7 @@
         <v>16</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>57</v>
@@ -2724,7 +2747,7 @@
         <v>17</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>58</v>
@@ -2771,7 +2794,7 @@
         <v>18</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>59</v>
@@ -2863,7 +2886,7 @@
         <v>20</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C9" s="5" t="s">
         <v>62</v>
@@ -2910,7 +2933,7 @@
         <v>21</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C10" s="5" t="s">
         <v>107</v>
@@ -2957,7 +2980,7 @@
         <v>22</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C11" s="5" t="s">
         <v>63</v>
@@ -3004,10 +3027,10 @@
         <v>23</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>65</v>
@@ -3051,10 +3074,10 @@
         <v>24</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D13" s="3" t="s">
         <v>65</v>
@@ -3098,7 +3121,7 @@
         <v>25</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>94</v>
@@ -3192,7 +3215,7 @@
         <v>27</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C16" s="5" t="s">
         <v>101</v>
@@ -3239,7 +3262,7 @@
         <v>28</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C17" s="5" t="s">
         <v>102</v>
@@ -3257,7 +3280,7 @@
         <v>98</v>
       </c>
       <c r="H17" s="5" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="I17" s="5" t="s">
         <v>104</v>
@@ -3286,7 +3309,7 @@
         <v>29</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C18" s="5" t="s">
         <v>114</v>
@@ -3333,7 +3356,7 @@
         <v>30</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C19" s="5" t="s">
         <v>115</v>
@@ -3375,15 +3398,15 @@
       <c r="X19" s="2"/>
       <c r="Y19" s="2"/>
     </row>
-    <row r="20" spans="1:25" ht="37.5" thickTop="1" thickBot="1">
+    <row r="20" spans="1:25" ht="49.5" thickTop="1" thickBot="1">
       <c r="A20" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B20" s="3" t="s">
-        <v>139</v>
+      <c r="B20" s="16" t="s">
+        <v>144</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>118</v>
+        <v>145</v>
       </c>
       <c r="D20" s="3" t="s">
         <v>65</v>
@@ -3395,16 +3418,16 @@
         <v>49</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>103</v>
+        <v>152</v>
       </c>
       <c r="H20" s="5" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="I20" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="J20" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="K20" s="5"/>
       <c r="L20" s="4"/>
@@ -3422,15 +3445,15 @@
       <c r="X20" s="2"/>
       <c r="Y20" s="2"/>
     </row>
-    <row r="21" spans="1:25" s="14" customFormat="1" ht="49.5" thickTop="1" thickBot="1">
-      <c r="A21" s="19" t="s">
-        <v>140</v>
+    <row r="21" spans="1:25" s="14" customFormat="1" ht="73.5" thickTop="1" thickBot="1">
+      <c r="A21" s="16" t="s">
+        <v>138</v>
       </c>
       <c r="B21" s="16" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="C21" s="18" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="D21" s="16" t="s">
         <v>65</v>
@@ -3442,10 +3465,10 @@
         <v>49</v>
       </c>
       <c r="G21" s="16" t="s">
-        <v>148</v>
+        <v>153</v>
       </c>
       <c r="H21" s="18" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="I21" s="18" t="s">
         <v>150</v>
@@ -3471,15 +3494,19 @@
     </row>
     <row r="22" spans="1:25" ht="37.5" thickTop="1" thickBot="1">
       <c r="A22" s="16" t="s">
-        <v>141</v>
-      </c>
-      <c r="B22" s="3"/>
-      <c r="C22" s="5"/>
+        <v>139</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>154</v>
+      </c>
       <c r="D22" s="3" t="s">
         <v>65</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>12</v>
+        <v>109</v>
       </c>
       <c r="F22" s="3" t="s">
         <v>49</v>
@@ -3487,9 +3514,15 @@
       <c r="G22" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="H22" s="5"/>
-      <c r="I22" s="5"/>
-      <c r="J22" s="5"/>
+      <c r="H22" s="18" t="s">
+        <v>155</v>
+      </c>
+      <c r="I22" s="18" t="s">
+        <v>154</v>
+      </c>
+      <c r="J22" s="18" t="s">
+        <v>154</v>
+      </c>
       <c r="K22" s="5"/>
       <c r="L22" s="4"/>
       <c r="M22" s="2"/>
@@ -3507,10 +3540,12 @@
       <c r="Y22" s="2"/>
     </row>
     <row r="23" spans="1:25" ht="85.5" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A23" s="3" t="s">
-        <v>142</v>
-      </c>
-      <c r="B23" s="3"/>
+      <c r="A23" s="19" t="s">
+        <v>140</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>147</v>
+      </c>
       <c r="C23" s="5"/>
       <c r="D23" s="3" t="s">
         <v>65</v>
@@ -3544,8 +3579,8 @@
       <c r="Y23" s="2"/>
     </row>
     <row r="24" spans="1:25" ht="37.5" thickTop="1" thickBot="1">
-      <c r="A24" s="3" t="s">
-        <v>143</v>
+      <c r="A24" s="16" t="s">
+        <v>141</v>
       </c>
       <c r="B24" s="3"/>
       <c r="C24" s="5"/>
@@ -3581,8 +3616,8 @@
       <c r="Y24" s="2"/>
     </row>
     <row r="25" spans="1:25" ht="37.5" thickTop="1" thickBot="1">
-      <c r="A25" s="3" t="s">
-        <v>144</v>
+      <c r="A25" s="16" t="s">
+        <v>142</v>
       </c>
       <c r="B25" s="3"/>
       <c r="C25" s="5"/>
@@ -3618,8 +3653,8 @@
       <c r="Y25" s="2"/>
     </row>
     <row r="26" spans="1:25" ht="60" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A26" s="3" t="s">
-        <v>145</v>
+      <c r="A26" s="16" t="s">
+        <v>143</v>
       </c>
       <c r="B26" s="3"/>
       <c r="C26" s="5"/>
@@ -10343,857 +10378,857 @@
   </sheetData>
   <phoneticPr fontId="7" type="noConversion"/>
   <conditionalFormatting sqref="E22:E109 E2:E17">
-    <cfRule type="cellIs" dxfId="182" priority="235" operator="equal">
+    <cfRule type="cellIs" dxfId="182" priority="259" operator="equal">
       <formula>"Alacsony"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E22:E109 E2:E17">
-    <cfRule type="cellIs" dxfId="181" priority="236" operator="equal">
+    <cfRule type="cellIs" dxfId="181" priority="260" operator="equal">
       <formula>"Normál"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E22:E109 E2:E17">
-    <cfRule type="cellIs" dxfId="180" priority="237" operator="equal">
+    <cfRule type="cellIs" dxfId="180" priority="261" operator="equal">
       <formula>"Magas"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K70:K84 K26:K61 K11 K3:K8 K22 K13:K17">
-    <cfRule type="cellIs" dxfId="179" priority="238" operator="equal">
+    <cfRule type="cellIs" dxfId="179" priority="262" operator="equal">
       <formula>"Siker"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K70:K84 K26:K61 K11 K3:K8 K22 K13:K17">
-    <cfRule type="cellIs" dxfId="178" priority="239" operator="equal">
+    <cfRule type="cellIs" dxfId="178" priority="263" operator="equal">
       <formula>"Nem futtatható"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K70:K84 K26:K61 K11 K3:K8 K22 K13:K17">
-    <cfRule type="cellIs" dxfId="177" priority="240" operator="equal">
+    <cfRule type="cellIs" dxfId="177" priority="264" operator="equal">
       <formula>"Hiba"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E11">
-    <cfRule type="cellIs" dxfId="176" priority="226" operator="equal">
+    <cfRule type="cellIs" dxfId="176" priority="250" operator="equal">
       <formula>"Alacsony"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E11">
-    <cfRule type="cellIs" dxfId="175" priority="227" operator="equal">
+    <cfRule type="cellIs" dxfId="175" priority="251" operator="equal">
       <formula>"Normál"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E11">
-    <cfRule type="cellIs" dxfId="174" priority="228" operator="equal">
+    <cfRule type="cellIs" dxfId="174" priority="252" operator="equal">
       <formula>"Magas"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K12">
-    <cfRule type="cellIs" dxfId="173" priority="220" operator="equal">
+    <cfRule type="cellIs" dxfId="173" priority="244" operator="equal">
       <formula>"Siker"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K12">
-    <cfRule type="cellIs" dxfId="172" priority="221" operator="equal">
+    <cfRule type="cellIs" dxfId="172" priority="245" operator="equal">
       <formula>"Nem futtatható"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K12">
-    <cfRule type="cellIs" dxfId="171" priority="222" operator="equal">
+    <cfRule type="cellIs" dxfId="171" priority="246" operator="equal">
       <formula>"Hiba"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E12">
-    <cfRule type="cellIs" dxfId="170" priority="217" operator="equal">
+    <cfRule type="cellIs" dxfId="170" priority="241" operator="equal">
       <formula>"Alacsony"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E12">
-    <cfRule type="cellIs" dxfId="169" priority="218" operator="equal">
+    <cfRule type="cellIs" dxfId="169" priority="242" operator="equal">
       <formula>"Normál"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E12">
-    <cfRule type="cellIs" dxfId="168" priority="219" operator="equal">
+    <cfRule type="cellIs" dxfId="168" priority="243" operator="equal">
       <formula>"Magas"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E24">
-    <cfRule type="cellIs" dxfId="167" priority="208" operator="equal">
+    <cfRule type="cellIs" dxfId="167" priority="232" operator="equal">
       <formula>"Alacsony"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E24">
-    <cfRule type="cellIs" dxfId="166" priority="209" operator="equal">
+    <cfRule type="cellIs" dxfId="166" priority="233" operator="equal">
       <formula>"Normál"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E24">
-    <cfRule type="cellIs" dxfId="165" priority="210" operator="equal">
+    <cfRule type="cellIs" dxfId="165" priority="234" operator="equal">
       <formula>"Magas"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K24">
-    <cfRule type="cellIs" dxfId="164" priority="211" operator="equal">
+    <cfRule type="cellIs" dxfId="164" priority="235" operator="equal">
       <formula>"Siker"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K24">
-    <cfRule type="cellIs" dxfId="163" priority="212" operator="equal">
+    <cfRule type="cellIs" dxfId="163" priority="236" operator="equal">
       <formula>"Nem futtatható"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K24">
-    <cfRule type="cellIs" dxfId="162" priority="213" operator="equal">
+    <cfRule type="cellIs" dxfId="162" priority="237" operator="equal">
       <formula>"Hiba"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E25">
-    <cfRule type="cellIs" dxfId="161" priority="202" operator="equal">
+    <cfRule type="cellIs" dxfId="161" priority="226" operator="equal">
       <formula>"Alacsony"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E25">
-    <cfRule type="cellIs" dxfId="160" priority="203" operator="equal">
+    <cfRule type="cellIs" dxfId="160" priority="227" operator="equal">
       <formula>"Normál"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E25">
-    <cfRule type="cellIs" dxfId="159" priority="204" operator="equal">
+    <cfRule type="cellIs" dxfId="159" priority="228" operator="equal">
       <formula>"Magas"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K25">
-    <cfRule type="cellIs" dxfId="158" priority="205" operator="equal">
+    <cfRule type="cellIs" dxfId="158" priority="229" operator="equal">
       <formula>"Siker"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K25">
-    <cfRule type="cellIs" dxfId="157" priority="206" operator="equal">
+    <cfRule type="cellIs" dxfId="157" priority="230" operator="equal">
       <formula>"Nem futtatható"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K25">
-    <cfRule type="cellIs" dxfId="156" priority="207" operator="equal">
+    <cfRule type="cellIs" dxfId="156" priority="231" operator="equal">
       <formula>"Hiba"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E26">
-    <cfRule type="cellIs" dxfId="155" priority="199" operator="equal">
+    <cfRule type="cellIs" dxfId="155" priority="223" operator="equal">
       <formula>"Alacsony"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E26">
-    <cfRule type="cellIs" dxfId="154" priority="200" operator="equal">
+    <cfRule type="cellIs" dxfId="154" priority="224" operator="equal">
       <formula>"Normál"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E26">
-    <cfRule type="cellIs" dxfId="153" priority="201" operator="equal">
+    <cfRule type="cellIs" dxfId="153" priority="225" operator="equal">
       <formula>"Magas"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E62:E65">
-    <cfRule type="cellIs" dxfId="152" priority="187" operator="equal">
+    <cfRule type="cellIs" dxfId="152" priority="211" operator="equal">
       <formula>"Alacsony"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E62:E65">
-    <cfRule type="cellIs" dxfId="151" priority="188" operator="equal">
+    <cfRule type="cellIs" dxfId="151" priority="212" operator="equal">
       <formula>"Normál"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E62:E65">
-    <cfRule type="cellIs" dxfId="150" priority="189" operator="equal">
+    <cfRule type="cellIs" dxfId="150" priority="213" operator="equal">
       <formula>"Magas"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K62:K65">
-    <cfRule type="cellIs" dxfId="149" priority="190" operator="equal">
+    <cfRule type="cellIs" dxfId="149" priority="214" operator="equal">
       <formula>"Siker"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K62:K65">
-    <cfRule type="cellIs" dxfId="148" priority="191" operator="equal">
+    <cfRule type="cellIs" dxfId="148" priority="215" operator="equal">
       <formula>"Nem futtatható"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K62:K65">
-    <cfRule type="cellIs" dxfId="147" priority="192" operator="equal">
+    <cfRule type="cellIs" dxfId="147" priority="216" operator="equal">
       <formula>"Hiba"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E66">
-    <cfRule type="cellIs" dxfId="146" priority="181" operator="equal">
+    <cfRule type="cellIs" dxfId="146" priority="205" operator="equal">
       <formula>"Alacsony"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E66">
-    <cfRule type="cellIs" dxfId="145" priority="182" operator="equal">
+    <cfRule type="cellIs" dxfId="145" priority="206" operator="equal">
       <formula>"Normál"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E66">
-    <cfRule type="cellIs" dxfId="144" priority="183" operator="equal">
+    <cfRule type="cellIs" dxfId="144" priority="207" operator="equal">
       <formula>"Magas"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K66:K67">
-    <cfRule type="cellIs" dxfId="143" priority="184" operator="equal">
+    <cfRule type="cellIs" dxfId="143" priority="208" operator="equal">
       <formula>"Siker"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K66:K67">
-    <cfRule type="cellIs" dxfId="142" priority="185" operator="equal">
+    <cfRule type="cellIs" dxfId="142" priority="209" operator="equal">
       <formula>"Nem futtatható"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K66:K67">
-    <cfRule type="cellIs" dxfId="141" priority="186" operator="equal">
+    <cfRule type="cellIs" dxfId="141" priority="210" operator="equal">
       <formula>"Hiba"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E67">
-    <cfRule type="cellIs" dxfId="140" priority="172" operator="equal">
+    <cfRule type="cellIs" dxfId="140" priority="196" operator="equal">
       <formula>"Alacsony"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E67">
-    <cfRule type="cellIs" dxfId="139" priority="173" operator="equal">
+    <cfRule type="cellIs" dxfId="139" priority="197" operator="equal">
       <formula>"Normál"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E67">
-    <cfRule type="cellIs" dxfId="138" priority="174" operator="equal">
+    <cfRule type="cellIs" dxfId="138" priority="198" operator="equal">
       <formula>"Magas"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E68">
-    <cfRule type="cellIs" dxfId="137" priority="166" operator="equal">
+    <cfRule type="cellIs" dxfId="137" priority="190" operator="equal">
       <formula>"Alacsony"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E68">
-    <cfRule type="cellIs" dxfId="136" priority="167" operator="equal">
+    <cfRule type="cellIs" dxfId="136" priority="191" operator="equal">
       <formula>"Normál"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E68">
-    <cfRule type="cellIs" dxfId="135" priority="168" operator="equal">
+    <cfRule type="cellIs" dxfId="135" priority="192" operator="equal">
       <formula>"Magas"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K68">
-    <cfRule type="cellIs" dxfId="134" priority="169" operator="equal">
+    <cfRule type="cellIs" dxfId="134" priority="193" operator="equal">
       <formula>"Siker"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K68">
-    <cfRule type="cellIs" dxfId="133" priority="170" operator="equal">
+    <cfRule type="cellIs" dxfId="133" priority="194" operator="equal">
       <formula>"Nem futtatható"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K68">
-    <cfRule type="cellIs" dxfId="132" priority="171" operator="equal">
+    <cfRule type="cellIs" dxfId="132" priority="195" operator="equal">
       <formula>"Hiba"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E69">
-    <cfRule type="cellIs" dxfId="131" priority="142" operator="equal">
+    <cfRule type="cellIs" dxfId="131" priority="166" operator="equal">
       <formula>"Alacsony"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E69">
-    <cfRule type="cellIs" dxfId="130" priority="143" operator="equal">
+    <cfRule type="cellIs" dxfId="130" priority="167" operator="equal">
       <formula>"Normál"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E69">
-    <cfRule type="cellIs" dxfId="129" priority="144" operator="equal">
+    <cfRule type="cellIs" dxfId="129" priority="168" operator="equal">
       <formula>"Magas"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K69">
-    <cfRule type="cellIs" dxfId="128" priority="145" operator="equal">
+    <cfRule type="cellIs" dxfId="128" priority="169" operator="equal">
       <formula>"Siker"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K69">
-    <cfRule type="cellIs" dxfId="127" priority="146" operator="equal">
+    <cfRule type="cellIs" dxfId="127" priority="170" operator="equal">
       <formula>"Nem futtatható"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K69">
-    <cfRule type="cellIs" dxfId="126" priority="147" operator="equal">
+    <cfRule type="cellIs" dxfId="126" priority="171" operator="equal">
       <formula>"Hiba"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E85:E89 E93:E104">
-    <cfRule type="cellIs" dxfId="125" priority="127" operator="equal">
+    <cfRule type="cellIs" dxfId="125" priority="151" operator="equal">
       <formula>"Alacsony"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E85:E89 E93:E104">
-    <cfRule type="cellIs" dxfId="124" priority="128" operator="equal">
+    <cfRule type="cellIs" dxfId="124" priority="152" operator="equal">
       <formula>"Normál"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E85:E89 E93:E104">
-    <cfRule type="cellIs" dxfId="123" priority="129" operator="equal">
+    <cfRule type="cellIs" dxfId="123" priority="153" operator="equal">
       <formula>"Magas"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K85:K90 K92:K104 K107:K110">
-    <cfRule type="cellIs" dxfId="122" priority="130" operator="equal">
+    <cfRule type="cellIs" dxfId="122" priority="154" operator="equal">
       <formula>"Siker"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K85:K90 K92:K104 K107:K110">
-    <cfRule type="cellIs" dxfId="121" priority="131" operator="equal">
+    <cfRule type="cellIs" dxfId="121" priority="155" operator="equal">
       <formula>"Nem futtatható"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K85:K90 K92:K104 K107:K110">
-    <cfRule type="cellIs" dxfId="120" priority="132" operator="equal">
+    <cfRule type="cellIs" dxfId="120" priority="156" operator="equal">
       <formula>"Hiba"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E90">
-    <cfRule type="cellIs" dxfId="119" priority="124" operator="equal">
+    <cfRule type="cellIs" dxfId="119" priority="148" operator="equal">
       <formula>"Alacsony"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E90">
-    <cfRule type="cellIs" dxfId="118" priority="125" operator="equal">
+    <cfRule type="cellIs" dxfId="118" priority="149" operator="equal">
       <formula>"Normál"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E90">
-    <cfRule type="cellIs" dxfId="117" priority="126" operator="equal">
+    <cfRule type="cellIs" dxfId="117" priority="150" operator="equal">
       <formula>"Magas"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K91">
-    <cfRule type="cellIs" dxfId="116" priority="121" operator="equal">
+    <cfRule type="cellIs" dxfId="116" priority="145" operator="equal">
       <formula>"Siker"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K91">
-    <cfRule type="cellIs" dxfId="115" priority="122" operator="equal">
+    <cfRule type="cellIs" dxfId="115" priority="146" operator="equal">
       <formula>"Nem futtatható"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K91">
-    <cfRule type="cellIs" dxfId="114" priority="123" operator="equal">
+    <cfRule type="cellIs" dxfId="114" priority="147" operator="equal">
       <formula>"Hiba"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E91">
-    <cfRule type="cellIs" dxfId="113" priority="118" operator="equal">
+    <cfRule type="cellIs" dxfId="113" priority="142" operator="equal">
       <formula>"Alacsony"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E91">
-    <cfRule type="cellIs" dxfId="112" priority="119" operator="equal">
+    <cfRule type="cellIs" dxfId="112" priority="143" operator="equal">
       <formula>"Normál"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E91">
-    <cfRule type="cellIs" dxfId="111" priority="120" operator="equal">
+    <cfRule type="cellIs" dxfId="111" priority="144" operator="equal">
       <formula>"Magas"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E92">
-    <cfRule type="cellIs" dxfId="110" priority="115" operator="equal">
+    <cfRule type="cellIs" dxfId="110" priority="139" operator="equal">
       <formula>"Alacsony"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E92">
-    <cfRule type="cellIs" dxfId="109" priority="116" operator="equal">
+    <cfRule type="cellIs" dxfId="109" priority="140" operator="equal">
       <formula>"Normál"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E92">
-    <cfRule type="cellIs" dxfId="108" priority="117" operator="equal">
+    <cfRule type="cellIs" dxfId="108" priority="141" operator="equal">
       <formula>"Magas"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E105">
-    <cfRule type="cellIs" dxfId="107" priority="109" operator="equal">
+    <cfRule type="cellIs" dxfId="107" priority="133" operator="equal">
       <formula>"Alacsony"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E105">
-    <cfRule type="cellIs" dxfId="106" priority="110" operator="equal">
+    <cfRule type="cellIs" dxfId="106" priority="134" operator="equal">
       <formula>"Normál"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E105">
-    <cfRule type="cellIs" dxfId="105" priority="111" operator="equal">
+    <cfRule type="cellIs" dxfId="105" priority="135" operator="equal">
       <formula>"Magas"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K105">
-    <cfRule type="cellIs" dxfId="104" priority="112" operator="equal">
+    <cfRule type="cellIs" dxfId="104" priority="136" operator="equal">
       <formula>"Siker"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K105">
-    <cfRule type="cellIs" dxfId="103" priority="113" operator="equal">
+    <cfRule type="cellIs" dxfId="103" priority="137" operator="equal">
       <formula>"Nem futtatható"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K105">
-    <cfRule type="cellIs" dxfId="102" priority="114" operator="equal">
+    <cfRule type="cellIs" dxfId="102" priority="138" operator="equal">
       <formula>"Hiba"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E106">
-    <cfRule type="cellIs" dxfId="101" priority="103" operator="equal">
+    <cfRule type="cellIs" dxfId="101" priority="127" operator="equal">
       <formula>"Alacsony"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E106">
-    <cfRule type="cellIs" dxfId="100" priority="104" operator="equal">
+    <cfRule type="cellIs" dxfId="100" priority="128" operator="equal">
       <formula>"Normál"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E106">
-    <cfRule type="cellIs" dxfId="99" priority="105" operator="equal">
+    <cfRule type="cellIs" dxfId="99" priority="129" operator="equal">
       <formula>"Magas"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K106">
-    <cfRule type="cellIs" dxfId="98" priority="106" operator="equal">
+    <cfRule type="cellIs" dxfId="98" priority="130" operator="equal">
       <formula>"Siker"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K106">
-    <cfRule type="cellIs" dxfId="97" priority="107" operator="equal">
+    <cfRule type="cellIs" dxfId="97" priority="131" operator="equal">
       <formula>"Nem futtatható"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K106">
-    <cfRule type="cellIs" dxfId="96" priority="108" operator="equal">
+    <cfRule type="cellIs" dxfId="96" priority="132" operator="equal">
       <formula>"Hiba"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E107">
-    <cfRule type="cellIs" dxfId="95" priority="100" operator="equal">
+    <cfRule type="cellIs" dxfId="95" priority="124" operator="equal">
       <formula>"Alacsony"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E107">
-    <cfRule type="cellIs" dxfId="94" priority="101" operator="equal">
+    <cfRule type="cellIs" dxfId="94" priority="125" operator="equal">
       <formula>"Normál"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E107">
-    <cfRule type="cellIs" dxfId="93" priority="102" operator="equal">
+    <cfRule type="cellIs" dxfId="93" priority="126" operator="equal">
       <formula>"Magas"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E108:E109">
-    <cfRule type="cellIs" dxfId="92" priority="97" operator="equal">
+    <cfRule type="cellIs" dxfId="92" priority="121" operator="equal">
       <formula>"Alacsony"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E108:E109">
-    <cfRule type="cellIs" dxfId="91" priority="98" operator="equal">
+    <cfRule type="cellIs" dxfId="91" priority="122" operator="equal">
       <formula>"Normál"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E108:E109">
-    <cfRule type="cellIs" dxfId="90" priority="99" operator="equal">
+    <cfRule type="cellIs" dxfId="90" priority="123" operator="equal">
       <formula>"Magas"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2">
-    <cfRule type="cellIs" dxfId="89" priority="79" operator="equal">
+    <cfRule type="cellIs" dxfId="89" priority="103" operator="equal">
       <formula>"Alacsony"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2">
-    <cfRule type="cellIs" dxfId="88" priority="80" operator="equal">
+    <cfRule type="cellIs" dxfId="88" priority="104" operator="equal">
       <formula>"Normál"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2">
-    <cfRule type="cellIs" dxfId="87" priority="81" operator="equal">
+    <cfRule type="cellIs" dxfId="87" priority="105" operator="equal">
       <formula>"Magas"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K2">
-    <cfRule type="cellIs" dxfId="86" priority="82" operator="equal">
+    <cfRule type="cellIs" dxfId="86" priority="106" operator="equal">
       <formula>"Siker"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K2">
-    <cfRule type="cellIs" dxfId="85" priority="83" operator="equal">
+    <cfRule type="cellIs" dxfId="85" priority="107" operator="equal">
       <formula>"Nem futtatható"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K2">
-    <cfRule type="cellIs" dxfId="84" priority="84" operator="equal">
+    <cfRule type="cellIs" dxfId="84" priority="108" operator="equal">
       <formula>"Hiba"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E9:E10">
-    <cfRule type="cellIs" dxfId="83" priority="73" operator="equal">
+    <cfRule type="cellIs" dxfId="83" priority="97" operator="equal">
       <formula>"Alacsony"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E9:E10">
-    <cfRule type="cellIs" dxfId="82" priority="74" operator="equal">
+    <cfRule type="cellIs" dxfId="82" priority="98" operator="equal">
       <formula>"Normál"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E9:E10">
-    <cfRule type="cellIs" dxfId="81" priority="75" operator="equal">
+    <cfRule type="cellIs" dxfId="81" priority="99" operator="equal">
       <formula>"Magas"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K9:K10">
-    <cfRule type="cellIs" dxfId="80" priority="76" operator="equal">
+    <cfRule type="cellIs" dxfId="80" priority="100" operator="equal">
       <formula>"Siker"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K9:K10">
-    <cfRule type="cellIs" dxfId="79" priority="77" operator="equal">
+    <cfRule type="cellIs" dxfId="79" priority="101" operator="equal">
       <formula>"Nem futtatható"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K9:K10">
-    <cfRule type="cellIs" dxfId="78" priority="78" operator="equal">
+    <cfRule type="cellIs" dxfId="78" priority="102" operator="equal">
       <formula>"Hiba"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E10">
-    <cfRule type="cellIs" dxfId="77" priority="67" operator="equal">
+    <cfRule type="cellIs" dxfId="77" priority="91" operator="equal">
       <formula>"Alacsony"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E10">
-    <cfRule type="cellIs" dxfId="76" priority="68" operator="equal">
+    <cfRule type="cellIs" dxfId="76" priority="92" operator="equal">
       <formula>"Normál"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E10">
-    <cfRule type="cellIs" dxfId="75" priority="69" operator="equal">
+    <cfRule type="cellIs" dxfId="75" priority="93" operator="equal">
       <formula>"Magas"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K10">
-    <cfRule type="cellIs" dxfId="74" priority="70" operator="equal">
+    <cfRule type="cellIs" dxfId="74" priority="94" operator="equal">
       <formula>"Siker"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K10">
-    <cfRule type="cellIs" dxfId="73" priority="71" operator="equal">
+    <cfRule type="cellIs" dxfId="73" priority="95" operator="equal">
       <formula>"Nem futtatható"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K10">
-    <cfRule type="cellIs" dxfId="72" priority="72" operator="equal">
+    <cfRule type="cellIs" dxfId="72" priority="96" operator="equal">
       <formula>"Hiba"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E23">
-    <cfRule type="cellIs" dxfId="71" priority="55" operator="equal">
+    <cfRule type="cellIs" dxfId="71" priority="79" operator="equal">
       <formula>"Alacsony"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E23">
-    <cfRule type="cellIs" dxfId="70" priority="56" operator="equal">
+    <cfRule type="cellIs" dxfId="70" priority="80" operator="equal">
       <formula>"Normál"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E23">
-    <cfRule type="cellIs" dxfId="69" priority="57" operator="equal">
+    <cfRule type="cellIs" dxfId="69" priority="81" operator="equal">
       <formula>"Magas"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K23">
-    <cfRule type="cellIs" dxfId="68" priority="58" operator="equal">
+    <cfRule type="cellIs" dxfId="68" priority="82" operator="equal">
       <formula>"Siker"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K23">
-    <cfRule type="cellIs" dxfId="67" priority="59" operator="equal">
+    <cfRule type="cellIs" dxfId="67" priority="83" operator="equal">
       <formula>"Nem futtatható"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K23">
-    <cfRule type="cellIs" dxfId="66" priority="60" operator="equal">
+    <cfRule type="cellIs" dxfId="66" priority="84" operator="equal">
       <formula>"Hiba"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E4">
-    <cfRule type="cellIs" dxfId="65" priority="52" operator="equal">
+    <cfRule type="cellIs" dxfId="65" priority="76" operator="equal">
       <formula>"Alacsony"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E4">
-    <cfRule type="cellIs" dxfId="64" priority="53" operator="equal">
+    <cfRule type="cellIs" dxfId="64" priority="77" operator="equal">
       <formula>"Normál"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E4">
-    <cfRule type="cellIs" dxfId="63" priority="54" operator="equal">
+    <cfRule type="cellIs" dxfId="63" priority="78" operator="equal">
       <formula>"Magas"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E5">
-    <cfRule type="cellIs" dxfId="62" priority="49" operator="equal">
+    <cfRule type="cellIs" dxfId="62" priority="73" operator="equal">
       <formula>"Alacsony"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E5">
-    <cfRule type="cellIs" dxfId="61" priority="50" operator="equal">
+    <cfRule type="cellIs" dxfId="61" priority="74" operator="equal">
       <formula>"Normál"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E5">
-    <cfRule type="cellIs" dxfId="60" priority="51" operator="equal">
+    <cfRule type="cellIs" dxfId="60" priority="75" operator="equal">
       <formula>"Magas"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E6">
-    <cfRule type="cellIs" dxfId="59" priority="46" operator="equal">
+    <cfRule type="cellIs" dxfId="59" priority="70" operator="equal">
       <formula>"Alacsony"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E6">
-    <cfRule type="cellIs" dxfId="58" priority="47" operator="equal">
+    <cfRule type="cellIs" dxfId="58" priority="71" operator="equal">
       <formula>"Normál"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E6">
-    <cfRule type="cellIs" dxfId="57" priority="48" operator="equal">
+    <cfRule type="cellIs" dxfId="57" priority="72" operator="equal">
       <formula>"Magas"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E7">
-    <cfRule type="cellIs" dxfId="56" priority="43" operator="equal">
+    <cfRule type="cellIs" dxfId="56" priority="67" operator="equal">
       <formula>"Alacsony"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E7">
-    <cfRule type="cellIs" dxfId="55" priority="44" operator="equal">
+    <cfRule type="cellIs" dxfId="55" priority="68" operator="equal">
       <formula>"Normál"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E7">
-    <cfRule type="cellIs" dxfId="54" priority="45" operator="equal">
+    <cfRule type="cellIs" dxfId="54" priority="69" operator="equal">
       <formula>"Magas"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E8">
-    <cfRule type="cellIs" dxfId="53" priority="40" operator="equal">
+    <cfRule type="cellIs" dxfId="53" priority="64" operator="equal">
       <formula>"Alacsony"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E8">
-    <cfRule type="cellIs" dxfId="52" priority="41" operator="equal">
+    <cfRule type="cellIs" dxfId="52" priority="65" operator="equal">
       <formula>"Normál"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E8">
-    <cfRule type="cellIs" dxfId="51" priority="42" operator="equal">
+    <cfRule type="cellIs" dxfId="51" priority="66" operator="equal">
       <formula>"Magas"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E11">
-    <cfRule type="cellIs" dxfId="50" priority="37" operator="equal">
+    <cfRule type="cellIs" dxfId="50" priority="61" operator="equal">
       <formula>"Alacsony"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E11">
-    <cfRule type="cellIs" dxfId="49" priority="38" operator="equal">
+    <cfRule type="cellIs" dxfId="49" priority="62" operator="equal">
       <formula>"Normál"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E11">
-    <cfRule type="cellIs" dxfId="48" priority="39" operator="equal">
+    <cfRule type="cellIs" dxfId="48" priority="63" operator="equal">
       <formula>"Magas"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E12">
-    <cfRule type="cellIs" dxfId="47" priority="34" operator="equal">
+    <cfRule type="cellIs" dxfId="47" priority="58" operator="equal">
       <formula>"Alacsony"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E12">
-    <cfRule type="cellIs" dxfId="46" priority="35" operator="equal">
+    <cfRule type="cellIs" dxfId="46" priority="59" operator="equal">
       <formula>"Normál"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E12">
-    <cfRule type="cellIs" dxfId="45" priority="36" operator="equal">
+    <cfRule type="cellIs" dxfId="45" priority="60" operator="equal">
       <formula>"Magas"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E13">
-    <cfRule type="cellIs" dxfId="44" priority="31" operator="equal">
+    <cfRule type="cellIs" dxfId="44" priority="55" operator="equal">
       <formula>"Alacsony"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E13">
-    <cfRule type="cellIs" dxfId="43" priority="32" operator="equal">
+    <cfRule type="cellIs" dxfId="43" priority="56" operator="equal">
       <formula>"Normál"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E13">
-    <cfRule type="cellIs" dxfId="42" priority="33" operator="equal">
+    <cfRule type="cellIs" dxfId="42" priority="57" operator="equal">
       <formula>"Magas"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E14">
-    <cfRule type="cellIs" dxfId="41" priority="28" operator="equal">
+    <cfRule type="cellIs" dxfId="41" priority="52" operator="equal">
       <formula>"Alacsony"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E14">
-    <cfRule type="cellIs" dxfId="40" priority="29" operator="equal">
+    <cfRule type="cellIs" dxfId="40" priority="53" operator="equal">
       <formula>"Normál"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E14">
-    <cfRule type="cellIs" dxfId="39" priority="30" operator="equal">
+    <cfRule type="cellIs" dxfId="39" priority="54" operator="equal">
       <formula>"Magas"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E15">
-    <cfRule type="cellIs" dxfId="38" priority="25" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="49" operator="equal">
       <formula>"Alacsony"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E15">
-    <cfRule type="cellIs" dxfId="37" priority="26" operator="equal">
+    <cfRule type="cellIs" dxfId="37" priority="50" operator="equal">
       <formula>"Normál"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E15">
-    <cfRule type="cellIs" dxfId="36" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="51" operator="equal">
       <formula>"Magas"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E20">
-    <cfRule type="cellIs" dxfId="35" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="43" operator="equal">
       <formula>"Alacsony"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E20">
-    <cfRule type="cellIs" dxfId="34" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="44" operator="equal">
       <formula>"Normál"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E20">
-    <cfRule type="cellIs" dxfId="33" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="45" operator="equal">
       <formula>"Magas"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K20">
-    <cfRule type="cellIs" dxfId="32" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="46" operator="equal">
       <formula>"Siker"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K20">
-    <cfRule type="cellIs" dxfId="31" priority="23" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="47" operator="equal">
       <formula>"Nem futtatható"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K20">
-    <cfRule type="cellIs" dxfId="30" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="48" operator="equal">
       <formula>"Hiba"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E19">
-    <cfRule type="cellIs" dxfId="29" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="37" operator="equal">
       <formula>"Alacsony"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E19">
-    <cfRule type="cellIs" dxfId="28" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="38" operator="equal">
       <formula>"Normál"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E19">
-    <cfRule type="cellIs" dxfId="27" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="39" operator="equal">
       <formula>"Magas"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K19">
-    <cfRule type="cellIs" dxfId="26" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="40" operator="equal">
       <formula>"Siker"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K19">
-    <cfRule type="cellIs" dxfId="25" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="41" operator="equal">
       <formula>"Nem futtatható"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K19">
-    <cfRule type="cellIs" dxfId="24" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="42" operator="equal">
       <formula>"Hiba"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E18">
-    <cfRule type="cellIs" dxfId="23" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="31" operator="equal">
       <formula>"Alacsony"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E18">
-    <cfRule type="cellIs" dxfId="22" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="32" operator="equal">
       <formula>"Normál"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E18">
-    <cfRule type="cellIs" dxfId="21" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="33" operator="equal">
       <formula>"Magas"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K18">
-    <cfRule type="cellIs" dxfId="20" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="34" operator="equal">
       <formula>"Siker"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K18">
-    <cfRule type="cellIs" dxfId="19" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="35" operator="equal">
       <formula>"Nem futtatható"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K18">
-    <cfRule type="cellIs" dxfId="18" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="36" operator="equal">
       <formula>"Hiba"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E21">
-    <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="25" operator="equal">
       <formula>"Alacsony"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E21">
-    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="26" operator="equal">
       <formula>"Normál"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E21">
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="27" operator="equal">
       <formula>"Magas"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K21">
-    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="28" operator="equal">
       <formula>"Siker"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K21">
-    <cfRule type="cellIs" dxfId="1" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="29" operator="equal">
       <formula>"Nem futtatható"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K21">
-    <cfRule type="cellIs" dxfId="0" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="30" operator="equal">
       <formula>"Hiba"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -17306,62 +17341,62 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B6">
-    <cfRule type="cellIs" dxfId="17" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="1" operator="equal">
       <formula>"Alacsony"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B6">
-    <cfRule type="cellIs" dxfId="16" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="2" operator="equal">
       <formula>"Normál"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B6">
-    <cfRule type="cellIs" dxfId="15" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="3" operator="equal">
       <formula>"Magas"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C6:E6">
-    <cfRule type="cellIs" dxfId="14" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="4" operator="equal">
       <formula>"Alacsony"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C6:E6">
-    <cfRule type="cellIs" dxfId="13" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="5" operator="equal">
       <formula>"Normál"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C6:E6">
-    <cfRule type="cellIs" dxfId="12" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="6" operator="equal">
       <formula>"Magas"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B7">
-    <cfRule type="cellIs" dxfId="11" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="7" operator="equal">
       <formula>"Alacsony"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B7">
-    <cfRule type="cellIs" dxfId="10" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="8" operator="equal">
       <formula>"Normál"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B7">
-    <cfRule type="cellIs" dxfId="9" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="9" operator="equal">
       <formula>"Magas"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C7:E7">
-    <cfRule type="cellIs" dxfId="8" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="10" operator="equal">
       <formula>"Alacsony"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C7:E7">
-    <cfRule type="cellIs" dxfId="7" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="11" operator="equal">
       <formula>"Normál"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C7:E7">
-    <cfRule type="cellIs" dxfId="6" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="12" operator="equal">
       <formula>"Magas"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Add tags, use softAssert in multiple data entry tests with testNG, add new directory for data files
</commit_message>
<xml_diff>
--- a/Test_Cases.xlsx
+++ b/Test_Cases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vivike\Desktop\autotesting\vizsgaremeknew\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98520605-6F0D-49DD-8B1F-1846B192B7B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDC8AF4D-1670-4034-A1BD-063CFD9A51F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="604" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="639" uniqueCount="167">
   <si>
     <t>Azonosító (ID)</t>
   </si>
@@ -411,13 +411,6 @@
     <t>A blogposztok címe megegyezik az elvárt szöveggel</t>
   </si>
   <si>
-    <t>1. Navigálj a portioUrl oldalra
-3. Regisztrációhoz olvasd be az adatokat a MOCK_DATA:csv fájlból</t>
-  </si>
-  <si>
-    <t>MOCK_DATA.csv</t>
-  </si>
-  <si>
     <t>Sorozatos regisztráció fájlból adatokkal</t>
   </si>
   <si>
@@ -543,12 +536,6 @@
     <t>TC23</t>
   </si>
   <si>
-    <t>TC24</t>
-  </si>
-  <si>
-    <t>TC25</t>
-  </si>
-  <si>
     <t>h2 Heading szövegstílus ellenőrzése</t>
   </si>
   <si>
@@ -594,6 +581,61 @@
   </si>
   <si>
     <t>képernyő méret = 980x540px</t>
+  </si>
+  <si>
+    <t>1. Navigálj a portioUrl oldalra
+2. Sikeres regisztráció
+3. Sikeres bejelentkezés
+4. Állítsd be a képernyő méretet</t>
+  </si>
+  <si>
+    <t>Felhasználói profil módosítása</t>
+  </si>
+  <si>
+    <t>"Profile Edited!" felirat megjelenik</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"Profile Edited!" felirat megjelenik az </t>
+  </si>
+  <si>
+    <t>1. Navigálj a portioUrl oldalra
+2. Sikeres regisztráció
+3. Sikeres bejelentkezés
+4. Kattints a "Profile" gombra
+5. Töltsd ki a fájl alapján a mezőket
+6. Kattints a "Save Profile" gombra</t>
+  </si>
+  <si>
+    <t>Sorozatos regisztráció invalid email cím</t>
+  </si>
+  <si>
+    <t>1. Navigálj a portioUrl oldalra
+3. Regisztrációhoz olvasd be az adatokat a registrationData.csv fájlból</t>
+  </si>
+  <si>
+    <t>registrationData.csv</t>
+  </si>
+  <si>
+    <t>profileInfoData.csv</t>
+  </si>
+  <si>
+    <t>invalidEmailRegistrationData.csv</t>
+  </si>
+  <si>
+    <t>1. Navigálj a portioUrl oldalra
+3. Regisztrációhoz olvasd be az adatokat a invalidEmailRegistrationData.csv fájlból</t>
+  </si>
+  <si>
+    <t>NEM jelenik meg sikeres regisztrációra utaló felirat</t>
+  </si>
+  <si>
+    <t>Hiba</t>
+  </si>
+  <si>
+    <t>Siker</t>
+  </si>
+  <si>
+    <t>Sorozatos regisztráció különböző, helytelen email címekkel</t>
   </si>
 </sst>
 </file>
@@ -643,7 +685,7 @@
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -666,18 +708,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFFF"/>
         <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor rgb="FFF3F3F3"/>
       </patternFill>
     </fill>
   </fills>
@@ -708,7 +738,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -732,8 +762,6 @@
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -748,14 +776,563 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="183">
+  <dxfs count="252">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFEA9999"/>
+          <bgColor rgb="FFEA9999"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFE598"/>
+          <bgColor rgb="FFFFE598"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFEA9999"/>
+          <bgColor rgb="FFEA9999"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFE598"/>
+          <bgColor rgb="FFFFE598"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFEA9999"/>
+          <bgColor rgb="FFEA9999"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFE598"/>
+          <bgColor rgb="FFFFE598"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFEA9999"/>
+          <bgColor rgb="FFEA9999"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFE598"/>
+          <bgColor rgb="FFFFE598"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFEA9999"/>
+          <bgColor rgb="FFEA9999"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFE598"/>
+          <bgColor rgb="FFFFE598"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFEA9999"/>
+          <bgColor rgb="FFEA9999"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFE598"/>
+          <bgColor rgb="FFFFE598"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFEA9999"/>
+          <bgColor rgb="FFEA9999"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFE598"/>
+          <bgColor rgb="FFFFE598"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFEA9999"/>
+          <bgColor rgb="FFEA9999"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFE598"/>
+          <bgColor rgb="FFFFE598"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFEA9999"/>
+          <bgColor rgb="FFEA9999"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFE598"/>
+          <bgColor rgb="FFFFE598"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFEA9999"/>
+          <bgColor rgb="FFEA9999"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFE598"/>
+          <bgColor rgb="FFFFE598"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFEA9999"/>
+          <bgColor rgb="FFEA9999"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFE598"/>
+          <bgColor rgb="FFFFE598"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFEA9999"/>
+          <bgColor rgb="FFEA9999"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFE598"/>
+          <bgColor rgb="FFFFE598"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFEA9999"/>
+          <bgColor rgb="FFEA9999"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFE598"/>
+          <bgColor rgb="FFFFE598"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFEA9999"/>
+          <bgColor rgb="FFEA9999"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFE598"/>
+          <bgColor rgb="FFFFE598"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFEA9999"/>
+          <bgColor rgb="FFEA9999"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFE598"/>
+          <bgColor rgb="FFFFE598"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFEA9999"/>
+          <bgColor rgb="FFEA9999"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFE598"/>
+          <bgColor rgb="FFFFE598"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFEA9999"/>
+          <bgColor rgb="FFEA9999"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFE598"/>
+          <bgColor rgb="FFFFE598"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFEA9999"/>
+          <bgColor rgb="FFEA9999"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFE598"/>
+          <bgColor rgb="FFFFE598"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFEA9999"/>
+          <bgColor rgb="FFEA9999"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFE598"/>
+          <bgColor rgb="FFFFE598"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFEA9999"/>
+          <bgColor rgb="FFEA9999"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFE598"/>
+          <bgColor rgb="FFFFE598"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFEA9999"/>
+          <bgColor rgb="FFEA9999"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFE598"/>
+          <bgColor rgb="FFFFE598"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFEA9999"/>
+          <bgColor rgb="FFEA9999"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFE598"/>
+          <bgColor rgb="FFFFE598"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFEA9999"/>
+          <bgColor rgb="FFEA9999"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFE598"/>
+          <bgColor rgb="FFFFE598"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -2239,13 +2816,13 @@
     <xdr:from>
       <xdr:col>11</xdr:col>
       <xdr:colOff>238125</xdr:colOff>
-      <xdr:row>65</xdr:row>
+      <xdr:row>66</xdr:row>
       <xdr:rowOff>904875</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>1838325</xdr:colOff>
-      <xdr:row>67</xdr:row>
+      <xdr:row>68</xdr:row>
       <xdr:rowOff>190500</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2480,11 +3057,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Y1008"/>
+  <dimension ref="A1:Y1009"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C23" sqref="C23"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1"/>
@@ -2568,7 +3145,7 @@
         <v>65</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>49</v>
@@ -2585,7 +3162,9 @@
       <c r="J2" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="K2" s="3"/>
+      <c r="K2" s="3" t="s">
+        <v>165</v>
+      </c>
       <c r="L2" s="4"/>
       <c r="M2" s="2"/>
       <c r="N2" s="2"/>
@@ -2606,7 +3185,7 @@
         <v>14</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>55</v>
@@ -2615,7 +3194,7 @@
         <v>65</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>49</v>
@@ -2632,7 +3211,9 @@
       <c r="J3" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="K3" s="3"/>
+      <c r="K3" s="14" t="s">
+        <v>165</v>
+      </c>
       <c r="L3" s="4"/>
       <c r="M3" s="2"/>
       <c r="N3" s="2"/>
@@ -2653,7 +3234,7 @@
         <v>15</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>56</v>
@@ -2662,7 +3243,7 @@
         <v>65</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>49</v>
@@ -2679,7 +3260,9 @@
       <c r="J4" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="K4" s="3"/>
+      <c r="K4" s="14" t="s">
+        <v>165</v>
+      </c>
       <c r="L4" s="4"/>
       <c r="M4" s="2"/>
       <c r="N4" s="2"/>
@@ -2700,7 +3283,7 @@
         <v>16</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>57</v>
@@ -2709,7 +3292,7 @@
         <v>65</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="F5" s="3" t="s">
         <v>49</v>
@@ -2726,7 +3309,9 @@
       <c r="J5" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="K5" s="3"/>
+      <c r="K5" s="14" t="s">
+        <v>165</v>
+      </c>
       <c r="L5" s="4"/>
       <c r="M5" s="2"/>
       <c r="N5" s="2"/>
@@ -2747,7 +3332,7 @@
         <v>17</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>58</v>
@@ -2756,7 +3341,7 @@
         <v>65</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="F6" s="3" t="s">
         <v>49</v>
@@ -2773,7 +3358,9 @@
       <c r="J6" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="K6" s="3"/>
+      <c r="K6" s="14" t="s">
+        <v>165</v>
+      </c>
       <c r="L6" s="4"/>
       <c r="M6" s="2"/>
       <c r="N6" s="2"/>
@@ -2794,7 +3381,7 @@
         <v>18</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>59</v>
@@ -2803,7 +3390,7 @@
         <v>65</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="F7" s="3" t="s">
         <v>49</v>
@@ -2820,7 +3407,9 @@
       <c r="J7" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="K7" s="5"/>
+      <c r="K7" s="14" t="s">
+        <v>165</v>
+      </c>
       <c r="L7" s="4"/>
       <c r="M7" s="2"/>
       <c r="N7" s="2"/>
@@ -2850,7 +3439,7 @@
         <v>65</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="F8" s="3" t="s">
         <v>49</v>
@@ -2864,8 +3453,12 @@
       <c r="I8" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="J8" s="5"/>
-      <c r="K8" s="5"/>
+      <c r="J8" s="16" t="s">
+        <v>81</v>
+      </c>
+      <c r="K8" s="5" t="s">
+        <v>164</v>
+      </c>
       <c r="L8" s="4"/>
       <c r="M8" s="2"/>
       <c r="N8" s="2"/>
@@ -2886,7 +3479,7 @@
         <v>20</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C9" s="5" t="s">
         <v>62</v>
@@ -2912,7 +3505,9 @@
       <c r="J9" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="K9" s="5"/>
+      <c r="K9" s="14" t="s">
+        <v>165</v>
+      </c>
       <c r="L9" s="4"/>
       <c r="M9" s="2"/>
       <c r="N9" s="2"/>
@@ -2933,10 +3528,10 @@
         <v>21</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>65</v>
@@ -2948,10 +3543,10 @@
         <v>49</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>105</v>
+        <v>158</v>
       </c>
       <c r="H10" s="5" t="s">
-        <v>106</v>
+        <v>159</v>
       </c>
       <c r="I10" s="5" t="s">
         <v>81</v>
@@ -2959,7 +3554,9 @@
       <c r="J10" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="K10" s="5"/>
+      <c r="K10" s="14" t="s">
+        <v>165</v>
+      </c>
       <c r="L10" s="4"/>
       <c r="M10" s="2"/>
       <c r="N10" s="2"/>
@@ -2975,68 +3572,70 @@
       <c r="X10" s="2"/>
       <c r="Y10" s="2"/>
     </row>
-    <row r="11" spans="1:25" ht="73.5" thickTop="1" thickBot="1">
-      <c r="A11" s="3" t="s">
+    <row r="11" spans="1:25" s="12" customFormat="1" ht="85.5" customHeight="1" thickTop="1" thickBot="1">
+      <c r="A11" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="B11" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="C11" s="5" t="s">
+      <c r="B11" s="14" t="s">
+        <v>157</v>
+      </c>
+      <c r="C11" s="16" t="s">
+        <v>166</v>
+      </c>
+      <c r="D11" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="E11" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="F11" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="G11" s="14" t="s">
+        <v>162</v>
+      </c>
+      <c r="H11" s="16" t="s">
+        <v>161</v>
+      </c>
+      <c r="I11" s="16" t="s">
+        <v>163</v>
+      </c>
+      <c r="J11" s="16" t="s">
+        <v>81</v>
+      </c>
+      <c r="K11" s="16" t="s">
+        <v>164</v>
+      </c>
+      <c r="L11" s="15"/>
+      <c r="M11" s="13"/>
+      <c r="N11" s="13"/>
+      <c r="O11" s="13"/>
+      <c r="P11" s="13"/>
+      <c r="Q11" s="13"/>
+      <c r="R11" s="13"/>
+      <c r="S11" s="13"/>
+      <c r="T11" s="13"/>
+      <c r="U11" s="13"/>
+      <c r="V11" s="13"/>
+      <c r="W11" s="13"/>
+      <c r="X11" s="13"/>
+      <c r="Y11" s="13"/>
+    </row>
+    <row r="12" spans="1:25" ht="73.5" thickTop="1" thickBot="1">
+      <c r="A12" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="C12" s="5" t="s">
         <v>63</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="G11" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="H11" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="I11" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="J11" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="K11" s="5"/>
-      <c r="L11" s="4"/>
-      <c r="M11" s="2"/>
-      <c r="N11" s="2"/>
-      <c r="O11" s="2"/>
-      <c r="P11" s="2"/>
-      <c r="Q11" s="2"/>
-      <c r="R11" s="2"/>
-      <c r="S11" s="2"/>
-      <c r="T11" s="2"/>
-      <c r="U11" s="2"/>
-      <c r="V11" s="2"/>
-      <c r="W11" s="2"/>
-      <c r="X11" s="2"/>
-      <c r="Y11" s="2"/>
-    </row>
-    <row r="12" spans="1:25" ht="73.5" thickTop="1" thickBot="1">
-      <c r="A12" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>127</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>129</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>65</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="F12" s="3" t="s">
         <v>49</v>
@@ -3045,15 +3644,17 @@
         <v>93</v>
       </c>
       <c r="H12" s="5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I12" s="5" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="J12" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="K12" s="5"/>
+        <v>83</v>
+      </c>
+      <c r="K12" s="14" t="s">
+        <v>165</v>
+      </c>
       <c r="L12" s="4"/>
       <c r="M12" s="2"/>
       <c r="N12" s="2"/>
@@ -3069,21 +3670,21 @@
       <c r="X12" s="2"/>
       <c r="Y12" s="2"/>
     </row>
-    <row r="13" spans="1:25" s="10" customFormat="1" ht="73.5" thickTop="1" thickBot="1">
-      <c r="A13" s="3" t="s">
+    <row r="13" spans="1:25" ht="73.5" thickTop="1" thickBot="1">
+      <c r="A13" s="14" t="s">
         <v>24</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>130</v>
+        <v>125</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>127</v>
       </c>
       <c r="D13" s="3" t="s">
         <v>65</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="F13" s="3" t="s">
         <v>49</v>
@@ -3092,62 +3693,66 @@
         <v>93</v>
       </c>
       <c r="H13" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="I13" s="5" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="J13" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="K13" s="3"/>
+        <v>85</v>
+      </c>
+      <c r="K13" s="14" t="s">
+        <v>165</v>
+      </c>
       <c r="L13" s="4"/>
-      <c r="M13" s="9"/>
-      <c r="N13" s="9"/>
-      <c r="O13" s="9"/>
-      <c r="P13" s="9"/>
-      <c r="Q13" s="9"/>
-      <c r="R13" s="9"/>
-      <c r="S13" s="9"/>
-      <c r="T13" s="9"/>
-      <c r="U13" s="9"/>
-      <c r="V13" s="9"/>
-      <c r="W13" s="9"/>
-      <c r="X13" s="9"/>
-      <c r="Y13" s="9"/>
-    </row>
-    <row r="14" spans="1:25" s="10" customFormat="1" ht="49.5" thickTop="1" thickBot="1">
-      <c r="A14" s="3" t="s">
+      <c r="M13" s="2"/>
+      <c r="N13" s="2"/>
+      <c r="O13" s="2"/>
+      <c r="P13" s="2"/>
+      <c r="Q13" s="2"/>
+      <c r="R13" s="2"/>
+      <c r="S13" s="2"/>
+      <c r="T13" s="2"/>
+      <c r="U13" s="2"/>
+      <c r="V13" s="2"/>
+      <c r="W13" s="2"/>
+      <c r="X13" s="2"/>
+      <c r="Y13" s="2"/>
+    </row>
+    <row r="14" spans="1:25" s="10" customFormat="1" ht="73.5" thickTop="1" thickBot="1">
+      <c r="A14" s="14" t="s">
         <v>25</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>94</v>
+        <v>128</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>65</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="F14" s="3" t="s">
         <v>49</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="H14" s="5" t="s">
-        <v>95</v>
+        <v>75</v>
       </c>
       <c r="I14" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="J14" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="K14" s="3"/>
+        <v>84</v>
+      </c>
+      <c r="K14" s="14" t="s">
+        <v>165</v>
+      </c>
       <c r="L14" s="4"/>
       <c r="M14" s="9"/>
       <c r="N14" s="9"/>
@@ -3163,38 +3768,40 @@
       <c r="X14" s="9"/>
       <c r="Y14" s="9"/>
     </row>
-    <row r="15" spans="1:25" s="10" customFormat="1" ht="37.5" thickTop="1" thickBot="1">
-      <c r="A15" s="3" t="s">
+    <row r="15" spans="1:25" s="10" customFormat="1" ht="49.5" thickTop="1" thickBot="1">
+      <c r="A15" s="14" t="s">
         <v>26</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>64</v>
+        <v>129</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>94</v>
       </c>
       <c r="D15" s="3" t="s">
         <v>65</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="F15" s="3" t="s">
         <v>49</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H15" s="5" t="s">
-        <v>86</v>
+        <v>95</v>
       </c>
       <c r="I15" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="J15" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="K15" s="5"/>
+        <v>85</v>
+      </c>
+      <c r="K15" s="14" t="s">
+        <v>165</v>
+      </c>
       <c r="L15" s="4"/>
       <c r="M15" s="9"/>
       <c r="N15" s="9"/>
@@ -3210,38 +3817,40 @@
       <c r="X15" s="9"/>
       <c r="Y15" s="9"/>
     </row>
-    <row r="16" spans="1:25" s="10" customFormat="1" ht="97.5" thickTop="1" thickBot="1">
-      <c r="A16" s="3" t="s">
+    <row r="16" spans="1:25" s="10" customFormat="1" ht="37.5" thickTop="1" thickBot="1">
+      <c r="A16" s="14" t="s">
         <v>27</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>132</v>
+        <v>52</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>101</v>
+        <v>64</v>
       </c>
       <c r="D16" s="3" t="s">
         <v>65</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>12</v>
+        <v>106</v>
       </c>
       <c r="F16" s="3" t="s">
         <v>49</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H16" s="5" t="s">
-        <v>99</v>
+        <v>86</v>
       </c>
       <c r="I16" s="5" t="s">
-        <v>100</v>
+        <v>87</v>
       </c>
       <c r="J16" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="K16" s="5"/>
+        <v>87</v>
+      </c>
+      <c r="K16" s="14" t="s">
+        <v>165</v>
+      </c>
       <c r="L16" s="4"/>
       <c r="M16" s="9"/>
       <c r="N16" s="9"/>
@@ -3257,15 +3866,15 @@
       <c r="X16" s="9"/>
       <c r="Y16" s="9"/>
     </row>
-    <row r="17" spans="1:25" ht="97.5" thickTop="1" thickBot="1">
-      <c r="A17" s="3" t="s">
+    <row r="17" spans="1:25" s="10" customFormat="1" ht="97.5" thickTop="1" thickBot="1">
+      <c r="A17" s="14" t="s">
         <v>28</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D17" s="3" t="s">
         <v>65</v>
@@ -3280,62 +3889,66 @@
         <v>98</v>
       </c>
       <c r="H17" s="5" t="s">
-        <v>134</v>
+        <v>99</v>
       </c>
       <c r="I17" s="5" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="J17" s="5" t="s">
-        <v>104</v>
-      </c>
-      <c r="K17" s="5"/>
+        <v>100</v>
+      </c>
+      <c r="K17" s="14" t="s">
+        <v>165</v>
+      </c>
       <c r="L17" s="4"/>
-      <c r="M17" s="2"/>
-      <c r="N17" s="2"/>
-      <c r="O17" s="2"/>
-      <c r="P17" s="2"/>
-      <c r="Q17" s="2"/>
-      <c r="R17" s="2"/>
-      <c r="S17" s="2"/>
-      <c r="T17" s="2"/>
-      <c r="U17" s="2"/>
-      <c r="V17" s="2"/>
-      <c r="W17" s="2"/>
-      <c r="X17" s="2"/>
-      <c r="Y17" s="2"/>
+      <c r="M17" s="9"/>
+      <c r="N17" s="9"/>
+      <c r="O17" s="9"/>
+      <c r="P17" s="9"/>
+      <c r="Q17" s="9"/>
+      <c r="R17" s="9"/>
+      <c r="S17" s="9"/>
+      <c r="T17" s="9"/>
+      <c r="U17" s="9"/>
+      <c r="V17" s="9"/>
+      <c r="W17" s="9"/>
+      <c r="X17" s="9"/>
+      <c r="Y17" s="9"/>
     </row>
     <row r="18" spans="1:25" ht="97.5" thickTop="1" thickBot="1">
-      <c r="A18" s="3" t="s">
+      <c r="A18" s="14" t="s">
         <v>29</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>114</v>
+        <v>102</v>
       </c>
       <c r="D18" s="3" t="s">
         <v>65</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>108</v>
+        <v>12</v>
       </c>
       <c r="F18" s="3" t="s">
         <v>49</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="H18" s="5" t="s">
-        <v>111</v>
+        <v>132</v>
       </c>
       <c r="I18" s="5" t="s">
-        <v>116</v>
+        <v>104</v>
       </c>
       <c r="J18" s="5" t="s">
-        <v>116</v>
-      </c>
-      <c r="K18" s="5"/>
+        <v>104</v>
+      </c>
+      <c r="K18" s="14" t="s">
+        <v>165</v>
+      </c>
       <c r="L18" s="4"/>
       <c r="M18" s="2"/>
       <c r="N18" s="2"/>
@@ -3351,38 +3964,40 @@
       <c r="X18" s="2"/>
       <c r="Y18" s="2"/>
     </row>
-    <row r="19" spans="1:25" ht="121.5" thickTop="1" thickBot="1">
-      <c r="A19" s="3" t="s">
+    <row r="19" spans="1:25" ht="97.5" thickTop="1" thickBot="1">
+      <c r="A19" s="14" t="s">
         <v>30</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="D19" s="3" t="s">
         <v>65</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="F19" s="3" t="s">
         <v>49</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="H19" s="5" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="I19" s="5" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="J19" s="5" t="s">
-        <v>117</v>
-      </c>
-      <c r="K19" s="5"/>
+        <v>114</v>
+      </c>
+      <c r="K19" s="14" t="s">
+        <v>165</v>
+      </c>
       <c r="L19" s="4"/>
       <c r="M19" s="2"/>
       <c r="N19" s="2"/>
@@ -3398,38 +4013,40 @@
       <c r="X19" s="2"/>
       <c r="Y19" s="2"/>
     </row>
-    <row r="20" spans="1:25" ht="49.5" thickTop="1" thickBot="1">
-      <c r="A20" s="3" t="s">
+    <row r="20" spans="1:25" ht="121.5" thickTop="1" thickBot="1">
+      <c r="A20" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="B20" s="16" t="s">
-        <v>144</v>
+      <c r="B20" s="3" t="s">
+        <v>135</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>145</v>
+        <v>113</v>
       </c>
       <c r="D20" s="3" t="s">
         <v>65</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="F20" s="3" t="s">
         <v>49</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>152</v>
+        <v>110</v>
       </c>
       <c r="H20" s="5" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="I20" s="5" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="J20" s="5" t="s">
-        <v>118</v>
-      </c>
-      <c r="K20" s="5"/>
+        <v>115</v>
+      </c>
+      <c r="K20" s="14" t="s">
+        <v>165</v>
+      </c>
       <c r="L20" s="4"/>
       <c r="M20" s="2"/>
       <c r="N20" s="2"/>
@@ -3445,124 +4062,138 @@
       <c r="X20" s="2"/>
       <c r="Y20" s="2"/>
     </row>
-    <row r="21" spans="1:25" s="14" customFormat="1" ht="73.5" thickTop="1" thickBot="1">
-      <c r="A21" s="16" t="s">
+    <row r="21" spans="1:25" ht="49.5" thickTop="1" thickBot="1">
+      <c r="A21" s="14" t="s">
+        <v>136</v>
+      </c>
+      <c r="B21" s="14" t="s">
+        <v>140</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="G21" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="H21" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="I21" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="J21" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="K21" s="14" t="s">
+        <v>165</v>
+      </c>
+      <c r="L21" s="4"/>
+      <c r="M21" s="2"/>
+      <c r="N21" s="2"/>
+      <c r="O21" s="2"/>
+      <c r="P21" s="2"/>
+      <c r="Q21" s="2"/>
+      <c r="R21" s="2"/>
+      <c r="S21" s="2"/>
+      <c r="T21" s="2"/>
+      <c r="U21" s="2"/>
+      <c r="V21" s="2"/>
+      <c r="W21" s="2"/>
+      <c r="X21" s="2"/>
+      <c r="Y21" s="2"/>
+    </row>
+    <row r="22" spans="1:25" s="12" customFormat="1" ht="73.5" thickTop="1" thickBot="1">
+      <c r="A22" s="14" t="s">
+        <v>137</v>
+      </c>
+      <c r="B22" s="14" t="s">
+        <v>145</v>
+      </c>
+      <c r="C22" s="16" t="s">
+        <v>144</v>
+      </c>
+      <c r="D22" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="E22" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="F22" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="G22" s="14" t="s">
+        <v>149</v>
+      </c>
+      <c r="H22" s="16" t="s">
+        <v>147</v>
+      </c>
+      <c r="I22" s="16" t="s">
+        <v>146</v>
+      </c>
+      <c r="J22" s="16" t="s">
+        <v>146</v>
+      </c>
+      <c r="K22" s="14" t="s">
+        <v>165</v>
+      </c>
+      <c r="L22" s="15"/>
+      <c r="M22" s="13"/>
+      <c r="N22" s="13"/>
+      <c r="O22" s="13"/>
+      <c r="P22" s="13"/>
+      <c r="Q22" s="13"/>
+      <c r="R22" s="13"/>
+      <c r="S22" s="13"/>
+      <c r="T22" s="13"/>
+      <c r="U22" s="13"/>
+      <c r="V22" s="13"/>
+      <c r="W22" s="13"/>
+      <c r="X22" s="13"/>
+      <c r="Y22" s="13"/>
+    </row>
+    <row r="23" spans="1:25" ht="49.5" thickTop="1" thickBot="1">
+      <c r="A23" s="14" t="s">
         <v>138</v>
       </c>
-      <c r="B21" s="16" t="s">
-        <v>149</v>
-      </c>
-      <c r="C21" s="18" t="s">
-        <v>148</v>
-      </c>
-      <c r="D21" s="16" t="s">
-        <v>65</v>
-      </c>
-      <c r="E21" s="16" t="s">
-        <v>12</v>
-      </c>
-      <c r="F21" s="16" t="s">
-        <v>49</v>
-      </c>
-      <c r="G21" s="16" t="s">
-        <v>153</v>
-      </c>
-      <c r="H21" s="18" t="s">
-        <v>151</v>
-      </c>
-      <c r="I21" s="18" t="s">
+      <c r="B23" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="C23" s="5" t="s">
         <v>150</v>
       </c>
-      <c r="J21" s="18" t="s">
-        <v>150</v>
-      </c>
-      <c r="K21" s="18"/>
-      <c r="L21" s="17"/>
-      <c r="M21" s="15"/>
-      <c r="N21" s="15"/>
-      <c r="O21" s="15"/>
-      <c r="P21" s="15"/>
-      <c r="Q21" s="15"/>
-      <c r="R21" s="15"/>
-      <c r="S21" s="15"/>
-      <c r="T21" s="15"/>
-      <c r="U21" s="15"/>
-      <c r="V21" s="15"/>
-      <c r="W21" s="15"/>
-      <c r="X21" s="15"/>
-      <c r="Y21" s="15"/>
-    </row>
-    <row r="22" spans="1:25" ht="37.5" thickTop="1" thickBot="1">
-      <c r="A22" s="16" t="s">
-        <v>139</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>146</v>
-      </c>
-      <c r="C22" s="5" t="s">
-        <v>154</v>
-      </c>
-      <c r="D22" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="E22" s="3" t="s">
-        <v>109</v>
-      </c>
-      <c r="F22" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="G22" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="H22" s="18" t="s">
-        <v>155</v>
-      </c>
-      <c r="I22" s="18" t="s">
-        <v>154</v>
-      </c>
-      <c r="J22" s="18" t="s">
-        <v>154</v>
-      </c>
-      <c r="K22" s="5"/>
-      <c r="L22" s="4"/>
-      <c r="M22" s="2"/>
-      <c r="N22" s="2"/>
-      <c r="O22" s="2"/>
-      <c r="P22" s="2"/>
-      <c r="Q22" s="2"/>
-      <c r="R22" s="2"/>
-      <c r="S22" s="2"/>
-      <c r="T22" s="2"/>
-      <c r="U22" s="2"/>
-      <c r="V22" s="2"/>
-      <c r="W22" s="2"/>
-      <c r="X22" s="2"/>
-      <c r="Y22" s="2"/>
-    </row>
-    <row r="23" spans="1:25" ht="85.5" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A23" s="19" t="s">
-        <v>140</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>147</v>
-      </c>
-      <c r="C23" s="5"/>
       <c r="D23" s="3" t="s">
         <v>65</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>12</v>
+        <v>107</v>
       </c>
       <c r="F23" s="3" t="s">
         <v>49</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="H23" s="5"/>
-      <c r="I23" s="5"/>
-      <c r="J23" s="5"/>
-      <c r="K23" s="5"/>
+        <v>152</v>
+      </c>
+      <c r="H23" s="16" t="s">
+        <v>151</v>
+      </c>
+      <c r="I23" s="16" t="s">
+        <v>150</v>
+      </c>
+      <c r="J23" s="16" t="s">
+        <v>150</v>
+      </c>
+      <c r="K23" s="14" t="s">
+        <v>165</v>
+      </c>
       <c r="L23" s="4"/>
       <c r="M23" s="2"/>
       <c r="N23" s="2"/>
@@ -3578,12 +4209,16 @@
       <c r="X23" s="2"/>
       <c r="Y23" s="2"/>
     </row>
-    <row r="24" spans="1:25" ht="37.5" thickTop="1" thickBot="1">
-      <c r="A24" s="16" t="s">
-        <v>141</v>
-      </c>
-      <c r="B24" s="3"/>
-      <c r="C24" s="5"/>
+    <row r="24" spans="1:25" ht="97.5" thickTop="1" thickBot="1">
+      <c r="A24" s="14" t="s">
+        <v>139</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>153</v>
+      </c>
       <c r="D24" s="3" t="s">
         <v>65</v>
       </c>
@@ -3594,12 +4229,20 @@
         <v>49</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="H24" s="5"/>
-      <c r="I24" s="5"/>
-      <c r="J24" s="5"/>
-      <c r="K24" s="5"/>
+        <v>156</v>
+      </c>
+      <c r="H24" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="I24" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="J24" s="16" t="s">
+        <v>154</v>
+      </c>
+      <c r="K24" s="14" t="s">
+        <v>165</v>
+      </c>
       <c r="L24" s="4"/>
       <c r="M24" s="2"/>
       <c r="N24" s="2"/>
@@ -3616,9 +4259,7 @@
       <c r="Y24" s="2"/>
     </row>
     <row r="25" spans="1:25" ht="37.5" thickTop="1" thickBot="1">
-      <c r="A25" s="16" t="s">
-        <v>142</v>
-      </c>
+      <c r="A25" s="14"/>
       <c r="B25" s="3"/>
       <c r="C25" s="5"/>
       <c r="D25" s="3" t="s">
@@ -3652,10 +4293,8 @@
       <c r="X25" s="2"/>
       <c r="Y25" s="2"/>
     </row>
-    <row r="26" spans="1:25" ht="60" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A26" s="16" t="s">
-        <v>143</v>
-      </c>
+    <row r="26" spans="1:25" ht="37.5" thickTop="1" thickBot="1">
+      <c r="A26" s="14"/>
       <c r="B26" s="3"/>
       <c r="C26" s="5"/>
       <c r="D26" s="3" t="s">
@@ -3689,8 +4328,8 @@
       <c r="X26" s="2"/>
       <c r="Y26" s="2"/>
     </row>
-    <row r="27" spans="1:25" ht="37.5" thickTop="1" thickBot="1">
-      <c r="A27" s="3"/>
+    <row r="27" spans="1:25" ht="60" customHeight="1" thickTop="1" thickBot="1">
+      <c r="A27" s="14"/>
       <c r="B27" s="3"/>
       <c r="C27" s="5"/>
       <c r="D27" s="3" t="s">
@@ -3725,7 +4364,7 @@
       <c r="Y27" s="2"/>
     </row>
     <row r="28" spans="1:25" ht="37.5" thickTop="1" thickBot="1">
-      <c r="A28" s="3"/>
+      <c r="A28" s="14"/>
       <c r="B28" s="3"/>
       <c r="C28" s="5"/>
       <c r="D28" s="3" t="s">
@@ -3743,7 +4382,7 @@
       <c r="H28" s="5"/>
       <c r="I28" s="5"/>
       <c r="J28" s="5"/>
-      <c r="K28" s="7"/>
+      <c r="K28" s="5"/>
       <c r="L28" s="4"/>
       <c r="M28" s="2"/>
       <c r="N28" s="2"/>
@@ -3760,9 +4399,9 @@
       <c r="Y28" s="2"/>
     </row>
     <row r="29" spans="1:25" ht="37.5" thickTop="1" thickBot="1">
-      <c r="A29" s="3"/>
+      <c r="A29" s="14"/>
       <c r="B29" s="3"/>
-      <c r="C29" s="3"/>
+      <c r="C29" s="5"/>
       <c r="D29" s="3" t="s">
         <v>65</v>
       </c>
@@ -3776,7 +4415,7 @@
         <v>103</v>
       </c>
       <c r="H29" s="5"/>
-      <c r="I29" s="7"/>
+      <c r="I29" s="5"/>
       <c r="J29" s="5"/>
       <c r="K29" s="7"/>
       <c r="L29" s="4"/>
@@ -3794,8 +4433,8 @@
       <c r="X29" s="2"/>
       <c r="Y29" s="2"/>
     </row>
-    <row r="30" spans="1:25" s="12" customFormat="1" ht="37.5" thickTop="1" thickBot="1">
-      <c r="A30" s="3"/>
+    <row r="30" spans="1:25" ht="37.5" thickTop="1" thickBot="1">
+      <c r="A30" s="14"/>
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
       <c r="D30" s="3" t="s">
@@ -3811,58 +4450,58 @@
         <v>103</v>
       </c>
       <c r="H30" s="5"/>
-      <c r="I30" s="3"/>
+      <c r="I30" s="7"/>
       <c r="J30" s="5"/>
       <c r="K30" s="7"/>
       <c r="L30" s="4"/>
-      <c r="M30" s="11"/>
-      <c r="N30" s="11"/>
-      <c r="O30" s="11"/>
-      <c r="P30" s="11"/>
-      <c r="Q30" s="11"/>
-      <c r="R30" s="11"/>
-      <c r="S30" s="11"/>
-      <c r="T30" s="11"/>
-      <c r="U30" s="11"/>
-      <c r="V30" s="11"/>
-      <c r="W30" s="11"/>
-      <c r="X30" s="11"/>
-      <c r="Y30" s="11"/>
-    </row>
-    <row r="31" spans="1:25" ht="37.5" thickTop="1" thickBot="1">
-      <c r="A31" s="3"/>
-      <c r="B31" s="3"/>
-      <c r="C31" s="3"/>
-      <c r="D31" s="3" t="s">
+      <c r="M30" s="2"/>
+      <c r="N30" s="2"/>
+      <c r="O30" s="2"/>
+      <c r="P30" s="2"/>
+      <c r="Q30" s="2"/>
+      <c r="R30" s="2"/>
+      <c r="S30" s="2"/>
+      <c r="T30" s="2"/>
+      <c r="U30" s="2"/>
+      <c r="V30" s="2"/>
+      <c r="W30" s="2"/>
+      <c r="X30" s="2"/>
+      <c r="Y30" s="2"/>
+    </row>
+    <row r="31" spans="1:25" s="12" customFormat="1" ht="37.5" thickTop="1" thickBot="1">
+      <c r="A31" s="14"/>
+      <c r="B31" s="14"/>
+      <c r="C31" s="14"/>
+      <c r="D31" s="14" t="s">
         <v>65</v>
       </c>
-      <c r="E31" s="3" t="s">
+      <c r="E31" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="F31" s="3" t="s">
+      <c r="F31" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="G31" s="3" t="s">
+      <c r="G31" s="14" t="s">
         <v>103</v>
       </c>
-      <c r="H31" s="5"/>
-      <c r="I31" s="3"/>
-      <c r="J31" s="3"/>
+      <c r="H31" s="16"/>
+      <c r="I31" s="7"/>
+      <c r="J31" s="16"/>
       <c r="K31" s="7"/>
-      <c r="L31" s="4"/>
-      <c r="M31" s="2"/>
-      <c r="N31" s="2"/>
-      <c r="O31" s="2"/>
-      <c r="P31" s="2"/>
-      <c r="Q31" s="2"/>
-      <c r="R31" s="2"/>
-      <c r="S31" s="2"/>
-      <c r="T31" s="2"/>
-      <c r="U31" s="2"/>
-      <c r="V31" s="2"/>
-      <c r="W31" s="2"/>
-      <c r="X31" s="2"/>
-      <c r="Y31" s="2"/>
+      <c r="L31" s="15"/>
+      <c r="M31" s="13"/>
+      <c r="N31" s="13"/>
+      <c r="O31" s="13"/>
+      <c r="P31" s="13"/>
+      <c r="Q31" s="13"/>
+      <c r="R31" s="13"/>
+      <c r="S31" s="13"/>
+      <c r="T31" s="13"/>
+      <c r="U31" s="13"/>
+      <c r="V31" s="13"/>
+      <c r="W31" s="13"/>
+      <c r="X31" s="13"/>
+      <c r="Y31" s="13"/>
     </row>
     <row r="32" spans="1:25" ht="37.5" thickTop="1" thickBot="1">
       <c r="A32" s="3"/>
@@ -3885,8 +4524,21 @@
       <c r="J32" s="3"/>
       <c r="K32" s="7"/>
       <c r="L32" s="4"/>
-    </row>
-    <row r="33" spans="1:25" ht="60" customHeight="1" thickTop="1" thickBot="1">
+      <c r="M32" s="2"/>
+      <c r="N32" s="2"/>
+      <c r="O32" s="2"/>
+      <c r="P32" s="2"/>
+      <c r="Q32" s="2"/>
+      <c r="R32" s="2"/>
+      <c r="S32" s="2"/>
+      <c r="T32" s="2"/>
+      <c r="U32" s="2"/>
+      <c r="V32" s="2"/>
+      <c r="W32" s="2"/>
+      <c r="X32" s="2"/>
+      <c r="Y32" s="2"/>
+    </row>
+    <row r="33" spans="1:25" ht="37.5" thickTop="1" thickBot="1">
       <c r="A33" s="3"/>
       <c r="B33" s="3"/>
       <c r="C33" s="3"/>
@@ -3907,19 +4559,6 @@
       <c r="J33" s="3"/>
       <c r="K33" s="7"/>
       <c r="L33" s="4"/>
-      <c r="M33" s="2"/>
-      <c r="N33" s="2"/>
-      <c r="O33" s="2"/>
-      <c r="P33" s="2"/>
-      <c r="Q33" s="2"/>
-      <c r="R33" s="2"/>
-      <c r="S33" s="2"/>
-      <c r="T33" s="2"/>
-      <c r="U33" s="2"/>
-      <c r="V33" s="2"/>
-      <c r="W33" s="2"/>
-      <c r="X33" s="2"/>
-      <c r="Y33" s="2"/>
     </row>
     <row r="34" spans="1:25" ht="60" customHeight="1" thickTop="1" thickBot="1">
       <c r="A34" s="3"/>
@@ -3940,7 +4579,7 @@
       <c r="H34" s="5"/>
       <c r="I34" s="3"/>
       <c r="J34" s="3"/>
-      <c r="K34" s="3"/>
+      <c r="K34" s="7"/>
       <c r="L34" s="4"/>
       <c r="M34" s="2"/>
       <c r="N34" s="2"/>
@@ -3956,7 +4595,7 @@
       <c r="X34" s="2"/>
       <c r="Y34" s="2"/>
     </row>
-    <row r="35" spans="1:25" ht="37.5" thickTop="1" thickBot="1">
+    <row r="35" spans="1:25" ht="60" customHeight="1" thickTop="1" thickBot="1">
       <c r="A35" s="3"/>
       <c r="B35" s="3"/>
       <c r="C35" s="3"/>
@@ -4026,10 +4665,10 @@
       <c r="X36" s="2"/>
       <c r="Y36" s="2"/>
     </row>
-    <row r="37" spans="1:25" ht="60" customHeight="1" thickTop="1" thickBot="1">
+    <row r="37" spans="1:25" ht="37.5" thickTop="1" thickBot="1">
       <c r="A37" s="3"/>
       <c r="B37" s="3"/>
-      <c r="C37" s="5"/>
+      <c r="C37" s="3"/>
       <c r="D37" s="3" t="s">
         <v>65</v>
       </c>
@@ -4901,7 +5540,7 @@
       <c r="X61" s="2"/>
       <c r="Y61" s="2"/>
     </row>
-    <row r="62" spans="1:25" ht="37.5" thickTop="1" thickBot="1">
+    <row r="62" spans="1:25" ht="60" customHeight="1" thickTop="1" thickBot="1">
       <c r="A62" s="3"/>
       <c r="B62" s="3"/>
       <c r="C62" s="5"/>
@@ -4953,9 +5592,9 @@
         <v>103</v>
       </c>
       <c r="H63" s="5"/>
-      <c r="I63" s="5"/>
-      <c r="J63" s="5"/>
-      <c r="K63" s="5"/>
+      <c r="I63" s="3"/>
+      <c r="J63" s="3"/>
+      <c r="K63" s="3"/>
       <c r="L63" s="4"/>
       <c r="M63" s="2"/>
       <c r="N63" s="2"/>
@@ -5076,7 +5715,7 @@
       <c r="X66" s="2"/>
       <c r="Y66" s="2"/>
     </row>
-    <row r="67" spans="1:25" ht="79.5" customHeight="1" thickTop="1" thickBot="1">
+    <row r="67" spans="1:25" ht="37.5" thickTop="1" thickBot="1">
       <c r="A67" s="3"/>
       <c r="B67" s="3"/>
       <c r="C67" s="5"/>
@@ -5111,7 +5750,7 @@
       <c r="X67" s="2"/>
       <c r="Y67" s="2"/>
     </row>
-    <row r="68" spans="1:25" ht="37.5" thickTop="1" thickBot="1">
+    <row r="68" spans="1:25" ht="79.5" customHeight="1" thickTop="1" thickBot="1">
       <c r="A68" s="3"/>
       <c r="B68" s="3"/>
       <c r="C68" s="5"/>
@@ -5132,6 +5771,7 @@
       <c r="J68" s="5"/>
       <c r="K68" s="5"/>
       <c r="L68" s="4"/>
+      <c r="M68" s="2"/>
       <c r="N68" s="2"/>
       <c r="O68" s="2"/>
       <c r="P68" s="2"/>
@@ -5166,7 +5806,6 @@
       <c r="J69" s="5"/>
       <c r="K69" s="5"/>
       <c r="L69" s="4"/>
-      <c r="M69" s="8"/>
       <c r="N69" s="2"/>
       <c r="O69" s="2"/>
       <c r="P69" s="2"/>
@@ -5201,6 +5840,7 @@
       <c r="J70" s="5"/>
       <c r="K70" s="5"/>
       <c r="L70" s="4"/>
+      <c r="M70" s="8"/>
       <c r="N70" s="2"/>
       <c r="O70" s="2"/>
       <c r="P70" s="2"/>
@@ -5235,7 +5875,6 @@
       <c r="J71" s="5"/>
       <c r="K71" s="5"/>
       <c r="L71" s="4"/>
-      <c r="M71" s="8"/>
       <c r="N71" s="2"/>
       <c r="O71" s="2"/>
       <c r="P71" s="2"/>
@@ -5305,6 +5944,7 @@
       <c r="J73" s="5"/>
       <c r="K73" s="5"/>
       <c r="L73" s="4"/>
+      <c r="M73" s="8"/>
       <c r="N73" s="2"/>
       <c r="O73" s="2"/>
       <c r="P73" s="2"/>
@@ -5368,7 +6008,7 @@
       <c r="G75" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="H75" s="13"/>
+      <c r="H75" s="5"/>
       <c r="I75" s="5"/>
       <c r="J75" s="5"/>
       <c r="K75" s="5"/>
@@ -5402,7 +6042,7 @@
       <c r="G76" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="H76" s="5"/>
+      <c r="H76" s="11"/>
       <c r="I76" s="5"/>
       <c r="J76" s="5"/>
       <c r="K76" s="5"/>
@@ -5660,7 +6300,7 @@
     </row>
     <row r="84" spans="1:25" ht="37.5" thickTop="1" thickBot="1">
       <c r="A84" s="3"/>
-      <c r="B84" s="5"/>
+      <c r="B84" s="3"/>
       <c r="C84" s="5"/>
       <c r="D84" s="3" t="s">
         <v>65</v>
@@ -5694,7 +6334,7 @@
     </row>
     <row r="85" spans="1:25" ht="37.5" thickTop="1" thickBot="1">
       <c r="A85" s="3"/>
-      <c r="B85" s="3"/>
+      <c r="B85" s="5"/>
       <c r="C85" s="5"/>
       <c r="D85" s="3" t="s">
         <v>65</v>
@@ -5709,11 +6349,10 @@
         <v>103</v>
       </c>
       <c r="H85" s="5"/>
-      <c r="I85" s="3"/>
-      <c r="J85" s="3"/>
-      <c r="K85" s="3"/>
+      <c r="I85" s="5"/>
+      <c r="J85" s="5"/>
+      <c r="K85" s="5"/>
       <c r="L85" s="4"/>
-      <c r="M85" s="2"/>
       <c r="N85" s="2"/>
       <c r="O85" s="2"/>
       <c r="P85" s="2"/>
@@ -5744,9 +6383,9 @@
         <v>103</v>
       </c>
       <c r="H86" s="5"/>
-      <c r="I86" s="5"/>
-      <c r="J86" s="5"/>
-      <c r="K86" s="5"/>
+      <c r="I86" s="3"/>
+      <c r="J86" s="3"/>
+      <c r="K86" s="3"/>
       <c r="L86" s="4"/>
       <c r="M86" s="2"/>
       <c r="N86" s="2"/>
@@ -6567,15 +7206,25 @@
       <c r="X109" s="2"/>
       <c r="Y109" s="2"/>
     </row>
-    <row r="110" spans="1:25" ht="15.75" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A110" s="2"/>
-      <c r="B110" s="2"/>
-      <c r="D110" s="2"/>
-      <c r="F110" s="2"/>
-      <c r="G110" s="2"/>
-      <c r="H110" s="2"/>
-      <c r="I110" s="2"/>
-      <c r="J110" s="2"/>
+    <row r="110" spans="1:25" ht="37.5" thickTop="1" thickBot="1">
+      <c r="A110" s="3"/>
+      <c r="B110" s="3"/>
+      <c r="C110" s="5"/>
+      <c r="D110" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="E110" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F110" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="G110" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="H110" s="5"/>
+      <c r="I110" s="5"/>
+      <c r="J110" s="5"/>
       <c r="K110" s="5"/>
       <c r="L110" s="4"/>
       <c r="M110" s="2"/>
@@ -6592,7 +7241,7 @@
       <c r="X110" s="2"/>
       <c r="Y110" s="2"/>
     </row>
-    <row r="111" spans="1:25" ht="15.75" customHeight="1" thickTop="1">
+    <row r="111" spans="1:25" ht="15.75" customHeight="1" thickTop="1" thickBot="1">
       <c r="A111" s="2"/>
       <c r="B111" s="2"/>
       <c r="D111" s="2"/>
@@ -6601,8 +7250,8 @@
       <c r="H111" s="2"/>
       <c r="I111" s="2"/>
       <c r="J111" s="2"/>
-      <c r="K111" s="2"/>
-      <c r="L111" s="2"/>
+      <c r="K111" s="5"/>
+      <c r="L111" s="4"/>
       <c r="M111" s="2"/>
       <c r="N111" s="2"/>
       <c r="O111" s="2"/>
@@ -6617,7 +7266,7 @@
       <c r="X111" s="2"/>
       <c r="Y111" s="2"/>
     </row>
-    <row r="112" spans="1:25" ht="15.75" customHeight="1">
+    <row r="112" spans="1:25" ht="15.75" customHeight="1" thickTop="1">
       <c r="A112" s="2"/>
       <c r="B112" s="2"/>
       <c r="D112" s="2"/>
@@ -8220,7 +8869,6 @@
     <row r="176" spans="1:25" ht="15.75" customHeight="1">
       <c r="A176" s="2"/>
       <c r="B176" s="2"/>
-      <c r="C176" s="2"/>
       <c r="D176" s="2"/>
       <c r="F176" s="2"/>
       <c r="G176" s="2"/>
@@ -9595,7 +10243,32 @@
       <c r="X228" s="2"/>
       <c r="Y228" s="2"/>
     </row>
-    <row r="229" spans="1:25" ht="15.75" customHeight="1"/>
+    <row r="229" spans="1:25" ht="15.75" customHeight="1">
+      <c r="A229" s="2"/>
+      <c r="B229" s="2"/>
+      <c r="C229" s="2"/>
+      <c r="D229" s="2"/>
+      <c r="F229" s="2"/>
+      <c r="G229" s="2"/>
+      <c r="H229" s="2"/>
+      <c r="I229" s="2"/>
+      <c r="J229" s="2"/>
+      <c r="K229" s="2"/>
+      <c r="L229" s="2"/>
+      <c r="M229" s="2"/>
+      <c r="N229" s="2"/>
+      <c r="O229" s="2"/>
+      <c r="P229" s="2"/>
+      <c r="Q229" s="2"/>
+      <c r="R229" s="2"/>
+      <c r="S229" s="2"/>
+      <c r="T229" s="2"/>
+      <c r="U229" s="2"/>
+      <c r="V229" s="2"/>
+      <c r="W229" s="2"/>
+      <c r="X229" s="2"/>
+      <c r="Y229" s="2"/>
+    </row>
     <row r="230" spans="1:25" ht="15.75" customHeight="1"/>
     <row r="231" spans="1:25" ht="15.75" customHeight="1"/>
     <row r="232" spans="1:25" ht="15.75" customHeight="1"/>
@@ -10375,865 +11048,1106 @@
     <row r="1006" ht="15.75" customHeight="1"/>
     <row r="1007" ht="15.75" customHeight="1"/>
     <row r="1008" ht="15.75" customHeight="1"/>
+    <row r="1009" ht="15.75" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="7" type="noConversion"/>
-  <conditionalFormatting sqref="E22:E109 E2:E17">
-    <cfRule type="cellIs" dxfId="182" priority="259" operator="equal">
+  <conditionalFormatting sqref="E23:E30 E2:E18 E32:E110">
+    <cfRule type="cellIs" dxfId="251" priority="328" operator="equal">
       <formula>"Alacsony"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E22:E109 E2:E17">
-    <cfRule type="cellIs" dxfId="181" priority="260" operator="equal">
+  <conditionalFormatting sqref="E23:E30 E2:E18 E32:E110">
+    <cfRule type="cellIs" dxfId="250" priority="329" operator="equal">
       <formula>"Normál"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E22:E109 E2:E17">
-    <cfRule type="cellIs" dxfId="180" priority="261" operator="equal">
+  <conditionalFormatting sqref="E23:E30 E2:E18 E32:E110">
+    <cfRule type="cellIs" dxfId="249" priority="330" operator="equal">
       <formula>"Magas"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K70:K84 K26:K61 K11 K3:K8 K22 K13:K17">
-    <cfRule type="cellIs" dxfId="179" priority="262" operator="equal">
+  <conditionalFormatting sqref="K71:K85 K27:K30 K8 K32:K62">
+    <cfRule type="cellIs" dxfId="248" priority="331" operator="equal">
       <formula>"Siker"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K70:K84 K26:K61 K11 K3:K8 K22 K13:K17">
-    <cfRule type="cellIs" dxfId="178" priority="263" operator="equal">
+  <conditionalFormatting sqref="K71:K85 K27:K30 K8 K32:K62">
+    <cfRule type="cellIs" dxfId="247" priority="332" operator="equal">
       <formula>"Nem futtatható"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K70:K84 K26:K61 K11 K3:K8 K22 K13:K17">
-    <cfRule type="cellIs" dxfId="177" priority="264" operator="equal">
+  <conditionalFormatting sqref="K71:K85 K27:K30 K8 K32:K62">
+    <cfRule type="cellIs" dxfId="246" priority="333" operator="equal">
       <formula>"Hiba"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E11">
-    <cfRule type="cellIs" dxfId="176" priority="250" operator="equal">
+  <conditionalFormatting sqref="E12">
+    <cfRule type="cellIs" dxfId="245" priority="319" operator="equal">
       <formula>"Alacsony"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E11">
-    <cfRule type="cellIs" dxfId="175" priority="251" operator="equal">
+  <conditionalFormatting sqref="E12">
+    <cfRule type="cellIs" dxfId="244" priority="320" operator="equal">
       <formula>"Normál"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E11">
-    <cfRule type="cellIs" dxfId="174" priority="252" operator="equal">
+  <conditionalFormatting sqref="E12">
+    <cfRule type="cellIs" dxfId="243" priority="321" operator="equal">
       <formula>"Magas"</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="E13">
+    <cfRule type="cellIs" dxfId="239" priority="310" operator="equal">
+      <formula>"Alacsony"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E13">
+    <cfRule type="cellIs" dxfId="238" priority="311" operator="equal">
+      <formula>"Normál"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E13">
+    <cfRule type="cellIs" dxfId="237" priority="312" operator="equal">
+      <formula>"Magas"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="cellIs" dxfId="236" priority="301" operator="equal">
+      <formula>"Alacsony"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="cellIs" dxfId="235" priority="302" operator="equal">
+      <formula>"Normál"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="cellIs" dxfId="234" priority="303" operator="equal">
+      <formula>"Magas"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K25">
+    <cfRule type="cellIs" dxfId="233" priority="304" operator="equal">
+      <formula>"Siker"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K25">
+    <cfRule type="cellIs" dxfId="232" priority="305" operator="equal">
+      <formula>"Nem futtatható"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K25">
+    <cfRule type="cellIs" dxfId="231" priority="306" operator="equal">
+      <formula>"Hiba"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E26">
+    <cfRule type="cellIs" dxfId="230" priority="295" operator="equal">
+      <formula>"Alacsony"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E26">
+    <cfRule type="cellIs" dxfId="229" priority="296" operator="equal">
+      <formula>"Normál"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E26">
+    <cfRule type="cellIs" dxfId="228" priority="297" operator="equal">
+      <formula>"Magas"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K26">
+    <cfRule type="cellIs" dxfId="227" priority="298" operator="equal">
+      <formula>"Siker"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K26">
+    <cfRule type="cellIs" dxfId="226" priority="299" operator="equal">
+      <formula>"Nem futtatható"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K26">
+    <cfRule type="cellIs" dxfId="225" priority="300" operator="equal">
+      <formula>"Hiba"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E27">
+    <cfRule type="cellIs" dxfId="224" priority="292" operator="equal">
+      <formula>"Alacsony"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E27">
+    <cfRule type="cellIs" dxfId="223" priority="293" operator="equal">
+      <formula>"Normál"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E27">
+    <cfRule type="cellIs" dxfId="222" priority="294" operator="equal">
+      <formula>"Magas"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E63:E66">
+    <cfRule type="cellIs" dxfId="221" priority="280" operator="equal">
+      <formula>"Alacsony"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E63:E66">
+    <cfRule type="cellIs" dxfId="220" priority="281" operator="equal">
+      <formula>"Normál"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E63:E66">
+    <cfRule type="cellIs" dxfId="219" priority="282" operator="equal">
+      <formula>"Magas"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K63:K66">
+    <cfRule type="cellIs" dxfId="218" priority="283" operator="equal">
+      <formula>"Siker"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K63:K66">
+    <cfRule type="cellIs" dxfId="217" priority="284" operator="equal">
+      <formula>"Nem futtatható"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K63:K66">
+    <cfRule type="cellIs" dxfId="216" priority="285" operator="equal">
+      <formula>"Hiba"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E67">
+    <cfRule type="cellIs" dxfId="215" priority="274" operator="equal">
+      <formula>"Alacsony"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E67">
+    <cfRule type="cellIs" dxfId="214" priority="275" operator="equal">
+      <formula>"Normál"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E67">
+    <cfRule type="cellIs" dxfId="213" priority="276" operator="equal">
+      <formula>"Magas"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K67:K68">
+    <cfRule type="cellIs" dxfId="212" priority="277" operator="equal">
+      <formula>"Siker"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K67:K68">
+    <cfRule type="cellIs" dxfId="211" priority="278" operator="equal">
+      <formula>"Nem futtatható"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K67:K68">
+    <cfRule type="cellIs" dxfId="210" priority="279" operator="equal">
+      <formula>"Hiba"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E68">
+    <cfRule type="cellIs" dxfId="209" priority="265" operator="equal">
+      <formula>"Alacsony"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E68">
+    <cfRule type="cellIs" dxfId="208" priority="266" operator="equal">
+      <formula>"Normál"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E68">
+    <cfRule type="cellIs" dxfId="207" priority="267" operator="equal">
+      <formula>"Magas"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E69">
+    <cfRule type="cellIs" dxfId="206" priority="259" operator="equal">
+      <formula>"Alacsony"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E69">
+    <cfRule type="cellIs" dxfId="205" priority="260" operator="equal">
+      <formula>"Normál"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E69">
+    <cfRule type="cellIs" dxfId="204" priority="261" operator="equal">
+      <formula>"Magas"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K69">
+    <cfRule type="cellIs" dxfId="203" priority="262" operator="equal">
+      <formula>"Siker"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K69">
+    <cfRule type="cellIs" dxfId="202" priority="263" operator="equal">
+      <formula>"Nem futtatható"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K69">
+    <cfRule type="cellIs" dxfId="201" priority="264" operator="equal">
+      <formula>"Hiba"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E70">
+    <cfRule type="cellIs" dxfId="200" priority="235" operator="equal">
+      <formula>"Alacsony"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E70">
+    <cfRule type="cellIs" dxfId="199" priority="236" operator="equal">
+      <formula>"Normál"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E70">
+    <cfRule type="cellIs" dxfId="198" priority="237" operator="equal">
+      <formula>"Magas"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K70">
+    <cfRule type="cellIs" dxfId="197" priority="238" operator="equal">
+      <formula>"Siker"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K70">
+    <cfRule type="cellIs" dxfId="196" priority="239" operator="equal">
+      <formula>"Nem futtatható"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K70">
+    <cfRule type="cellIs" dxfId="195" priority="240" operator="equal">
+      <formula>"Hiba"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E86:E90 E94:E105">
+    <cfRule type="cellIs" dxfId="194" priority="220" operator="equal">
+      <formula>"Alacsony"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E86:E90 E94:E105">
+    <cfRule type="cellIs" dxfId="193" priority="221" operator="equal">
+      <formula>"Normál"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E86:E90 E94:E105">
+    <cfRule type="cellIs" dxfId="192" priority="222" operator="equal">
+      <formula>"Magas"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K86:K91 K93:K105 K108:K111">
+    <cfRule type="cellIs" dxfId="191" priority="223" operator="equal">
+      <formula>"Siker"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K86:K91 K93:K105 K108:K111">
+    <cfRule type="cellIs" dxfId="190" priority="224" operator="equal">
+      <formula>"Nem futtatható"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K86:K91 K93:K105 K108:K111">
+    <cfRule type="cellIs" dxfId="189" priority="225" operator="equal">
+      <formula>"Hiba"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E91">
+    <cfRule type="cellIs" dxfId="188" priority="217" operator="equal">
+      <formula>"Alacsony"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E91">
+    <cfRule type="cellIs" dxfId="187" priority="218" operator="equal">
+      <formula>"Normál"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E91">
+    <cfRule type="cellIs" dxfId="186" priority="219" operator="equal">
+      <formula>"Magas"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K92">
+    <cfRule type="cellIs" dxfId="185" priority="214" operator="equal">
+      <formula>"Siker"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K92">
+    <cfRule type="cellIs" dxfId="184" priority="215" operator="equal">
+      <formula>"Nem futtatható"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K92">
+    <cfRule type="cellIs" dxfId="183" priority="216" operator="equal">
+      <formula>"Hiba"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E92">
+    <cfRule type="cellIs" dxfId="182" priority="211" operator="equal">
+      <formula>"Alacsony"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E92">
+    <cfRule type="cellIs" dxfId="181" priority="212" operator="equal">
+      <formula>"Normál"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E92">
+    <cfRule type="cellIs" dxfId="180" priority="213" operator="equal">
+      <formula>"Magas"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E93">
+    <cfRule type="cellIs" dxfId="179" priority="208" operator="equal">
+      <formula>"Alacsony"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E93">
+    <cfRule type="cellIs" dxfId="178" priority="209" operator="equal">
+      <formula>"Normál"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E93">
+    <cfRule type="cellIs" dxfId="177" priority="210" operator="equal">
+      <formula>"Magas"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E106">
+    <cfRule type="cellIs" dxfId="176" priority="202" operator="equal">
+      <formula>"Alacsony"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E106">
+    <cfRule type="cellIs" dxfId="175" priority="203" operator="equal">
+      <formula>"Normál"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E106">
+    <cfRule type="cellIs" dxfId="174" priority="204" operator="equal">
+      <formula>"Magas"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K106">
+    <cfRule type="cellIs" dxfId="173" priority="205" operator="equal">
+      <formula>"Siker"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K106">
+    <cfRule type="cellIs" dxfId="172" priority="206" operator="equal">
+      <formula>"Nem futtatható"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K106">
+    <cfRule type="cellIs" dxfId="171" priority="207" operator="equal">
+      <formula>"Hiba"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E107">
+    <cfRule type="cellIs" dxfId="170" priority="196" operator="equal">
+      <formula>"Alacsony"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E107">
+    <cfRule type="cellIs" dxfId="169" priority="197" operator="equal">
+      <formula>"Normál"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E107">
+    <cfRule type="cellIs" dxfId="168" priority="198" operator="equal">
+      <formula>"Magas"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K107">
+    <cfRule type="cellIs" dxfId="167" priority="199" operator="equal">
+      <formula>"Siker"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K107">
+    <cfRule type="cellIs" dxfId="166" priority="200" operator="equal">
+      <formula>"Nem futtatható"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K107">
+    <cfRule type="cellIs" dxfId="165" priority="201" operator="equal">
+      <formula>"Hiba"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E108">
+    <cfRule type="cellIs" dxfId="164" priority="193" operator="equal">
+      <formula>"Alacsony"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E108">
+    <cfRule type="cellIs" dxfId="163" priority="194" operator="equal">
+      <formula>"Normál"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E108">
+    <cfRule type="cellIs" dxfId="162" priority="195" operator="equal">
+      <formula>"Magas"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E109:E110">
+    <cfRule type="cellIs" dxfId="161" priority="190" operator="equal">
+      <formula>"Alacsony"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E109:E110">
+    <cfRule type="cellIs" dxfId="160" priority="191" operator="equal">
+      <formula>"Normál"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E109:E110">
+    <cfRule type="cellIs" dxfId="159" priority="192" operator="equal">
+      <formula>"Magas"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E2">
+    <cfRule type="cellIs" dxfId="158" priority="172" operator="equal">
+      <formula>"Alacsony"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E2">
+    <cfRule type="cellIs" dxfId="157" priority="173" operator="equal">
+      <formula>"Normál"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E2">
+    <cfRule type="cellIs" dxfId="156" priority="174" operator="equal">
+      <formula>"Magas"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K2">
+    <cfRule type="cellIs" dxfId="155" priority="175" operator="equal">
+      <formula>"Siker"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K2">
+    <cfRule type="cellIs" dxfId="154" priority="176" operator="equal">
+      <formula>"Nem futtatható"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K2">
+    <cfRule type="cellIs" dxfId="153" priority="177" operator="equal">
+      <formula>"Hiba"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E9:E11">
+    <cfRule type="cellIs" dxfId="152" priority="166" operator="equal">
+      <formula>"Alacsony"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E9:E11">
+    <cfRule type="cellIs" dxfId="151" priority="167" operator="equal">
+      <formula>"Normál"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E9:E11">
+    <cfRule type="cellIs" dxfId="150" priority="168" operator="equal">
+      <formula>"Magas"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K11">
+    <cfRule type="cellIs" dxfId="149" priority="169" operator="equal">
+      <formula>"Siker"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K11">
+    <cfRule type="cellIs" dxfId="148" priority="170" operator="equal">
+      <formula>"Nem futtatható"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K11">
+    <cfRule type="cellIs" dxfId="147" priority="171" operator="equal">
+      <formula>"Hiba"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E10:E11">
+    <cfRule type="cellIs" dxfId="146" priority="160" operator="equal">
+      <formula>"Alacsony"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E10:E11">
+    <cfRule type="cellIs" dxfId="145" priority="161" operator="equal">
+      <formula>"Normál"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E10:E11">
+    <cfRule type="cellIs" dxfId="144" priority="162" operator="equal">
+      <formula>"Magas"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K11">
+    <cfRule type="cellIs" dxfId="143" priority="163" operator="equal">
+      <formula>"Siker"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K11">
+    <cfRule type="cellIs" dxfId="142" priority="164" operator="equal">
+      <formula>"Nem futtatható"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K11">
+    <cfRule type="cellIs" dxfId="141" priority="165" operator="equal">
+      <formula>"Hiba"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E24">
+    <cfRule type="cellIs" dxfId="140" priority="148" operator="equal">
+      <formula>"Alacsony"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E24">
+    <cfRule type="cellIs" dxfId="139" priority="149" operator="equal">
+      <formula>"Normál"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E24">
+    <cfRule type="cellIs" dxfId="138" priority="150" operator="equal">
+      <formula>"Magas"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E4">
+    <cfRule type="cellIs" dxfId="134" priority="145" operator="equal">
+      <formula>"Alacsony"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E4">
+    <cfRule type="cellIs" dxfId="133" priority="146" operator="equal">
+      <formula>"Normál"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E4">
+    <cfRule type="cellIs" dxfId="132" priority="147" operator="equal">
+      <formula>"Magas"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E5">
+    <cfRule type="cellIs" dxfId="131" priority="142" operator="equal">
+      <formula>"Alacsony"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E5">
+    <cfRule type="cellIs" dxfId="130" priority="143" operator="equal">
+      <formula>"Normál"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E5">
+    <cfRule type="cellIs" dxfId="129" priority="144" operator="equal">
+      <formula>"Magas"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E6">
+    <cfRule type="cellIs" dxfId="128" priority="139" operator="equal">
+      <formula>"Alacsony"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E6">
+    <cfRule type="cellIs" dxfId="127" priority="140" operator="equal">
+      <formula>"Normál"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E6">
+    <cfRule type="cellIs" dxfId="126" priority="141" operator="equal">
+      <formula>"Magas"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E7">
+    <cfRule type="cellIs" dxfId="125" priority="136" operator="equal">
+      <formula>"Alacsony"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E7">
+    <cfRule type="cellIs" dxfId="124" priority="137" operator="equal">
+      <formula>"Normál"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E7">
+    <cfRule type="cellIs" dxfId="123" priority="138" operator="equal">
+      <formula>"Magas"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E8">
+    <cfRule type="cellIs" dxfId="122" priority="133" operator="equal">
+      <formula>"Alacsony"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E8">
+    <cfRule type="cellIs" dxfId="121" priority="134" operator="equal">
+      <formula>"Normál"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E8">
+    <cfRule type="cellIs" dxfId="120" priority="135" operator="equal">
+      <formula>"Magas"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E12">
+    <cfRule type="cellIs" dxfId="119" priority="130" operator="equal">
+      <formula>"Alacsony"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E12">
+    <cfRule type="cellIs" dxfId="118" priority="131" operator="equal">
+      <formula>"Normál"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E12">
+    <cfRule type="cellIs" dxfId="117" priority="132" operator="equal">
+      <formula>"Magas"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E13">
+    <cfRule type="cellIs" dxfId="116" priority="127" operator="equal">
+      <formula>"Alacsony"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E13">
+    <cfRule type="cellIs" dxfId="115" priority="128" operator="equal">
+      <formula>"Normál"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E13">
+    <cfRule type="cellIs" dxfId="114" priority="129" operator="equal">
+      <formula>"Magas"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E14">
+    <cfRule type="cellIs" dxfId="113" priority="124" operator="equal">
+      <formula>"Alacsony"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E14">
+    <cfRule type="cellIs" dxfId="112" priority="125" operator="equal">
+      <formula>"Normál"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E14">
+    <cfRule type="cellIs" dxfId="111" priority="126" operator="equal">
+      <formula>"Magas"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E15">
+    <cfRule type="cellIs" dxfId="110" priority="121" operator="equal">
+      <formula>"Alacsony"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E15">
+    <cfRule type="cellIs" dxfId="109" priority="122" operator="equal">
+      <formula>"Normál"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E15">
+    <cfRule type="cellIs" dxfId="108" priority="123" operator="equal">
+      <formula>"Magas"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E16">
+    <cfRule type="cellIs" dxfId="107" priority="118" operator="equal">
+      <formula>"Alacsony"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E16">
+    <cfRule type="cellIs" dxfId="106" priority="119" operator="equal">
+      <formula>"Normál"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E16">
+    <cfRule type="cellIs" dxfId="105" priority="120" operator="equal">
+      <formula>"Magas"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E21">
+    <cfRule type="cellIs" dxfId="104" priority="112" operator="equal">
+      <formula>"Alacsony"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E21">
+    <cfRule type="cellIs" dxfId="103" priority="113" operator="equal">
+      <formula>"Normál"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E21">
+    <cfRule type="cellIs" dxfId="102" priority="114" operator="equal">
+      <formula>"Magas"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E20">
+    <cfRule type="cellIs" dxfId="98" priority="106" operator="equal">
+      <formula>"Alacsony"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E20">
+    <cfRule type="cellIs" dxfId="97" priority="107" operator="equal">
+      <formula>"Normál"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E20">
+    <cfRule type="cellIs" dxfId="96" priority="108" operator="equal">
+      <formula>"Magas"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E19">
+    <cfRule type="cellIs" dxfId="92" priority="100" operator="equal">
+      <formula>"Alacsony"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E19">
+    <cfRule type="cellIs" dxfId="91" priority="101" operator="equal">
+      <formula>"Normál"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E19">
+    <cfRule type="cellIs" dxfId="90" priority="102" operator="equal">
+      <formula>"Magas"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E22">
+    <cfRule type="cellIs" dxfId="86" priority="94" operator="equal">
+      <formula>"Alacsony"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E22">
+    <cfRule type="cellIs" dxfId="85" priority="95" operator="equal">
+      <formula>"Normál"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E22">
+    <cfRule type="cellIs" dxfId="84" priority="96" operator="equal">
+      <formula>"Magas"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E31">
+    <cfRule type="cellIs" dxfId="80" priority="64" operator="equal">
+      <formula>"Alacsony"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E31">
+    <cfRule type="cellIs" dxfId="79" priority="65" operator="equal">
+      <formula>"Normál"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E31">
+    <cfRule type="cellIs" dxfId="78" priority="66" operator="equal">
+      <formula>"Magas"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K31">
+    <cfRule type="cellIs" dxfId="77" priority="67" operator="equal">
+      <formula>"Siker"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K31">
+    <cfRule type="cellIs" dxfId="76" priority="68" operator="equal">
+      <formula>"Nem futtatható"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K31">
+    <cfRule type="cellIs" dxfId="75" priority="69" operator="equal">
+      <formula>"Hiba"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K3">
+    <cfRule type="cellIs" dxfId="62" priority="61" operator="equal">
+      <formula>"Siker"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K3">
+    <cfRule type="cellIs" dxfId="61" priority="62" operator="equal">
+      <formula>"Nem futtatható"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K3">
+    <cfRule type="cellIs" dxfId="60" priority="63" operator="equal">
+      <formula>"Hiba"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K4">
+    <cfRule type="cellIs" dxfId="59" priority="58" operator="equal">
+      <formula>"Siker"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K4">
+    <cfRule type="cellIs" dxfId="58" priority="59" operator="equal">
+      <formula>"Nem futtatható"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K4">
+    <cfRule type="cellIs" dxfId="57" priority="60" operator="equal">
+      <formula>"Hiba"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K5">
+    <cfRule type="cellIs" dxfId="56" priority="55" operator="equal">
+      <formula>"Siker"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K5">
+    <cfRule type="cellIs" dxfId="55" priority="56" operator="equal">
+      <formula>"Nem futtatható"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K5">
+    <cfRule type="cellIs" dxfId="54" priority="57" operator="equal">
+      <formula>"Hiba"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K6">
+    <cfRule type="cellIs" dxfId="53" priority="52" operator="equal">
+      <formula>"Siker"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K6">
+    <cfRule type="cellIs" dxfId="52" priority="53" operator="equal">
+      <formula>"Nem futtatható"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K6">
+    <cfRule type="cellIs" dxfId="51" priority="54" operator="equal">
+      <formula>"Hiba"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K7">
+    <cfRule type="cellIs" dxfId="50" priority="49" operator="equal">
+      <formula>"Siker"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K7">
+    <cfRule type="cellIs" dxfId="49" priority="50" operator="equal">
+      <formula>"Nem futtatható"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K7">
+    <cfRule type="cellIs" dxfId="48" priority="51" operator="equal">
+      <formula>"Hiba"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K9">
+    <cfRule type="cellIs" dxfId="47" priority="46" operator="equal">
+      <formula>"Siker"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K9">
+    <cfRule type="cellIs" dxfId="46" priority="47" operator="equal">
+      <formula>"Nem futtatható"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K9">
+    <cfRule type="cellIs" dxfId="45" priority="48" operator="equal">
+      <formula>"Hiba"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K10">
+    <cfRule type="cellIs" dxfId="44" priority="43" operator="equal">
+      <formula>"Siker"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K10">
+    <cfRule type="cellIs" dxfId="43" priority="44" operator="equal">
+      <formula>"Nem futtatható"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K10">
+    <cfRule type="cellIs" dxfId="42" priority="45" operator="equal">
+      <formula>"Hiba"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="K12">
-    <cfRule type="cellIs" dxfId="173" priority="244" operator="equal">
+    <cfRule type="cellIs" dxfId="41" priority="40" operator="equal">
       <formula>"Siker"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K12">
-    <cfRule type="cellIs" dxfId="172" priority="245" operator="equal">
+    <cfRule type="cellIs" dxfId="40" priority="41" operator="equal">
       <formula>"Nem futtatható"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K12">
-    <cfRule type="cellIs" dxfId="171" priority="246" operator="equal">
+    <cfRule type="cellIs" dxfId="39" priority="42" operator="equal">
       <formula>"Hiba"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E12">
-    <cfRule type="cellIs" dxfId="170" priority="241" operator="equal">
-      <formula>"Alacsony"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E12">
-    <cfRule type="cellIs" dxfId="169" priority="242" operator="equal">
-      <formula>"Normál"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E12">
-    <cfRule type="cellIs" dxfId="168" priority="243" operator="equal">
-      <formula>"Magas"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E24">
-    <cfRule type="cellIs" dxfId="167" priority="232" operator="equal">
-      <formula>"Alacsony"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E24">
-    <cfRule type="cellIs" dxfId="166" priority="233" operator="equal">
-      <formula>"Normál"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E24">
-    <cfRule type="cellIs" dxfId="165" priority="234" operator="equal">
-      <formula>"Magas"</formula>
+  <conditionalFormatting sqref="K13">
+    <cfRule type="cellIs" dxfId="38" priority="37" operator="equal">
+      <formula>"Siker"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K13">
+    <cfRule type="cellIs" dxfId="37" priority="38" operator="equal">
+      <formula>"Nem futtatható"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K13">
+    <cfRule type="cellIs" dxfId="36" priority="39" operator="equal">
+      <formula>"Hiba"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K14">
+    <cfRule type="cellIs" dxfId="35" priority="34" operator="equal">
+      <formula>"Siker"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K14">
+    <cfRule type="cellIs" dxfId="34" priority="35" operator="equal">
+      <formula>"Nem futtatható"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K14">
+    <cfRule type="cellIs" dxfId="33" priority="36" operator="equal">
+      <formula>"Hiba"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K15">
+    <cfRule type="cellIs" dxfId="32" priority="31" operator="equal">
+      <formula>"Siker"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K15">
+    <cfRule type="cellIs" dxfId="31" priority="32" operator="equal">
+      <formula>"Nem futtatható"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K15">
+    <cfRule type="cellIs" dxfId="30" priority="33" operator="equal">
+      <formula>"Hiba"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K16">
+    <cfRule type="cellIs" dxfId="29" priority="28" operator="equal">
+      <formula>"Siker"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K16">
+    <cfRule type="cellIs" dxfId="28" priority="29" operator="equal">
+      <formula>"Nem futtatható"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K16">
+    <cfRule type="cellIs" dxfId="27" priority="30" operator="equal">
+      <formula>"Hiba"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K17">
+    <cfRule type="cellIs" dxfId="23" priority="22" operator="equal">
+      <formula>"Siker"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K17">
+    <cfRule type="cellIs" dxfId="22" priority="23" operator="equal">
+      <formula>"Nem futtatható"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K17">
+    <cfRule type="cellIs" dxfId="21" priority="24" operator="equal">
+      <formula>"Hiba"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K18">
+    <cfRule type="cellIs" dxfId="20" priority="19" operator="equal">
+      <formula>"Siker"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K18">
+    <cfRule type="cellIs" dxfId="19" priority="20" operator="equal">
+      <formula>"Nem futtatható"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K18">
+    <cfRule type="cellIs" dxfId="18" priority="21" operator="equal">
+      <formula>"Hiba"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K19">
+    <cfRule type="cellIs" dxfId="17" priority="16" operator="equal">
+      <formula>"Siker"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K19">
+    <cfRule type="cellIs" dxfId="16" priority="17" operator="equal">
+      <formula>"Nem futtatható"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K19">
+    <cfRule type="cellIs" dxfId="15" priority="18" operator="equal">
+      <formula>"Hiba"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K20">
+    <cfRule type="cellIs" dxfId="14" priority="13" operator="equal">
+      <formula>"Siker"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K20">
+    <cfRule type="cellIs" dxfId="13" priority="14" operator="equal">
+      <formula>"Nem futtatható"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K20">
+    <cfRule type="cellIs" dxfId="12" priority="15" operator="equal">
+      <formula>"Hiba"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K21">
+    <cfRule type="cellIs" dxfId="11" priority="10" operator="equal">
+      <formula>"Siker"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K21">
+    <cfRule type="cellIs" dxfId="10" priority="11" operator="equal">
+      <formula>"Nem futtatható"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K21">
+    <cfRule type="cellIs" dxfId="9" priority="12" operator="equal">
+      <formula>"Hiba"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K22">
+    <cfRule type="cellIs" dxfId="8" priority="7" operator="equal">
+      <formula>"Siker"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K22">
+    <cfRule type="cellIs" dxfId="7" priority="8" operator="equal">
+      <formula>"Nem futtatható"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K22">
+    <cfRule type="cellIs" dxfId="6" priority="9" operator="equal">
+      <formula>"Hiba"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K23">
+    <cfRule type="cellIs" dxfId="5" priority="4" operator="equal">
+      <formula>"Siker"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K23">
+    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
+      <formula>"Nem futtatható"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K23">
+    <cfRule type="cellIs" dxfId="3" priority="6" operator="equal">
+      <formula>"Hiba"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K24">
-    <cfRule type="cellIs" dxfId="164" priority="235" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
       <formula>"Siker"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K24">
-    <cfRule type="cellIs" dxfId="163" priority="236" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>"Nem futtatható"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K24">
-    <cfRule type="cellIs" dxfId="162" priority="237" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="3" operator="equal">
       <formula>"Hiba"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="cellIs" dxfId="161" priority="226" operator="equal">
-      <formula>"Alacsony"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="cellIs" dxfId="160" priority="227" operator="equal">
-      <formula>"Normál"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E25">
-    <cfRule type="cellIs" dxfId="159" priority="228" operator="equal">
-      <formula>"Magas"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K25">
-    <cfRule type="cellIs" dxfId="158" priority="229" operator="equal">
-      <formula>"Siker"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K25">
-    <cfRule type="cellIs" dxfId="157" priority="230" operator="equal">
-      <formula>"Nem futtatható"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K25">
-    <cfRule type="cellIs" dxfId="156" priority="231" operator="equal">
-      <formula>"Hiba"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E26">
-    <cfRule type="cellIs" dxfId="155" priority="223" operator="equal">
-      <formula>"Alacsony"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E26">
-    <cfRule type="cellIs" dxfId="154" priority="224" operator="equal">
-      <formula>"Normál"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E26">
-    <cfRule type="cellIs" dxfId="153" priority="225" operator="equal">
-      <formula>"Magas"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E62:E65">
-    <cfRule type="cellIs" dxfId="152" priority="211" operator="equal">
-      <formula>"Alacsony"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E62:E65">
-    <cfRule type="cellIs" dxfId="151" priority="212" operator="equal">
-      <formula>"Normál"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E62:E65">
-    <cfRule type="cellIs" dxfId="150" priority="213" operator="equal">
-      <formula>"Magas"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K62:K65">
-    <cfRule type="cellIs" dxfId="149" priority="214" operator="equal">
-      <formula>"Siker"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K62:K65">
-    <cfRule type="cellIs" dxfId="148" priority="215" operator="equal">
-      <formula>"Nem futtatható"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K62:K65">
-    <cfRule type="cellIs" dxfId="147" priority="216" operator="equal">
-      <formula>"Hiba"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E66">
-    <cfRule type="cellIs" dxfId="146" priority="205" operator="equal">
-      <formula>"Alacsony"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E66">
-    <cfRule type="cellIs" dxfId="145" priority="206" operator="equal">
-      <formula>"Normál"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E66">
-    <cfRule type="cellIs" dxfId="144" priority="207" operator="equal">
-      <formula>"Magas"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K66:K67">
-    <cfRule type="cellIs" dxfId="143" priority="208" operator="equal">
-      <formula>"Siker"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K66:K67">
-    <cfRule type="cellIs" dxfId="142" priority="209" operator="equal">
-      <formula>"Nem futtatható"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K66:K67">
-    <cfRule type="cellIs" dxfId="141" priority="210" operator="equal">
-      <formula>"Hiba"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E67">
-    <cfRule type="cellIs" dxfId="140" priority="196" operator="equal">
-      <formula>"Alacsony"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E67">
-    <cfRule type="cellIs" dxfId="139" priority="197" operator="equal">
-      <formula>"Normál"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E67">
-    <cfRule type="cellIs" dxfId="138" priority="198" operator="equal">
-      <formula>"Magas"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E68">
-    <cfRule type="cellIs" dxfId="137" priority="190" operator="equal">
-      <formula>"Alacsony"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E68">
-    <cfRule type="cellIs" dxfId="136" priority="191" operator="equal">
-      <formula>"Normál"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E68">
-    <cfRule type="cellIs" dxfId="135" priority="192" operator="equal">
-      <formula>"Magas"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K68">
-    <cfRule type="cellIs" dxfId="134" priority="193" operator="equal">
-      <formula>"Siker"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K68">
-    <cfRule type="cellIs" dxfId="133" priority="194" operator="equal">
-      <formula>"Nem futtatható"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K68">
-    <cfRule type="cellIs" dxfId="132" priority="195" operator="equal">
-      <formula>"Hiba"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E69">
-    <cfRule type="cellIs" dxfId="131" priority="166" operator="equal">
-      <formula>"Alacsony"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E69">
-    <cfRule type="cellIs" dxfId="130" priority="167" operator="equal">
-      <formula>"Normál"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E69">
-    <cfRule type="cellIs" dxfId="129" priority="168" operator="equal">
-      <formula>"Magas"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K69">
-    <cfRule type="cellIs" dxfId="128" priority="169" operator="equal">
-      <formula>"Siker"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K69">
-    <cfRule type="cellIs" dxfId="127" priority="170" operator="equal">
-      <formula>"Nem futtatható"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K69">
-    <cfRule type="cellIs" dxfId="126" priority="171" operator="equal">
-      <formula>"Hiba"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E85:E89 E93:E104">
-    <cfRule type="cellIs" dxfId="125" priority="151" operator="equal">
-      <formula>"Alacsony"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E85:E89 E93:E104">
-    <cfRule type="cellIs" dxfId="124" priority="152" operator="equal">
-      <formula>"Normál"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E85:E89 E93:E104">
-    <cfRule type="cellIs" dxfId="123" priority="153" operator="equal">
-      <formula>"Magas"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K85:K90 K92:K104 K107:K110">
-    <cfRule type="cellIs" dxfId="122" priority="154" operator="equal">
-      <formula>"Siker"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K85:K90 K92:K104 K107:K110">
-    <cfRule type="cellIs" dxfId="121" priority="155" operator="equal">
-      <formula>"Nem futtatható"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K85:K90 K92:K104 K107:K110">
-    <cfRule type="cellIs" dxfId="120" priority="156" operator="equal">
-      <formula>"Hiba"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E90">
-    <cfRule type="cellIs" dxfId="119" priority="148" operator="equal">
-      <formula>"Alacsony"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E90">
-    <cfRule type="cellIs" dxfId="118" priority="149" operator="equal">
-      <formula>"Normál"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E90">
-    <cfRule type="cellIs" dxfId="117" priority="150" operator="equal">
-      <formula>"Magas"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K91">
-    <cfRule type="cellIs" dxfId="116" priority="145" operator="equal">
-      <formula>"Siker"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K91">
-    <cfRule type="cellIs" dxfId="115" priority="146" operator="equal">
-      <formula>"Nem futtatható"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K91">
-    <cfRule type="cellIs" dxfId="114" priority="147" operator="equal">
-      <formula>"Hiba"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E91">
-    <cfRule type="cellIs" dxfId="113" priority="142" operator="equal">
-      <formula>"Alacsony"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E91">
-    <cfRule type="cellIs" dxfId="112" priority="143" operator="equal">
-      <formula>"Normál"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E91">
-    <cfRule type="cellIs" dxfId="111" priority="144" operator="equal">
-      <formula>"Magas"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E92">
-    <cfRule type="cellIs" dxfId="110" priority="139" operator="equal">
-      <formula>"Alacsony"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E92">
-    <cfRule type="cellIs" dxfId="109" priority="140" operator="equal">
-      <formula>"Normál"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E92">
-    <cfRule type="cellIs" dxfId="108" priority="141" operator="equal">
-      <formula>"Magas"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E105">
-    <cfRule type="cellIs" dxfId="107" priority="133" operator="equal">
-      <formula>"Alacsony"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E105">
-    <cfRule type="cellIs" dxfId="106" priority="134" operator="equal">
-      <formula>"Normál"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E105">
-    <cfRule type="cellIs" dxfId="105" priority="135" operator="equal">
-      <formula>"Magas"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K105">
-    <cfRule type="cellIs" dxfId="104" priority="136" operator="equal">
-      <formula>"Siker"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K105">
-    <cfRule type="cellIs" dxfId="103" priority="137" operator="equal">
-      <formula>"Nem futtatható"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K105">
-    <cfRule type="cellIs" dxfId="102" priority="138" operator="equal">
-      <formula>"Hiba"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E106">
-    <cfRule type="cellIs" dxfId="101" priority="127" operator="equal">
-      <formula>"Alacsony"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E106">
-    <cfRule type="cellIs" dxfId="100" priority="128" operator="equal">
-      <formula>"Normál"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E106">
-    <cfRule type="cellIs" dxfId="99" priority="129" operator="equal">
-      <formula>"Magas"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K106">
-    <cfRule type="cellIs" dxfId="98" priority="130" operator="equal">
-      <formula>"Siker"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K106">
-    <cfRule type="cellIs" dxfId="97" priority="131" operator="equal">
-      <formula>"Nem futtatható"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K106">
-    <cfRule type="cellIs" dxfId="96" priority="132" operator="equal">
-      <formula>"Hiba"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E107">
-    <cfRule type="cellIs" dxfId="95" priority="124" operator="equal">
-      <formula>"Alacsony"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E107">
-    <cfRule type="cellIs" dxfId="94" priority="125" operator="equal">
-      <formula>"Normál"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E107">
-    <cfRule type="cellIs" dxfId="93" priority="126" operator="equal">
-      <formula>"Magas"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E108:E109">
-    <cfRule type="cellIs" dxfId="92" priority="121" operator="equal">
-      <formula>"Alacsony"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E108:E109">
-    <cfRule type="cellIs" dxfId="91" priority="122" operator="equal">
-      <formula>"Normál"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E108:E109">
-    <cfRule type="cellIs" dxfId="90" priority="123" operator="equal">
-      <formula>"Magas"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E2">
-    <cfRule type="cellIs" dxfId="89" priority="103" operator="equal">
-      <formula>"Alacsony"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E2">
-    <cfRule type="cellIs" dxfId="88" priority="104" operator="equal">
-      <formula>"Normál"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E2">
-    <cfRule type="cellIs" dxfId="87" priority="105" operator="equal">
-      <formula>"Magas"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K2">
-    <cfRule type="cellIs" dxfId="86" priority="106" operator="equal">
-      <formula>"Siker"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K2">
-    <cfRule type="cellIs" dxfId="85" priority="107" operator="equal">
-      <formula>"Nem futtatható"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K2">
-    <cfRule type="cellIs" dxfId="84" priority="108" operator="equal">
-      <formula>"Hiba"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E9:E10">
-    <cfRule type="cellIs" dxfId="83" priority="97" operator="equal">
-      <formula>"Alacsony"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E9:E10">
-    <cfRule type="cellIs" dxfId="82" priority="98" operator="equal">
-      <formula>"Normál"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E9:E10">
-    <cfRule type="cellIs" dxfId="81" priority="99" operator="equal">
-      <formula>"Magas"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K9:K10">
-    <cfRule type="cellIs" dxfId="80" priority="100" operator="equal">
-      <formula>"Siker"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K9:K10">
-    <cfRule type="cellIs" dxfId="79" priority="101" operator="equal">
-      <formula>"Nem futtatható"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K9:K10">
-    <cfRule type="cellIs" dxfId="78" priority="102" operator="equal">
-      <formula>"Hiba"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E10">
-    <cfRule type="cellIs" dxfId="77" priority="91" operator="equal">
-      <formula>"Alacsony"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E10">
-    <cfRule type="cellIs" dxfId="76" priority="92" operator="equal">
-      <formula>"Normál"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E10">
-    <cfRule type="cellIs" dxfId="75" priority="93" operator="equal">
-      <formula>"Magas"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K10">
-    <cfRule type="cellIs" dxfId="74" priority="94" operator="equal">
-      <formula>"Siker"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K10">
-    <cfRule type="cellIs" dxfId="73" priority="95" operator="equal">
-      <formula>"Nem futtatható"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K10">
-    <cfRule type="cellIs" dxfId="72" priority="96" operator="equal">
-      <formula>"Hiba"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E23">
-    <cfRule type="cellIs" dxfId="71" priority="79" operator="equal">
-      <formula>"Alacsony"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E23">
-    <cfRule type="cellIs" dxfId="70" priority="80" operator="equal">
-      <formula>"Normál"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E23">
-    <cfRule type="cellIs" dxfId="69" priority="81" operator="equal">
-      <formula>"Magas"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K23">
-    <cfRule type="cellIs" dxfId="68" priority="82" operator="equal">
-      <formula>"Siker"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K23">
-    <cfRule type="cellIs" dxfId="67" priority="83" operator="equal">
-      <formula>"Nem futtatható"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K23">
-    <cfRule type="cellIs" dxfId="66" priority="84" operator="equal">
-      <formula>"Hiba"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E4">
-    <cfRule type="cellIs" dxfId="65" priority="76" operator="equal">
-      <formula>"Alacsony"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E4">
-    <cfRule type="cellIs" dxfId="64" priority="77" operator="equal">
-      <formula>"Normál"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E4">
-    <cfRule type="cellIs" dxfId="63" priority="78" operator="equal">
-      <formula>"Magas"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E5">
-    <cfRule type="cellIs" dxfId="62" priority="73" operator="equal">
-      <formula>"Alacsony"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E5">
-    <cfRule type="cellIs" dxfId="61" priority="74" operator="equal">
-      <formula>"Normál"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E5">
-    <cfRule type="cellIs" dxfId="60" priority="75" operator="equal">
-      <formula>"Magas"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E6">
-    <cfRule type="cellIs" dxfId="59" priority="70" operator="equal">
-      <formula>"Alacsony"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E6">
-    <cfRule type="cellIs" dxfId="58" priority="71" operator="equal">
-      <formula>"Normál"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E6">
-    <cfRule type="cellIs" dxfId="57" priority="72" operator="equal">
-      <formula>"Magas"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E7">
-    <cfRule type="cellIs" dxfId="56" priority="67" operator="equal">
-      <formula>"Alacsony"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E7">
-    <cfRule type="cellIs" dxfId="55" priority="68" operator="equal">
-      <formula>"Normál"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E7">
-    <cfRule type="cellIs" dxfId="54" priority="69" operator="equal">
-      <formula>"Magas"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E8">
-    <cfRule type="cellIs" dxfId="53" priority="64" operator="equal">
-      <formula>"Alacsony"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E8">
-    <cfRule type="cellIs" dxfId="52" priority="65" operator="equal">
-      <formula>"Normál"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E8">
-    <cfRule type="cellIs" dxfId="51" priority="66" operator="equal">
-      <formula>"Magas"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E11">
-    <cfRule type="cellIs" dxfId="50" priority="61" operator="equal">
-      <formula>"Alacsony"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E11">
-    <cfRule type="cellIs" dxfId="49" priority="62" operator="equal">
-      <formula>"Normál"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E11">
-    <cfRule type="cellIs" dxfId="48" priority="63" operator="equal">
-      <formula>"Magas"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E12">
-    <cfRule type="cellIs" dxfId="47" priority="58" operator="equal">
-      <formula>"Alacsony"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E12">
-    <cfRule type="cellIs" dxfId="46" priority="59" operator="equal">
-      <formula>"Normál"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E12">
-    <cfRule type="cellIs" dxfId="45" priority="60" operator="equal">
-      <formula>"Magas"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E13">
-    <cfRule type="cellIs" dxfId="44" priority="55" operator="equal">
-      <formula>"Alacsony"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E13">
-    <cfRule type="cellIs" dxfId="43" priority="56" operator="equal">
-      <formula>"Normál"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E13">
-    <cfRule type="cellIs" dxfId="42" priority="57" operator="equal">
-      <formula>"Magas"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E14">
-    <cfRule type="cellIs" dxfId="41" priority="52" operator="equal">
-      <formula>"Alacsony"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E14">
-    <cfRule type="cellIs" dxfId="40" priority="53" operator="equal">
-      <formula>"Normál"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E14">
-    <cfRule type="cellIs" dxfId="39" priority="54" operator="equal">
-      <formula>"Magas"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E15">
-    <cfRule type="cellIs" dxfId="38" priority="49" operator="equal">
-      <formula>"Alacsony"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E15">
-    <cfRule type="cellIs" dxfId="37" priority="50" operator="equal">
-      <formula>"Normál"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E15">
-    <cfRule type="cellIs" dxfId="36" priority="51" operator="equal">
-      <formula>"Magas"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E20">
-    <cfRule type="cellIs" dxfId="35" priority="43" operator="equal">
-      <formula>"Alacsony"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E20">
-    <cfRule type="cellIs" dxfId="34" priority="44" operator="equal">
-      <formula>"Normál"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E20">
-    <cfRule type="cellIs" dxfId="33" priority="45" operator="equal">
-      <formula>"Magas"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K20">
-    <cfRule type="cellIs" dxfId="32" priority="46" operator="equal">
-      <formula>"Siker"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K20">
-    <cfRule type="cellIs" dxfId="31" priority="47" operator="equal">
-      <formula>"Nem futtatható"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K20">
-    <cfRule type="cellIs" dxfId="30" priority="48" operator="equal">
-      <formula>"Hiba"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E19">
-    <cfRule type="cellIs" dxfId="29" priority="37" operator="equal">
-      <formula>"Alacsony"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E19">
-    <cfRule type="cellIs" dxfId="28" priority="38" operator="equal">
-      <formula>"Normál"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E19">
-    <cfRule type="cellIs" dxfId="27" priority="39" operator="equal">
-      <formula>"Magas"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K19">
-    <cfRule type="cellIs" dxfId="26" priority="40" operator="equal">
-      <formula>"Siker"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K19">
-    <cfRule type="cellIs" dxfId="25" priority="41" operator="equal">
-      <formula>"Nem futtatható"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K19">
-    <cfRule type="cellIs" dxfId="24" priority="42" operator="equal">
-      <formula>"Hiba"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E18">
-    <cfRule type="cellIs" dxfId="23" priority="31" operator="equal">
-      <formula>"Alacsony"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E18">
-    <cfRule type="cellIs" dxfId="22" priority="32" operator="equal">
-      <formula>"Normál"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E18">
-    <cfRule type="cellIs" dxfId="21" priority="33" operator="equal">
-      <formula>"Magas"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K18">
-    <cfRule type="cellIs" dxfId="20" priority="34" operator="equal">
-      <formula>"Siker"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K18">
-    <cfRule type="cellIs" dxfId="19" priority="35" operator="equal">
-      <formula>"Nem futtatható"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K18">
-    <cfRule type="cellIs" dxfId="18" priority="36" operator="equal">
-      <formula>"Hiba"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E21">
-    <cfRule type="cellIs" dxfId="17" priority="25" operator="equal">
-      <formula>"Alacsony"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E21">
-    <cfRule type="cellIs" dxfId="16" priority="26" operator="equal">
-      <formula>"Normál"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E21">
-    <cfRule type="cellIs" dxfId="15" priority="27" operator="equal">
-      <formula>"Magas"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K21">
-    <cfRule type="cellIs" dxfId="14" priority="28" operator="equal">
-      <formula>"Siker"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K21">
-    <cfRule type="cellIs" dxfId="13" priority="29" operator="equal">
-      <formula>"Nem futtatható"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K21">
-    <cfRule type="cellIs" dxfId="12" priority="30" operator="equal">
-      <formula>"Hiba"</formula>
-    </cfRule>
-  </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" sqref="K2:K110" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" sqref="K2:K111" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"Siker,Nem futtatható,Hiba"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" sqref="E2:E1048576" xr:uid="{D77BF901-4E7C-4E22-8ACE-0D8DD0ED0558}">
@@ -17341,62 +18255,62 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B6">
-    <cfRule type="cellIs" dxfId="11" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="74" priority="1" operator="equal">
       <formula>"Alacsony"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B6">
-    <cfRule type="cellIs" dxfId="10" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="73" priority="2" operator="equal">
       <formula>"Normál"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B6">
-    <cfRule type="cellIs" dxfId="9" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="72" priority="3" operator="equal">
       <formula>"Magas"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C6:E6">
-    <cfRule type="cellIs" dxfId="8" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="71" priority="4" operator="equal">
       <formula>"Alacsony"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C6:E6">
-    <cfRule type="cellIs" dxfId="7" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="70" priority="5" operator="equal">
       <formula>"Normál"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C6:E6">
-    <cfRule type="cellIs" dxfId="6" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="69" priority="6" operator="equal">
       <formula>"Magas"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B7">
-    <cfRule type="cellIs" dxfId="5" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="68" priority="7" operator="equal">
       <formula>"Alacsony"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B7">
-    <cfRule type="cellIs" dxfId="4" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="67" priority="8" operator="equal">
       <formula>"Normál"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B7">
-    <cfRule type="cellIs" dxfId="3" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="66" priority="9" operator="equal">
       <formula>"Magas"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C7:E7">
-    <cfRule type="cellIs" dxfId="2" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="65" priority="10" operator="equal">
       <formula>"Alacsony"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C7:E7">
-    <cfRule type="cellIs" dxfId="1" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="64" priority="11" operator="equal">
       <formula>"Normál"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C7:E7">
-    <cfRule type="cellIs" dxfId="0" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="63" priority="12" operator="equal">
       <formula>"Magas"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Refactoring, add defect report
</commit_message>
<xml_diff>
--- a/Test_Cases.xlsx
+++ b/Test_Cases.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vivike\Desktop\autotesting\vizsgaremeknew\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDC8AF4D-1670-4034-A1BD-063CFD9A51F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11829B62-2214-4FD4-9412-12F23A0955FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="tesztesetek (test case)" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="639" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="661" uniqueCount="171">
   <si>
     <t>Azonosító (ID)</t>
   </si>
@@ -300,9 +300,6 @@
   </si>
   <si>
     <t>Sikeres regisztrációra utaló felirat jelenik meg</t>
-  </si>
-  <si>
-    <t>Hibás regisztrációra utaló felirat jelenik meg</t>
   </si>
   <si>
     <t>Sikeres sign in, a Landing page jelenik meg</t>
@@ -622,13 +619,6 @@
     <t>invalidEmailRegistrationData.csv</t>
   </si>
   <si>
-    <t>1. Navigálj a portioUrl oldalra
-3. Regisztrációhoz olvasd be az adatokat a invalidEmailRegistrationData.csv fájlból</t>
-  </si>
-  <si>
-    <t>NEM jelenik meg sikeres regisztrációra utaló felirat</t>
-  </si>
-  <si>
     <t>Hiba</t>
   </si>
   <si>
@@ -636,6 +626,28 @@
   </si>
   <si>
     <t>Sorozatos regisztráció különböző, helytelen email címekkel</t>
+  </si>
+  <si>
+    <t>BUG2</t>
+  </si>
+  <si>
+    <t>BUG1</t>
+  </si>
+  <si>
+    <t>Fejlesztő</t>
+  </si>
+  <si>
+    <t>NEM jelenik meg sikeres regisztrációra utaló felirat/ Hibás regisztrációra utaló felirat jelenik meg</t>
+  </si>
+  <si>
+    <t>1. Navigálj a portioUrl oldalra
+3. Regisztrációhoz olvasd be az adatokat az invalidEmailRegistrationData.csv fájlból</t>
+  </si>
+  <si>
+    <t>Regisztráció üres adatokkal is lehetséges</t>
+  </si>
+  <si>
+    <t>Sorozatos regisztráció különböző, helytelen email címekkel is lehetséges</t>
   </si>
 </sst>
 </file>
@@ -738,7 +750,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -776,179 +788,14 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="4" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="252">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFEA9999"/>
-          <bgColor rgb="FFEA9999"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFE598"/>
-          <bgColor rgb="FFFFE598"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB7E1CD"/>
-          <bgColor rgb="FFB7E1CD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFEA9999"/>
-          <bgColor rgb="FFEA9999"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFE598"/>
-          <bgColor rgb="FFFFE598"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB7E1CD"/>
-          <bgColor rgb="FFB7E1CD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFEA9999"/>
-          <bgColor rgb="FFEA9999"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFE598"/>
-          <bgColor rgb="FFFFE598"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB7E1CD"/>
-          <bgColor rgb="FFB7E1CD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFEA9999"/>
-          <bgColor rgb="FFEA9999"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFE598"/>
-          <bgColor rgb="FFFFE598"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB7E1CD"/>
-          <bgColor rgb="FFB7E1CD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFEA9999"/>
-          <bgColor rgb="FFEA9999"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFE598"/>
-          <bgColor rgb="FFFFE598"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB7E1CD"/>
-          <bgColor rgb="FFB7E1CD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFEA9999"/>
-          <bgColor rgb="FFEA9999"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFE598"/>
-          <bgColor rgb="FFFFE598"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB7E1CD"/>
-          <bgColor rgb="FFB7E1CD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFEA9999"/>
-          <bgColor rgb="FFEA9999"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFE598"/>
-          <bgColor rgb="FFFFE598"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFB7E1CD"/>
-          <bgColor rgb="FFB7E1CD"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="231">
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -3059,9 +2906,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Y1009"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D11" sqref="D11"/>
+      <selection pane="bottomLeft" activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1"/>
@@ -3145,7 +2992,7 @@
         <v>65</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>49</v>
@@ -3163,7 +3010,7 @@
         <v>66</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="L2" s="4"/>
       <c r="M2" s="2"/>
@@ -3185,7 +3032,7 @@
         <v>14</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>55</v>
@@ -3194,7 +3041,7 @@
         <v>65</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>49</v>
@@ -3212,7 +3059,7 @@
         <v>79</v>
       </c>
       <c r="K3" s="14" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="L3" s="4"/>
       <c r="M3" s="2"/>
@@ -3234,7 +3081,7 @@
         <v>15</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>56</v>
@@ -3243,7 +3090,7 @@
         <v>65</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>49</v>
@@ -3261,7 +3108,7 @@
         <v>79</v>
       </c>
       <c r="K4" s="14" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="L4" s="4"/>
       <c r="M4" s="2"/>
@@ -3283,7 +3130,7 @@
         <v>16</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>57</v>
@@ -3292,7 +3139,7 @@
         <v>65</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F5" s="3" t="s">
         <v>49</v>
@@ -3310,7 +3157,7 @@
         <v>72</v>
       </c>
       <c r="K5" s="14" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="L5" s="4"/>
       <c r="M5" s="2"/>
@@ -3332,7 +3179,7 @@
         <v>17</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>58</v>
@@ -3341,16 +3188,16 @@
         <v>65</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F6" s="3" t="s">
         <v>49</v>
       </c>
       <c r="G6" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="H6" s="5" t="s">
         <v>88</v>
-      </c>
-      <c r="H6" s="5" t="s">
-        <v>89</v>
       </c>
       <c r="I6" s="3" t="s">
         <v>80</v>
@@ -3359,7 +3206,7 @@
         <v>80</v>
       </c>
       <c r="K6" s="14" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="L6" s="4"/>
       <c r="M6" s="2"/>
@@ -3381,7 +3228,7 @@
         <v>18</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>59</v>
@@ -3390,13 +3237,13 @@
         <v>65</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F7" s="3" t="s">
         <v>49</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H7" s="5" t="s">
         <v>50</v>
@@ -3408,7 +3255,7 @@
         <v>81</v>
       </c>
       <c r="K7" s="14" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="L7" s="4"/>
       <c r="M7" s="2"/>
@@ -3439,27 +3286,29 @@
         <v>65</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F8" s="3" t="s">
         <v>49</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H8" s="5" t="s">
         <v>61</v>
       </c>
       <c r="I8" s="5" t="s">
-        <v>82</v>
+        <v>167</v>
       </c>
       <c r="J8" s="16" t="s">
         <v>81</v>
       </c>
       <c r="K8" s="5" t="s">
-        <v>164</v>
-      </c>
-      <c r="L8" s="4"/>
+        <v>161</v>
+      </c>
+      <c r="L8" s="4" t="s">
+        <v>165</v>
+      </c>
       <c r="M8" s="2"/>
       <c r="N8" s="2"/>
       <c r="O8" s="2"/>
@@ -3479,7 +3328,7 @@
         <v>20</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C9" s="5" t="s">
         <v>62</v>
@@ -3494,7 +3343,7 @@
         <v>49</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H9" s="5" t="s">
         <v>51</v>
@@ -3506,7 +3355,7 @@
         <v>81</v>
       </c>
       <c r="K9" s="14" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="L9" s="4"/>
       <c r="M9" s="2"/>
@@ -3528,10 +3377,10 @@
         <v>21</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>65</v>
@@ -3543,10 +3392,10 @@
         <v>49</v>
       </c>
       <c r="G10" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="H10" s="5" t="s">
         <v>158</v>
-      </c>
-      <c r="H10" s="5" t="s">
-        <v>159</v>
       </c>
       <c r="I10" s="5" t="s">
         <v>81</v>
@@ -3555,7 +3404,7 @@
         <v>81</v>
       </c>
       <c r="K10" s="14" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="L10" s="4"/>
       <c r="M10" s="2"/>
@@ -3577,36 +3426,38 @@
         <v>22</v>
       </c>
       <c r="B11" s="14" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C11" s="16" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="D11" s="14" t="s">
         <v>65</v>
       </c>
       <c r="E11" s="14" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F11" s="14" t="s">
         <v>49</v>
       </c>
       <c r="G11" s="14" t="s">
-        <v>162</v>
+        <v>168</v>
       </c>
       <c r="H11" s="16" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="I11" s="16" t="s">
-        <v>163</v>
+        <v>167</v>
       </c>
       <c r="J11" s="16" t="s">
         <v>81</v>
       </c>
       <c r="K11" s="16" t="s">
+        <v>161</v>
+      </c>
+      <c r="L11" s="15" t="s">
         <v>164</v>
       </c>
-      <c r="L11" s="15"/>
       <c r="M11" s="13"/>
       <c r="N11" s="13"/>
       <c r="O11" s="13"/>
@@ -3626,7 +3477,7 @@
         <v>23</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C12" s="5" t="s">
         <v>63</v>
@@ -3635,25 +3486,25 @@
         <v>65</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F12" s="3" t="s">
         <v>49</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="H12" s="5" t="s">
         <v>73</v>
       </c>
       <c r="I12" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J12" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K12" s="14" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="L12" s="4"/>
       <c r="M12" s="2"/>
@@ -3675,34 +3526,34 @@
         <v>24</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D13" s="3" t="s">
         <v>65</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F13" s="3" t="s">
         <v>49</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="H13" s="5" t="s">
         <v>74</v>
       </c>
       <c r="I13" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="J13" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="K13" s="14" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="L13" s="4"/>
       <c r="M13" s="2"/>
@@ -3724,34 +3575,34 @@
         <v>25</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>65</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F14" s="3" t="s">
         <v>49</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="H14" s="5" t="s">
         <v>75</v>
       </c>
       <c r="I14" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="J14" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="K14" s="14" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="L14" s="4"/>
       <c r="M14" s="9"/>
@@ -3773,34 +3624,34 @@
         <v>26</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D15" s="3" t="s">
         <v>65</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F15" s="3" t="s">
         <v>49</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H15" s="5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I15" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="J15" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="K15" s="14" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="L15" s="4"/>
       <c r="M15" s="9"/>
@@ -3831,25 +3682,25 @@
         <v>65</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F16" s="3" t="s">
         <v>49</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H16" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="I16" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="I16" s="5" t="s">
-        <v>87</v>
-      </c>
       <c r="J16" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="K16" s="14" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="L16" s="4"/>
       <c r="M16" s="9"/>
@@ -3871,10 +3722,10 @@
         <v>28</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D17" s="3" t="s">
         <v>65</v>
@@ -3886,19 +3737,19 @@
         <v>49</v>
       </c>
       <c r="G17" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="H17" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="H17" s="5" t="s">
+      <c r="I17" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="I17" s="5" t="s">
-        <v>100</v>
-      </c>
       <c r="J17" s="5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="K17" s="14" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="L17" s="4"/>
       <c r="M17" s="9"/>
@@ -3920,10 +3771,10 @@
         <v>29</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D18" s="3" t="s">
         <v>65</v>
@@ -3935,19 +3786,19 @@
         <v>49</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H18" s="5" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="I18" s="5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="J18" s="5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="K18" s="14" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="L18" s="4"/>
       <c r="M18" s="2"/>
@@ -3969,34 +3820,34 @@
         <v>30</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D19" s="3" t="s">
         <v>65</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F19" s="3" t="s">
         <v>49</v>
       </c>
       <c r="G19" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="H19" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="H19" s="5" t="s">
-        <v>109</v>
-      </c>
       <c r="I19" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="J19" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="K19" s="14" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="L19" s="4"/>
       <c r="M19" s="2"/>
@@ -4018,34 +3869,34 @@
         <v>31</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D20" s="3" t="s">
         <v>65</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F20" s="3" t="s">
         <v>49</v>
       </c>
       <c r="G20" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="H20" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="H20" s="5" t="s">
-        <v>111</v>
-      </c>
       <c r="I20" s="5" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="J20" s="5" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="K20" s="14" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="L20" s="4"/>
       <c r="M20" s="2"/>
@@ -4064,37 +3915,37 @@
     </row>
     <row r="21" spans="1:25" ht="49.5" thickTop="1" thickBot="1">
       <c r="A21" s="14" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B21" s="14" t="s">
+        <v>139</v>
+      </c>
+      <c r="C21" s="5" t="s">
         <v>140</v>
-      </c>
-      <c r="C21" s="5" t="s">
-        <v>141</v>
       </c>
       <c r="D21" s="3" t="s">
         <v>65</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F21" s="3" t="s">
         <v>49</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="H21" s="5" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="I21" s="5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="J21" s="5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="K21" s="14" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="L21" s="4"/>
       <c r="M21" s="2"/>
@@ -4113,13 +3964,13 @@
     </row>
     <row r="22" spans="1:25" s="12" customFormat="1" ht="73.5" thickTop="1" thickBot="1">
       <c r="A22" s="14" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B22" s="14" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C22" s="16" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D22" s="14" t="s">
         <v>65</v>
@@ -4131,19 +3982,19 @@
         <v>49</v>
       </c>
       <c r="G22" s="14" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="H22" s="16" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="I22" s="16" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="J22" s="16" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="K22" s="14" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="L22" s="15"/>
       <c r="M22" s="13"/>
@@ -4162,37 +4013,37 @@
     </row>
     <row r="23" spans="1:25" ht="49.5" thickTop="1" thickBot="1">
       <c r="A23" s="14" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D23" s="3" t="s">
         <v>65</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F23" s="3" t="s">
         <v>49</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="H23" s="16" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="I23" s="16" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="J23" s="16" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="K23" s="14" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="L23" s="4"/>
       <c r="M23" s="2"/>
@@ -4211,13 +4062,13 @@
     </row>
     <row r="24" spans="1:25" ht="97.5" thickTop="1" thickBot="1">
       <c r="A24" s="14" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D24" s="3" t="s">
         <v>65</v>
@@ -4229,19 +4080,19 @@
         <v>49</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="H24" s="5" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="I24" s="5" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="J24" s="16" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="K24" s="14" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="L24" s="4"/>
       <c r="M24" s="2"/>
@@ -4272,7 +4123,7 @@
         <v>49</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H25" s="5"/>
       <c r="I25" s="5"/>
@@ -4307,7 +4158,7 @@
         <v>49</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H26" s="5"/>
       <c r="I26" s="5"/>
@@ -4342,7 +4193,7 @@
         <v>49</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H27" s="5"/>
       <c r="I27" s="5"/>
@@ -4377,7 +4228,7 @@
         <v>49</v>
       </c>
       <c r="G28" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H28" s="5"/>
       <c r="I28" s="5"/>
@@ -4412,7 +4263,7 @@
         <v>49</v>
       </c>
       <c r="G29" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H29" s="5"/>
       <c r="I29" s="5"/>
@@ -4447,7 +4298,7 @@
         <v>49</v>
       </c>
       <c r="G30" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H30" s="5"/>
       <c r="I30" s="7"/>
@@ -4482,7 +4333,7 @@
         <v>49</v>
       </c>
       <c r="G31" s="14" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H31" s="16"/>
       <c r="I31" s="7"/>
@@ -4517,7 +4368,7 @@
         <v>49</v>
       </c>
       <c r="G32" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H32" s="5"/>
       <c r="I32" s="3"/>
@@ -4552,7 +4403,7 @@
         <v>49</v>
       </c>
       <c r="G33" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H33" s="5"/>
       <c r="I33" s="3"/>
@@ -4574,7 +4425,7 @@
         <v>49</v>
       </c>
       <c r="G34" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H34" s="5"/>
       <c r="I34" s="3"/>
@@ -4609,7 +4460,7 @@
         <v>49</v>
       </c>
       <c r="G35" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H35" s="5"/>
       <c r="I35" s="3"/>
@@ -4644,7 +4495,7 @@
         <v>49</v>
       </c>
       <c r="G36" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H36" s="5"/>
       <c r="I36" s="3"/>
@@ -4679,7 +4530,7 @@
         <v>49</v>
       </c>
       <c r="G37" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H37" s="5"/>
       <c r="I37" s="3"/>
@@ -4714,7 +4565,7 @@
         <v>49</v>
       </c>
       <c r="G38" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H38" s="5"/>
       <c r="I38" s="3"/>
@@ -4749,7 +4600,7 @@
         <v>49</v>
       </c>
       <c r="G39" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H39" s="5"/>
       <c r="I39" s="3"/>
@@ -4784,7 +4635,7 @@
         <v>49</v>
       </c>
       <c r="G40" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H40" s="5"/>
       <c r="I40" s="3"/>
@@ -4819,7 +4670,7 @@
         <v>49</v>
       </c>
       <c r="G41" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H41" s="5"/>
       <c r="I41" s="3"/>
@@ -4854,7 +4705,7 @@
         <v>49</v>
       </c>
       <c r="G42" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H42" s="5"/>
       <c r="I42" s="3"/>
@@ -4889,7 +4740,7 @@
         <v>49</v>
       </c>
       <c r="G43" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H43" s="5"/>
       <c r="I43" s="3"/>
@@ -4924,7 +4775,7 @@
         <v>49</v>
       </c>
       <c r="G44" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H44" s="5"/>
       <c r="I44" s="3"/>
@@ -4959,7 +4810,7 @@
         <v>49</v>
       </c>
       <c r="G45" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H45" s="5"/>
       <c r="I45" s="3"/>
@@ -4994,7 +4845,7 @@
         <v>49</v>
       </c>
       <c r="G46" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H46" s="5"/>
       <c r="I46" s="3"/>
@@ -5029,7 +4880,7 @@
         <v>49</v>
       </c>
       <c r="G47" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H47" s="5"/>
       <c r="I47" s="3"/>
@@ -5064,7 +4915,7 @@
         <v>49</v>
       </c>
       <c r="G48" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H48" s="5"/>
       <c r="I48" s="3"/>
@@ -5099,7 +4950,7 @@
         <v>49</v>
       </c>
       <c r="G49" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H49" s="5"/>
       <c r="I49" s="3"/>
@@ -5134,7 +4985,7 @@
         <v>49</v>
       </c>
       <c r="G50" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H50" s="5"/>
       <c r="I50" s="3"/>
@@ -5169,7 +5020,7 @@
         <v>49</v>
       </c>
       <c r="G51" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H51" s="5"/>
       <c r="I51" s="3"/>
@@ -5204,7 +5055,7 @@
         <v>49</v>
       </c>
       <c r="G52" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H52" s="5"/>
       <c r="I52" s="3"/>
@@ -5239,7 +5090,7 @@
         <v>49</v>
       </c>
       <c r="G53" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H53" s="5"/>
       <c r="I53" s="3"/>
@@ -5274,7 +5125,7 @@
         <v>49</v>
       </c>
       <c r="G54" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H54" s="5"/>
       <c r="I54" s="3"/>
@@ -5309,7 +5160,7 @@
         <v>49</v>
       </c>
       <c r="G55" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H55" s="5"/>
       <c r="I55" s="3"/>
@@ -5344,7 +5195,7 @@
         <v>49</v>
       </c>
       <c r="G56" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H56" s="5"/>
       <c r="I56" s="3"/>
@@ -5379,7 +5230,7 @@
         <v>49</v>
       </c>
       <c r="G57" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H57" s="5"/>
       <c r="I57" s="3"/>
@@ -5414,7 +5265,7 @@
         <v>49</v>
       </c>
       <c r="G58" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H58" s="5"/>
       <c r="I58" s="3"/>
@@ -5449,7 +5300,7 @@
         <v>49</v>
       </c>
       <c r="G59" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H59" s="5"/>
       <c r="I59" s="3"/>
@@ -5484,7 +5335,7 @@
         <v>49</v>
       </c>
       <c r="G60" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H60" s="5"/>
       <c r="I60" s="3"/>
@@ -5519,7 +5370,7 @@
         <v>49</v>
       </c>
       <c r="G61" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H61" s="5"/>
       <c r="I61" s="3"/>
@@ -5554,7 +5405,7 @@
         <v>49</v>
       </c>
       <c r="G62" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H62" s="5"/>
       <c r="I62" s="3"/>
@@ -5589,7 +5440,7 @@
         <v>49</v>
       </c>
       <c r="G63" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H63" s="5"/>
       <c r="I63" s="3"/>
@@ -5624,7 +5475,7 @@
         <v>49</v>
       </c>
       <c r="G64" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H64" s="5"/>
       <c r="I64" s="5"/>
@@ -5659,7 +5510,7 @@
         <v>49</v>
       </c>
       <c r="G65" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H65" s="5"/>
       <c r="I65" s="5"/>
@@ -5694,7 +5545,7 @@
         <v>49</v>
       </c>
       <c r="G66" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H66" s="5"/>
       <c r="I66" s="5"/>
@@ -5729,7 +5580,7 @@
         <v>49</v>
       </c>
       <c r="G67" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H67" s="5"/>
       <c r="I67" s="5"/>
@@ -5764,7 +5615,7 @@
         <v>49</v>
       </c>
       <c r="G68" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H68" s="5"/>
       <c r="I68" s="5"/>
@@ -5799,7 +5650,7 @@
         <v>49</v>
       </c>
       <c r="G69" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H69" s="5"/>
       <c r="I69" s="5"/>
@@ -5833,7 +5684,7 @@
         <v>49</v>
       </c>
       <c r="G70" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H70" s="5"/>
       <c r="I70" s="5"/>
@@ -5868,7 +5719,7 @@
         <v>49</v>
       </c>
       <c r="G71" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H71" s="5"/>
       <c r="I71" s="5"/>
@@ -5902,7 +5753,7 @@
         <v>49</v>
       </c>
       <c r="G72" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H72" s="5"/>
       <c r="I72" s="5"/>
@@ -5937,7 +5788,7 @@
         <v>49</v>
       </c>
       <c r="G73" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H73" s="5"/>
       <c r="I73" s="5"/>
@@ -5972,7 +5823,7 @@
         <v>49</v>
       </c>
       <c r="G74" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H74" s="5"/>
       <c r="I74" s="5"/>
@@ -6006,7 +5857,7 @@
         <v>49</v>
       </c>
       <c r="G75" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H75" s="5"/>
       <c r="I75" s="5"/>
@@ -6040,7 +5891,7 @@
         <v>49</v>
       </c>
       <c r="G76" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H76" s="11"/>
       <c r="I76" s="5"/>
@@ -6074,7 +5925,7 @@
         <v>49</v>
       </c>
       <c r="G77" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H77" s="5"/>
       <c r="I77" s="5"/>
@@ -6108,7 +5959,7 @@
         <v>49</v>
       </c>
       <c r="G78" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H78" s="5"/>
       <c r="I78" s="5"/>
@@ -6142,7 +5993,7 @@
         <v>49</v>
       </c>
       <c r="G79" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H79" s="5"/>
       <c r="I79" s="5"/>
@@ -6176,7 +6027,7 @@
         <v>49</v>
       </c>
       <c r="G80" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H80" s="5"/>
       <c r="I80" s="5"/>
@@ -6210,7 +6061,7 @@
         <v>49</v>
       </c>
       <c r="G81" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H81" s="5"/>
       <c r="I81" s="5"/>
@@ -6244,7 +6095,7 @@
         <v>49</v>
       </c>
       <c r="G82" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H82" s="5"/>
       <c r="I82" s="5"/>
@@ -6278,7 +6129,7 @@
         <v>49</v>
       </c>
       <c r="G83" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H83" s="5"/>
       <c r="I83" s="5"/>
@@ -6312,7 +6163,7 @@
         <v>49</v>
       </c>
       <c r="G84" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H84" s="5"/>
       <c r="I84" s="5"/>
@@ -6346,7 +6197,7 @@
         <v>49</v>
       </c>
       <c r="G85" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H85" s="5"/>
       <c r="I85" s="5"/>
@@ -6380,7 +6231,7 @@
         <v>49</v>
       </c>
       <c r="G86" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H86" s="5"/>
       <c r="I86" s="3"/>
@@ -6415,7 +6266,7 @@
         <v>49</v>
       </c>
       <c r="G87" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H87" s="5"/>
       <c r="I87" s="5"/>
@@ -6450,7 +6301,7 @@
         <v>49</v>
       </c>
       <c r="G88" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H88" s="5"/>
       <c r="I88" s="5"/>
@@ -6485,7 +6336,7 @@
         <v>49</v>
       </c>
       <c r="G89" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H89" s="5"/>
       <c r="I89" s="5"/>
@@ -6520,7 +6371,7 @@
         <v>49</v>
       </c>
       <c r="G90" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H90" s="5"/>
       <c r="I90" s="5"/>
@@ -6555,7 +6406,7 @@
         <v>49</v>
       </c>
       <c r="G91" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H91" s="5"/>
       <c r="I91" s="5"/>
@@ -6590,7 +6441,7 @@
         <v>49</v>
       </c>
       <c r="G92" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H92" s="5"/>
       <c r="I92" s="5"/>
@@ -6625,7 +6476,7 @@
         <v>49</v>
       </c>
       <c r="G93" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H93" s="5"/>
       <c r="I93" s="5"/>
@@ -6660,7 +6511,7 @@
         <v>49</v>
       </c>
       <c r="G94" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H94" s="5"/>
       <c r="I94" s="5"/>
@@ -6695,7 +6546,7 @@
         <v>49</v>
       </c>
       <c r="G95" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H95" s="5"/>
       <c r="I95" s="5"/>
@@ -6730,7 +6581,7 @@
         <v>49</v>
       </c>
       <c r="G96" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H96" s="5"/>
       <c r="I96" s="5"/>
@@ -6765,7 +6616,7 @@
         <v>49</v>
       </c>
       <c r="G97" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H97" s="5"/>
       <c r="I97" s="5"/>
@@ -6800,7 +6651,7 @@
         <v>49</v>
       </c>
       <c r="G98" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H98" s="5"/>
       <c r="I98" s="5"/>
@@ -6835,7 +6686,7 @@
         <v>49</v>
       </c>
       <c r="G99" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H99" s="5"/>
       <c r="I99" s="5"/>
@@ -6870,7 +6721,7 @@
         <v>49</v>
       </c>
       <c r="G100" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H100" s="5"/>
       <c r="I100" s="5"/>
@@ -6905,7 +6756,7 @@
         <v>49</v>
       </c>
       <c r="G101" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H101" s="5"/>
       <c r="I101" s="5"/>
@@ -6940,7 +6791,7 @@
         <v>49</v>
       </c>
       <c r="G102" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H102" s="5"/>
       <c r="I102" s="5"/>
@@ -6975,7 +6826,7 @@
         <v>49</v>
       </c>
       <c r="G103" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H103" s="5"/>
       <c r="I103" s="5"/>
@@ -7010,7 +6861,7 @@
         <v>49</v>
       </c>
       <c r="G104" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H104" s="5"/>
       <c r="I104" s="5"/>
@@ -7045,7 +6896,7 @@
         <v>49</v>
       </c>
       <c r="G105" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H105" s="5"/>
       <c r="I105" s="5"/>
@@ -7080,7 +6931,7 @@
         <v>49</v>
       </c>
       <c r="G106" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H106" s="5"/>
       <c r="I106" s="5"/>
@@ -7115,7 +6966,7 @@
         <v>49</v>
       </c>
       <c r="G107" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H107" s="5"/>
       <c r="I107" s="5"/>
@@ -7150,7 +7001,7 @@
         <v>49</v>
       </c>
       <c r="G108" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H108" s="5"/>
       <c r="I108" s="5"/>
@@ -7185,7 +7036,7 @@
         <v>49</v>
       </c>
       <c r="G109" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H109" s="5"/>
       <c r="I109" s="5"/>
@@ -7220,7 +7071,7 @@
         <v>49</v>
       </c>
       <c r="G110" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H110" s="5"/>
       <c r="I110" s="5"/>
@@ -11052,1097 +10903,1097 @@
   </sheetData>
   <phoneticPr fontId="7" type="noConversion"/>
   <conditionalFormatting sqref="E23:E30 E2:E18 E32:E110">
-    <cfRule type="cellIs" dxfId="251" priority="328" operator="equal">
+    <cfRule type="cellIs" dxfId="230" priority="328" operator="equal">
       <formula>"Alacsony"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E23:E30 E2:E18 E32:E110">
-    <cfRule type="cellIs" dxfId="250" priority="329" operator="equal">
+    <cfRule type="cellIs" dxfId="229" priority="329" operator="equal">
       <formula>"Normál"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E23:E30 E2:E18 E32:E110">
-    <cfRule type="cellIs" dxfId="249" priority="330" operator="equal">
+    <cfRule type="cellIs" dxfId="228" priority="330" operator="equal">
       <formula>"Magas"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K71:K85 K27:K30 K8 K32:K62">
-    <cfRule type="cellIs" dxfId="248" priority="331" operator="equal">
+    <cfRule type="cellIs" dxfId="227" priority="331" operator="equal">
       <formula>"Siker"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K71:K85 K27:K30 K8 K32:K62">
-    <cfRule type="cellIs" dxfId="247" priority="332" operator="equal">
+    <cfRule type="cellIs" dxfId="226" priority="332" operator="equal">
       <formula>"Nem futtatható"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K71:K85 K27:K30 K8 K32:K62">
-    <cfRule type="cellIs" dxfId="246" priority="333" operator="equal">
+    <cfRule type="cellIs" dxfId="225" priority="333" operator="equal">
       <formula>"Hiba"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E12">
-    <cfRule type="cellIs" dxfId="245" priority="319" operator="equal">
+    <cfRule type="cellIs" dxfId="224" priority="319" operator="equal">
       <formula>"Alacsony"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E12">
-    <cfRule type="cellIs" dxfId="244" priority="320" operator="equal">
+    <cfRule type="cellIs" dxfId="223" priority="320" operator="equal">
       <formula>"Normál"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E12">
-    <cfRule type="cellIs" dxfId="243" priority="321" operator="equal">
+    <cfRule type="cellIs" dxfId="222" priority="321" operator="equal">
       <formula>"Magas"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E13">
-    <cfRule type="cellIs" dxfId="239" priority="310" operator="equal">
+    <cfRule type="cellIs" dxfId="221" priority="310" operator="equal">
       <formula>"Alacsony"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E13">
-    <cfRule type="cellIs" dxfId="238" priority="311" operator="equal">
+    <cfRule type="cellIs" dxfId="220" priority="311" operator="equal">
       <formula>"Normál"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E13">
-    <cfRule type="cellIs" dxfId="237" priority="312" operator="equal">
+    <cfRule type="cellIs" dxfId="219" priority="312" operator="equal">
       <formula>"Magas"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E25">
-    <cfRule type="cellIs" dxfId="236" priority="301" operator="equal">
+    <cfRule type="cellIs" dxfId="218" priority="301" operator="equal">
       <formula>"Alacsony"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E25">
-    <cfRule type="cellIs" dxfId="235" priority="302" operator="equal">
+    <cfRule type="cellIs" dxfId="217" priority="302" operator="equal">
       <formula>"Normál"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E25">
-    <cfRule type="cellIs" dxfId="234" priority="303" operator="equal">
+    <cfRule type="cellIs" dxfId="216" priority="303" operator="equal">
       <formula>"Magas"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K25">
-    <cfRule type="cellIs" dxfId="233" priority="304" operator="equal">
+    <cfRule type="cellIs" dxfId="215" priority="304" operator="equal">
       <formula>"Siker"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K25">
-    <cfRule type="cellIs" dxfId="232" priority="305" operator="equal">
+    <cfRule type="cellIs" dxfId="214" priority="305" operator="equal">
       <formula>"Nem futtatható"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K25">
-    <cfRule type="cellIs" dxfId="231" priority="306" operator="equal">
+    <cfRule type="cellIs" dxfId="213" priority="306" operator="equal">
       <formula>"Hiba"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E26">
-    <cfRule type="cellIs" dxfId="230" priority="295" operator="equal">
+    <cfRule type="cellIs" dxfId="212" priority="295" operator="equal">
       <formula>"Alacsony"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E26">
-    <cfRule type="cellIs" dxfId="229" priority="296" operator="equal">
+    <cfRule type="cellIs" dxfId="211" priority="296" operator="equal">
       <formula>"Normál"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E26">
-    <cfRule type="cellIs" dxfId="228" priority="297" operator="equal">
+    <cfRule type="cellIs" dxfId="210" priority="297" operator="equal">
       <formula>"Magas"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K26">
-    <cfRule type="cellIs" dxfId="227" priority="298" operator="equal">
+    <cfRule type="cellIs" dxfId="209" priority="298" operator="equal">
       <formula>"Siker"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K26">
-    <cfRule type="cellIs" dxfId="226" priority="299" operator="equal">
+    <cfRule type="cellIs" dxfId="208" priority="299" operator="equal">
       <formula>"Nem futtatható"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K26">
-    <cfRule type="cellIs" dxfId="225" priority="300" operator="equal">
+    <cfRule type="cellIs" dxfId="207" priority="300" operator="equal">
       <formula>"Hiba"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E27">
-    <cfRule type="cellIs" dxfId="224" priority="292" operator="equal">
+    <cfRule type="cellIs" dxfId="206" priority="292" operator="equal">
       <formula>"Alacsony"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E27">
-    <cfRule type="cellIs" dxfId="223" priority="293" operator="equal">
+    <cfRule type="cellIs" dxfId="205" priority="293" operator="equal">
       <formula>"Normál"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E27">
-    <cfRule type="cellIs" dxfId="222" priority="294" operator="equal">
+    <cfRule type="cellIs" dxfId="204" priority="294" operator="equal">
       <formula>"Magas"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E63:E66">
-    <cfRule type="cellIs" dxfId="221" priority="280" operator="equal">
+    <cfRule type="cellIs" dxfId="203" priority="280" operator="equal">
       <formula>"Alacsony"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E63:E66">
-    <cfRule type="cellIs" dxfId="220" priority="281" operator="equal">
+    <cfRule type="cellIs" dxfId="202" priority="281" operator="equal">
       <formula>"Normál"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E63:E66">
-    <cfRule type="cellIs" dxfId="219" priority="282" operator="equal">
+    <cfRule type="cellIs" dxfId="201" priority="282" operator="equal">
       <formula>"Magas"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K63:K66">
-    <cfRule type="cellIs" dxfId="218" priority="283" operator="equal">
+    <cfRule type="cellIs" dxfId="200" priority="283" operator="equal">
       <formula>"Siker"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K63:K66">
-    <cfRule type="cellIs" dxfId="217" priority="284" operator="equal">
+    <cfRule type="cellIs" dxfId="199" priority="284" operator="equal">
       <formula>"Nem futtatható"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K63:K66">
-    <cfRule type="cellIs" dxfId="216" priority="285" operator="equal">
+    <cfRule type="cellIs" dxfId="198" priority="285" operator="equal">
       <formula>"Hiba"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E67">
-    <cfRule type="cellIs" dxfId="215" priority="274" operator="equal">
+    <cfRule type="cellIs" dxfId="197" priority="274" operator="equal">
       <formula>"Alacsony"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E67">
-    <cfRule type="cellIs" dxfId="214" priority="275" operator="equal">
+    <cfRule type="cellIs" dxfId="196" priority="275" operator="equal">
       <formula>"Normál"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E67">
-    <cfRule type="cellIs" dxfId="213" priority="276" operator="equal">
+    <cfRule type="cellIs" dxfId="195" priority="276" operator="equal">
       <formula>"Magas"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K67:K68">
-    <cfRule type="cellIs" dxfId="212" priority="277" operator="equal">
+    <cfRule type="cellIs" dxfId="194" priority="277" operator="equal">
       <formula>"Siker"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K67:K68">
-    <cfRule type="cellIs" dxfId="211" priority="278" operator="equal">
+    <cfRule type="cellIs" dxfId="193" priority="278" operator="equal">
       <formula>"Nem futtatható"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K67:K68">
-    <cfRule type="cellIs" dxfId="210" priority="279" operator="equal">
+    <cfRule type="cellIs" dxfId="192" priority="279" operator="equal">
       <formula>"Hiba"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E68">
-    <cfRule type="cellIs" dxfId="209" priority="265" operator="equal">
+    <cfRule type="cellIs" dxfId="191" priority="265" operator="equal">
       <formula>"Alacsony"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E68">
-    <cfRule type="cellIs" dxfId="208" priority="266" operator="equal">
+    <cfRule type="cellIs" dxfId="190" priority="266" operator="equal">
       <formula>"Normál"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E68">
-    <cfRule type="cellIs" dxfId="207" priority="267" operator="equal">
+    <cfRule type="cellIs" dxfId="189" priority="267" operator="equal">
       <formula>"Magas"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E69">
-    <cfRule type="cellIs" dxfId="206" priority="259" operator="equal">
+    <cfRule type="cellIs" dxfId="188" priority="259" operator="equal">
       <formula>"Alacsony"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E69">
-    <cfRule type="cellIs" dxfId="205" priority="260" operator="equal">
+    <cfRule type="cellIs" dxfId="187" priority="260" operator="equal">
       <formula>"Normál"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E69">
-    <cfRule type="cellIs" dxfId="204" priority="261" operator="equal">
+    <cfRule type="cellIs" dxfId="186" priority="261" operator="equal">
       <formula>"Magas"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K69">
-    <cfRule type="cellIs" dxfId="203" priority="262" operator="equal">
+    <cfRule type="cellIs" dxfId="185" priority="262" operator="equal">
       <formula>"Siker"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K69">
-    <cfRule type="cellIs" dxfId="202" priority="263" operator="equal">
+    <cfRule type="cellIs" dxfId="184" priority="263" operator="equal">
       <formula>"Nem futtatható"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K69">
-    <cfRule type="cellIs" dxfId="201" priority="264" operator="equal">
+    <cfRule type="cellIs" dxfId="183" priority="264" operator="equal">
       <formula>"Hiba"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E70">
-    <cfRule type="cellIs" dxfId="200" priority="235" operator="equal">
+    <cfRule type="cellIs" dxfId="182" priority="235" operator="equal">
       <formula>"Alacsony"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E70">
-    <cfRule type="cellIs" dxfId="199" priority="236" operator="equal">
+    <cfRule type="cellIs" dxfId="181" priority="236" operator="equal">
       <formula>"Normál"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E70">
-    <cfRule type="cellIs" dxfId="198" priority="237" operator="equal">
+    <cfRule type="cellIs" dxfId="180" priority="237" operator="equal">
       <formula>"Magas"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K70">
-    <cfRule type="cellIs" dxfId="197" priority="238" operator="equal">
+    <cfRule type="cellIs" dxfId="179" priority="238" operator="equal">
       <formula>"Siker"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K70">
-    <cfRule type="cellIs" dxfId="196" priority="239" operator="equal">
+    <cfRule type="cellIs" dxfId="178" priority="239" operator="equal">
       <formula>"Nem futtatható"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K70">
-    <cfRule type="cellIs" dxfId="195" priority="240" operator="equal">
+    <cfRule type="cellIs" dxfId="177" priority="240" operator="equal">
       <formula>"Hiba"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E86:E90 E94:E105">
-    <cfRule type="cellIs" dxfId="194" priority="220" operator="equal">
+    <cfRule type="cellIs" dxfId="176" priority="220" operator="equal">
       <formula>"Alacsony"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E86:E90 E94:E105">
-    <cfRule type="cellIs" dxfId="193" priority="221" operator="equal">
+    <cfRule type="cellIs" dxfId="175" priority="221" operator="equal">
       <formula>"Normál"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E86:E90 E94:E105">
-    <cfRule type="cellIs" dxfId="192" priority="222" operator="equal">
+    <cfRule type="cellIs" dxfId="174" priority="222" operator="equal">
       <formula>"Magas"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K86:K91 K93:K105 K108:K111">
-    <cfRule type="cellIs" dxfId="191" priority="223" operator="equal">
+    <cfRule type="cellIs" dxfId="173" priority="223" operator="equal">
       <formula>"Siker"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K86:K91 K93:K105 K108:K111">
-    <cfRule type="cellIs" dxfId="190" priority="224" operator="equal">
+    <cfRule type="cellIs" dxfId="172" priority="224" operator="equal">
       <formula>"Nem futtatható"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K86:K91 K93:K105 K108:K111">
-    <cfRule type="cellIs" dxfId="189" priority="225" operator="equal">
+    <cfRule type="cellIs" dxfId="171" priority="225" operator="equal">
       <formula>"Hiba"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E91">
-    <cfRule type="cellIs" dxfId="188" priority="217" operator="equal">
+    <cfRule type="cellIs" dxfId="170" priority="217" operator="equal">
       <formula>"Alacsony"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E91">
-    <cfRule type="cellIs" dxfId="187" priority="218" operator="equal">
+    <cfRule type="cellIs" dxfId="169" priority="218" operator="equal">
       <formula>"Normál"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E91">
-    <cfRule type="cellIs" dxfId="186" priority="219" operator="equal">
+    <cfRule type="cellIs" dxfId="168" priority="219" operator="equal">
       <formula>"Magas"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K92">
-    <cfRule type="cellIs" dxfId="185" priority="214" operator="equal">
+    <cfRule type="cellIs" dxfId="167" priority="214" operator="equal">
       <formula>"Siker"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K92">
-    <cfRule type="cellIs" dxfId="184" priority="215" operator="equal">
+    <cfRule type="cellIs" dxfId="166" priority="215" operator="equal">
       <formula>"Nem futtatható"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K92">
-    <cfRule type="cellIs" dxfId="183" priority="216" operator="equal">
+    <cfRule type="cellIs" dxfId="165" priority="216" operator="equal">
       <formula>"Hiba"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E92">
-    <cfRule type="cellIs" dxfId="182" priority="211" operator="equal">
+    <cfRule type="cellIs" dxfId="164" priority="211" operator="equal">
       <formula>"Alacsony"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E92">
-    <cfRule type="cellIs" dxfId="181" priority="212" operator="equal">
+    <cfRule type="cellIs" dxfId="163" priority="212" operator="equal">
       <formula>"Normál"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E92">
-    <cfRule type="cellIs" dxfId="180" priority="213" operator="equal">
+    <cfRule type="cellIs" dxfId="162" priority="213" operator="equal">
       <formula>"Magas"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E93">
-    <cfRule type="cellIs" dxfId="179" priority="208" operator="equal">
+    <cfRule type="cellIs" dxfId="161" priority="208" operator="equal">
       <formula>"Alacsony"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E93">
-    <cfRule type="cellIs" dxfId="178" priority="209" operator="equal">
+    <cfRule type="cellIs" dxfId="160" priority="209" operator="equal">
       <formula>"Normál"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E93">
-    <cfRule type="cellIs" dxfId="177" priority="210" operator="equal">
+    <cfRule type="cellIs" dxfId="159" priority="210" operator="equal">
       <formula>"Magas"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E106">
-    <cfRule type="cellIs" dxfId="176" priority="202" operator="equal">
+    <cfRule type="cellIs" dxfId="158" priority="202" operator="equal">
       <formula>"Alacsony"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E106">
-    <cfRule type="cellIs" dxfId="175" priority="203" operator="equal">
+    <cfRule type="cellIs" dxfId="157" priority="203" operator="equal">
       <formula>"Normál"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E106">
-    <cfRule type="cellIs" dxfId="174" priority="204" operator="equal">
+    <cfRule type="cellIs" dxfId="156" priority="204" operator="equal">
       <formula>"Magas"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K106">
-    <cfRule type="cellIs" dxfId="173" priority="205" operator="equal">
+    <cfRule type="cellIs" dxfId="155" priority="205" operator="equal">
       <formula>"Siker"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K106">
-    <cfRule type="cellIs" dxfId="172" priority="206" operator="equal">
+    <cfRule type="cellIs" dxfId="154" priority="206" operator="equal">
       <formula>"Nem futtatható"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K106">
-    <cfRule type="cellIs" dxfId="171" priority="207" operator="equal">
+    <cfRule type="cellIs" dxfId="153" priority="207" operator="equal">
       <formula>"Hiba"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E107">
-    <cfRule type="cellIs" dxfId="170" priority="196" operator="equal">
+    <cfRule type="cellIs" dxfId="152" priority="196" operator="equal">
       <formula>"Alacsony"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E107">
-    <cfRule type="cellIs" dxfId="169" priority="197" operator="equal">
+    <cfRule type="cellIs" dxfId="151" priority="197" operator="equal">
       <formula>"Normál"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E107">
-    <cfRule type="cellIs" dxfId="168" priority="198" operator="equal">
+    <cfRule type="cellIs" dxfId="150" priority="198" operator="equal">
       <formula>"Magas"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K107">
-    <cfRule type="cellIs" dxfId="167" priority="199" operator="equal">
+    <cfRule type="cellIs" dxfId="149" priority="199" operator="equal">
       <formula>"Siker"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K107">
-    <cfRule type="cellIs" dxfId="166" priority="200" operator="equal">
+    <cfRule type="cellIs" dxfId="148" priority="200" operator="equal">
       <formula>"Nem futtatható"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K107">
-    <cfRule type="cellIs" dxfId="165" priority="201" operator="equal">
+    <cfRule type="cellIs" dxfId="147" priority="201" operator="equal">
       <formula>"Hiba"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E108">
-    <cfRule type="cellIs" dxfId="164" priority="193" operator="equal">
+    <cfRule type="cellIs" dxfId="146" priority="193" operator="equal">
       <formula>"Alacsony"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E108">
-    <cfRule type="cellIs" dxfId="163" priority="194" operator="equal">
+    <cfRule type="cellIs" dxfId="145" priority="194" operator="equal">
       <formula>"Normál"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E108">
-    <cfRule type="cellIs" dxfId="162" priority="195" operator="equal">
+    <cfRule type="cellIs" dxfId="144" priority="195" operator="equal">
       <formula>"Magas"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E109:E110">
-    <cfRule type="cellIs" dxfId="161" priority="190" operator="equal">
+    <cfRule type="cellIs" dxfId="143" priority="190" operator="equal">
       <formula>"Alacsony"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E109:E110">
-    <cfRule type="cellIs" dxfId="160" priority="191" operator="equal">
+    <cfRule type="cellIs" dxfId="142" priority="191" operator="equal">
       <formula>"Normál"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E109:E110">
-    <cfRule type="cellIs" dxfId="159" priority="192" operator="equal">
+    <cfRule type="cellIs" dxfId="141" priority="192" operator="equal">
       <formula>"Magas"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2">
-    <cfRule type="cellIs" dxfId="158" priority="172" operator="equal">
+    <cfRule type="cellIs" dxfId="140" priority="172" operator="equal">
       <formula>"Alacsony"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2">
-    <cfRule type="cellIs" dxfId="157" priority="173" operator="equal">
+    <cfRule type="cellIs" dxfId="139" priority="173" operator="equal">
       <formula>"Normál"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2">
-    <cfRule type="cellIs" dxfId="156" priority="174" operator="equal">
+    <cfRule type="cellIs" dxfId="138" priority="174" operator="equal">
       <formula>"Magas"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K2">
-    <cfRule type="cellIs" dxfId="155" priority="175" operator="equal">
+    <cfRule type="cellIs" dxfId="137" priority="175" operator="equal">
       <formula>"Siker"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K2">
-    <cfRule type="cellIs" dxfId="154" priority="176" operator="equal">
+    <cfRule type="cellIs" dxfId="136" priority="176" operator="equal">
       <formula>"Nem futtatható"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K2">
-    <cfRule type="cellIs" dxfId="153" priority="177" operator="equal">
+    <cfRule type="cellIs" dxfId="135" priority="177" operator="equal">
       <formula>"Hiba"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E9:E11">
-    <cfRule type="cellIs" dxfId="152" priority="166" operator="equal">
+    <cfRule type="cellIs" dxfId="134" priority="166" operator="equal">
       <formula>"Alacsony"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E9:E11">
-    <cfRule type="cellIs" dxfId="151" priority="167" operator="equal">
+    <cfRule type="cellIs" dxfId="133" priority="167" operator="equal">
       <formula>"Normál"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E9:E11">
-    <cfRule type="cellIs" dxfId="150" priority="168" operator="equal">
+    <cfRule type="cellIs" dxfId="132" priority="168" operator="equal">
       <formula>"Magas"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K11">
-    <cfRule type="cellIs" dxfId="149" priority="169" operator="equal">
+    <cfRule type="cellIs" dxfId="131" priority="169" operator="equal">
       <formula>"Siker"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K11">
-    <cfRule type="cellIs" dxfId="148" priority="170" operator="equal">
+    <cfRule type="cellIs" dxfId="130" priority="170" operator="equal">
       <formula>"Nem futtatható"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K11">
-    <cfRule type="cellIs" dxfId="147" priority="171" operator="equal">
+    <cfRule type="cellIs" dxfId="129" priority="171" operator="equal">
       <formula>"Hiba"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E10:E11">
-    <cfRule type="cellIs" dxfId="146" priority="160" operator="equal">
+    <cfRule type="cellIs" dxfId="128" priority="160" operator="equal">
       <formula>"Alacsony"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E10:E11">
-    <cfRule type="cellIs" dxfId="145" priority="161" operator="equal">
+    <cfRule type="cellIs" dxfId="127" priority="161" operator="equal">
       <formula>"Normál"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E10:E11">
-    <cfRule type="cellIs" dxfId="144" priority="162" operator="equal">
+    <cfRule type="cellIs" dxfId="126" priority="162" operator="equal">
       <formula>"Magas"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K11">
-    <cfRule type="cellIs" dxfId="143" priority="163" operator="equal">
+    <cfRule type="cellIs" dxfId="125" priority="163" operator="equal">
       <formula>"Siker"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K11">
-    <cfRule type="cellIs" dxfId="142" priority="164" operator="equal">
+    <cfRule type="cellIs" dxfId="124" priority="164" operator="equal">
       <formula>"Nem futtatható"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K11">
-    <cfRule type="cellIs" dxfId="141" priority="165" operator="equal">
+    <cfRule type="cellIs" dxfId="123" priority="165" operator="equal">
       <formula>"Hiba"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E24">
-    <cfRule type="cellIs" dxfId="140" priority="148" operator="equal">
+    <cfRule type="cellIs" dxfId="122" priority="148" operator="equal">
       <formula>"Alacsony"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E24">
-    <cfRule type="cellIs" dxfId="139" priority="149" operator="equal">
+    <cfRule type="cellIs" dxfId="121" priority="149" operator="equal">
       <formula>"Normál"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E24">
-    <cfRule type="cellIs" dxfId="138" priority="150" operator="equal">
+    <cfRule type="cellIs" dxfId="120" priority="150" operator="equal">
       <formula>"Magas"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E4">
-    <cfRule type="cellIs" dxfId="134" priority="145" operator="equal">
+    <cfRule type="cellIs" dxfId="119" priority="145" operator="equal">
       <formula>"Alacsony"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E4">
-    <cfRule type="cellIs" dxfId="133" priority="146" operator="equal">
+    <cfRule type="cellIs" dxfId="118" priority="146" operator="equal">
       <formula>"Normál"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E4">
-    <cfRule type="cellIs" dxfId="132" priority="147" operator="equal">
+    <cfRule type="cellIs" dxfId="117" priority="147" operator="equal">
       <formula>"Magas"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E5">
-    <cfRule type="cellIs" dxfId="131" priority="142" operator="equal">
+    <cfRule type="cellIs" dxfId="116" priority="142" operator="equal">
       <formula>"Alacsony"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E5">
-    <cfRule type="cellIs" dxfId="130" priority="143" operator="equal">
+    <cfRule type="cellIs" dxfId="115" priority="143" operator="equal">
       <formula>"Normál"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E5">
-    <cfRule type="cellIs" dxfId="129" priority="144" operator="equal">
+    <cfRule type="cellIs" dxfId="114" priority="144" operator="equal">
       <formula>"Magas"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E6">
-    <cfRule type="cellIs" dxfId="128" priority="139" operator="equal">
+    <cfRule type="cellIs" dxfId="113" priority="139" operator="equal">
       <formula>"Alacsony"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E6">
-    <cfRule type="cellIs" dxfId="127" priority="140" operator="equal">
+    <cfRule type="cellIs" dxfId="112" priority="140" operator="equal">
       <formula>"Normál"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E6">
-    <cfRule type="cellIs" dxfId="126" priority="141" operator="equal">
+    <cfRule type="cellIs" dxfId="111" priority="141" operator="equal">
       <formula>"Magas"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E7">
-    <cfRule type="cellIs" dxfId="125" priority="136" operator="equal">
+    <cfRule type="cellIs" dxfId="110" priority="136" operator="equal">
       <formula>"Alacsony"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E7">
-    <cfRule type="cellIs" dxfId="124" priority="137" operator="equal">
+    <cfRule type="cellIs" dxfId="109" priority="137" operator="equal">
       <formula>"Normál"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E7">
-    <cfRule type="cellIs" dxfId="123" priority="138" operator="equal">
+    <cfRule type="cellIs" dxfId="108" priority="138" operator="equal">
       <formula>"Magas"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E8">
-    <cfRule type="cellIs" dxfId="122" priority="133" operator="equal">
+    <cfRule type="cellIs" dxfId="107" priority="133" operator="equal">
       <formula>"Alacsony"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E8">
-    <cfRule type="cellIs" dxfId="121" priority="134" operator="equal">
+    <cfRule type="cellIs" dxfId="106" priority="134" operator="equal">
       <formula>"Normál"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E8">
-    <cfRule type="cellIs" dxfId="120" priority="135" operator="equal">
+    <cfRule type="cellIs" dxfId="105" priority="135" operator="equal">
       <formula>"Magas"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E12">
-    <cfRule type="cellIs" dxfId="119" priority="130" operator="equal">
+    <cfRule type="cellIs" dxfId="104" priority="130" operator="equal">
       <formula>"Alacsony"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E12">
-    <cfRule type="cellIs" dxfId="118" priority="131" operator="equal">
+    <cfRule type="cellIs" dxfId="103" priority="131" operator="equal">
       <formula>"Normál"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E12">
-    <cfRule type="cellIs" dxfId="117" priority="132" operator="equal">
+    <cfRule type="cellIs" dxfId="102" priority="132" operator="equal">
       <formula>"Magas"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E13">
-    <cfRule type="cellIs" dxfId="116" priority="127" operator="equal">
+    <cfRule type="cellIs" dxfId="101" priority="127" operator="equal">
       <formula>"Alacsony"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E13">
-    <cfRule type="cellIs" dxfId="115" priority="128" operator="equal">
+    <cfRule type="cellIs" dxfId="100" priority="128" operator="equal">
       <formula>"Normál"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E13">
-    <cfRule type="cellIs" dxfId="114" priority="129" operator="equal">
+    <cfRule type="cellIs" dxfId="99" priority="129" operator="equal">
       <formula>"Magas"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E14">
-    <cfRule type="cellIs" dxfId="113" priority="124" operator="equal">
+    <cfRule type="cellIs" dxfId="98" priority="124" operator="equal">
       <formula>"Alacsony"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E14">
-    <cfRule type="cellIs" dxfId="112" priority="125" operator="equal">
+    <cfRule type="cellIs" dxfId="97" priority="125" operator="equal">
       <formula>"Normál"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E14">
-    <cfRule type="cellIs" dxfId="111" priority="126" operator="equal">
+    <cfRule type="cellIs" dxfId="96" priority="126" operator="equal">
       <formula>"Magas"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E15">
-    <cfRule type="cellIs" dxfId="110" priority="121" operator="equal">
+    <cfRule type="cellIs" dxfId="95" priority="121" operator="equal">
       <formula>"Alacsony"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E15">
-    <cfRule type="cellIs" dxfId="109" priority="122" operator="equal">
+    <cfRule type="cellIs" dxfId="94" priority="122" operator="equal">
       <formula>"Normál"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E15">
-    <cfRule type="cellIs" dxfId="108" priority="123" operator="equal">
+    <cfRule type="cellIs" dxfId="93" priority="123" operator="equal">
       <formula>"Magas"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E16">
-    <cfRule type="cellIs" dxfId="107" priority="118" operator="equal">
+    <cfRule type="cellIs" dxfId="92" priority="118" operator="equal">
       <formula>"Alacsony"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E16">
-    <cfRule type="cellIs" dxfId="106" priority="119" operator="equal">
+    <cfRule type="cellIs" dxfId="91" priority="119" operator="equal">
       <formula>"Normál"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E16">
-    <cfRule type="cellIs" dxfId="105" priority="120" operator="equal">
+    <cfRule type="cellIs" dxfId="90" priority="120" operator="equal">
       <formula>"Magas"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E21">
-    <cfRule type="cellIs" dxfId="104" priority="112" operator="equal">
+    <cfRule type="cellIs" dxfId="89" priority="112" operator="equal">
       <formula>"Alacsony"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E21">
-    <cfRule type="cellIs" dxfId="103" priority="113" operator="equal">
+    <cfRule type="cellIs" dxfId="88" priority="113" operator="equal">
       <formula>"Normál"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E21">
-    <cfRule type="cellIs" dxfId="102" priority="114" operator="equal">
+    <cfRule type="cellIs" dxfId="87" priority="114" operator="equal">
       <formula>"Magas"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E20">
-    <cfRule type="cellIs" dxfId="98" priority="106" operator="equal">
+    <cfRule type="cellIs" dxfId="86" priority="106" operator="equal">
       <formula>"Alacsony"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E20">
-    <cfRule type="cellIs" dxfId="97" priority="107" operator="equal">
+    <cfRule type="cellIs" dxfId="85" priority="107" operator="equal">
       <formula>"Normál"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E20">
-    <cfRule type="cellIs" dxfId="96" priority="108" operator="equal">
+    <cfRule type="cellIs" dxfId="84" priority="108" operator="equal">
       <formula>"Magas"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E19">
-    <cfRule type="cellIs" dxfId="92" priority="100" operator="equal">
+    <cfRule type="cellIs" dxfId="83" priority="100" operator="equal">
       <formula>"Alacsony"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E19">
-    <cfRule type="cellIs" dxfId="91" priority="101" operator="equal">
+    <cfRule type="cellIs" dxfId="82" priority="101" operator="equal">
       <formula>"Normál"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E19">
-    <cfRule type="cellIs" dxfId="90" priority="102" operator="equal">
+    <cfRule type="cellIs" dxfId="81" priority="102" operator="equal">
       <formula>"Magas"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E22">
-    <cfRule type="cellIs" dxfId="86" priority="94" operator="equal">
+    <cfRule type="cellIs" dxfId="80" priority="94" operator="equal">
       <formula>"Alacsony"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E22">
-    <cfRule type="cellIs" dxfId="85" priority="95" operator="equal">
+    <cfRule type="cellIs" dxfId="79" priority="95" operator="equal">
       <formula>"Normál"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E22">
-    <cfRule type="cellIs" dxfId="84" priority="96" operator="equal">
+    <cfRule type="cellIs" dxfId="78" priority="96" operator="equal">
       <formula>"Magas"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E31">
-    <cfRule type="cellIs" dxfId="80" priority="64" operator="equal">
+    <cfRule type="cellIs" dxfId="77" priority="64" operator="equal">
       <formula>"Alacsony"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E31">
-    <cfRule type="cellIs" dxfId="79" priority="65" operator="equal">
+    <cfRule type="cellIs" dxfId="76" priority="65" operator="equal">
       <formula>"Normál"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E31">
-    <cfRule type="cellIs" dxfId="78" priority="66" operator="equal">
+    <cfRule type="cellIs" dxfId="75" priority="66" operator="equal">
       <formula>"Magas"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K31">
-    <cfRule type="cellIs" dxfId="77" priority="67" operator="equal">
+    <cfRule type="cellIs" dxfId="74" priority="67" operator="equal">
       <formula>"Siker"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K31">
-    <cfRule type="cellIs" dxfId="76" priority="68" operator="equal">
+    <cfRule type="cellIs" dxfId="73" priority="68" operator="equal">
       <formula>"Nem futtatható"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K31">
-    <cfRule type="cellIs" dxfId="75" priority="69" operator="equal">
+    <cfRule type="cellIs" dxfId="72" priority="69" operator="equal">
       <formula>"Hiba"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K3">
-    <cfRule type="cellIs" dxfId="62" priority="61" operator="equal">
+    <cfRule type="cellIs" dxfId="71" priority="61" operator="equal">
       <formula>"Siker"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K3">
-    <cfRule type="cellIs" dxfId="61" priority="62" operator="equal">
+    <cfRule type="cellIs" dxfId="70" priority="62" operator="equal">
       <formula>"Nem futtatható"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K3">
-    <cfRule type="cellIs" dxfId="60" priority="63" operator="equal">
+    <cfRule type="cellIs" dxfId="69" priority="63" operator="equal">
       <formula>"Hiba"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K4">
-    <cfRule type="cellIs" dxfId="59" priority="58" operator="equal">
+    <cfRule type="cellIs" dxfId="68" priority="58" operator="equal">
       <formula>"Siker"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K4">
-    <cfRule type="cellIs" dxfId="58" priority="59" operator="equal">
+    <cfRule type="cellIs" dxfId="67" priority="59" operator="equal">
       <formula>"Nem futtatható"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K4">
-    <cfRule type="cellIs" dxfId="57" priority="60" operator="equal">
+    <cfRule type="cellIs" dxfId="66" priority="60" operator="equal">
       <formula>"Hiba"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K5">
-    <cfRule type="cellIs" dxfId="56" priority="55" operator="equal">
+    <cfRule type="cellIs" dxfId="65" priority="55" operator="equal">
       <formula>"Siker"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K5">
-    <cfRule type="cellIs" dxfId="55" priority="56" operator="equal">
+    <cfRule type="cellIs" dxfId="64" priority="56" operator="equal">
       <formula>"Nem futtatható"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K5">
-    <cfRule type="cellIs" dxfId="54" priority="57" operator="equal">
+    <cfRule type="cellIs" dxfId="63" priority="57" operator="equal">
       <formula>"Hiba"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K6">
-    <cfRule type="cellIs" dxfId="53" priority="52" operator="equal">
+    <cfRule type="cellIs" dxfId="62" priority="52" operator="equal">
       <formula>"Siker"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K6">
-    <cfRule type="cellIs" dxfId="52" priority="53" operator="equal">
+    <cfRule type="cellIs" dxfId="61" priority="53" operator="equal">
       <formula>"Nem futtatható"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K6">
-    <cfRule type="cellIs" dxfId="51" priority="54" operator="equal">
+    <cfRule type="cellIs" dxfId="60" priority="54" operator="equal">
       <formula>"Hiba"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K7">
-    <cfRule type="cellIs" dxfId="50" priority="49" operator="equal">
+    <cfRule type="cellIs" dxfId="59" priority="49" operator="equal">
       <formula>"Siker"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K7">
-    <cfRule type="cellIs" dxfId="49" priority="50" operator="equal">
+    <cfRule type="cellIs" dxfId="58" priority="50" operator="equal">
       <formula>"Nem futtatható"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K7">
-    <cfRule type="cellIs" dxfId="48" priority="51" operator="equal">
+    <cfRule type="cellIs" dxfId="57" priority="51" operator="equal">
       <formula>"Hiba"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K9">
-    <cfRule type="cellIs" dxfId="47" priority="46" operator="equal">
+    <cfRule type="cellIs" dxfId="56" priority="46" operator="equal">
       <formula>"Siker"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K9">
-    <cfRule type="cellIs" dxfId="46" priority="47" operator="equal">
+    <cfRule type="cellIs" dxfId="55" priority="47" operator="equal">
       <formula>"Nem futtatható"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K9">
-    <cfRule type="cellIs" dxfId="45" priority="48" operator="equal">
+    <cfRule type="cellIs" dxfId="54" priority="48" operator="equal">
       <formula>"Hiba"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K10">
-    <cfRule type="cellIs" dxfId="44" priority="43" operator="equal">
+    <cfRule type="cellIs" dxfId="53" priority="43" operator="equal">
       <formula>"Siker"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K10">
-    <cfRule type="cellIs" dxfId="43" priority="44" operator="equal">
+    <cfRule type="cellIs" dxfId="52" priority="44" operator="equal">
       <formula>"Nem futtatható"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K10">
-    <cfRule type="cellIs" dxfId="42" priority="45" operator="equal">
+    <cfRule type="cellIs" dxfId="51" priority="45" operator="equal">
       <formula>"Hiba"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K12">
-    <cfRule type="cellIs" dxfId="41" priority="40" operator="equal">
+    <cfRule type="cellIs" dxfId="50" priority="40" operator="equal">
       <formula>"Siker"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K12">
-    <cfRule type="cellIs" dxfId="40" priority="41" operator="equal">
+    <cfRule type="cellIs" dxfId="49" priority="41" operator="equal">
       <formula>"Nem futtatható"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K12">
-    <cfRule type="cellIs" dxfId="39" priority="42" operator="equal">
+    <cfRule type="cellIs" dxfId="48" priority="42" operator="equal">
       <formula>"Hiba"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K13">
-    <cfRule type="cellIs" dxfId="38" priority="37" operator="equal">
+    <cfRule type="cellIs" dxfId="47" priority="37" operator="equal">
       <formula>"Siker"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K13">
-    <cfRule type="cellIs" dxfId="37" priority="38" operator="equal">
+    <cfRule type="cellIs" dxfId="46" priority="38" operator="equal">
       <formula>"Nem futtatható"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K13">
-    <cfRule type="cellIs" dxfId="36" priority="39" operator="equal">
+    <cfRule type="cellIs" dxfId="45" priority="39" operator="equal">
       <formula>"Hiba"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K14">
-    <cfRule type="cellIs" dxfId="35" priority="34" operator="equal">
+    <cfRule type="cellIs" dxfId="44" priority="34" operator="equal">
       <formula>"Siker"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K14">
-    <cfRule type="cellIs" dxfId="34" priority="35" operator="equal">
+    <cfRule type="cellIs" dxfId="43" priority="35" operator="equal">
       <formula>"Nem futtatható"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K14">
-    <cfRule type="cellIs" dxfId="33" priority="36" operator="equal">
+    <cfRule type="cellIs" dxfId="42" priority="36" operator="equal">
       <formula>"Hiba"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K15">
-    <cfRule type="cellIs" dxfId="32" priority="31" operator="equal">
+    <cfRule type="cellIs" dxfId="41" priority="31" operator="equal">
       <formula>"Siker"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K15">
-    <cfRule type="cellIs" dxfId="31" priority="32" operator="equal">
+    <cfRule type="cellIs" dxfId="40" priority="32" operator="equal">
       <formula>"Nem futtatható"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K15">
-    <cfRule type="cellIs" dxfId="30" priority="33" operator="equal">
+    <cfRule type="cellIs" dxfId="39" priority="33" operator="equal">
       <formula>"Hiba"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K16">
-    <cfRule type="cellIs" dxfId="29" priority="28" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="28" operator="equal">
       <formula>"Siker"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K16">
-    <cfRule type="cellIs" dxfId="28" priority="29" operator="equal">
+    <cfRule type="cellIs" dxfId="37" priority="29" operator="equal">
       <formula>"Nem futtatható"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K16">
-    <cfRule type="cellIs" dxfId="27" priority="30" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="30" operator="equal">
       <formula>"Hiba"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K17">
-    <cfRule type="cellIs" dxfId="23" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="22" operator="equal">
       <formula>"Siker"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K17">
-    <cfRule type="cellIs" dxfId="22" priority="23" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="23" operator="equal">
       <formula>"Nem futtatható"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K17">
-    <cfRule type="cellIs" dxfId="21" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="24" operator="equal">
       <formula>"Hiba"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K18">
-    <cfRule type="cellIs" dxfId="20" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="19" operator="equal">
       <formula>"Siker"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K18">
-    <cfRule type="cellIs" dxfId="19" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="20" operator="equal">
       <formula>"Nem futtatható"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K18">
-    <cfRule type="cellIs" dxfId="18" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="21" operator="equal">
       <formula>"Hiba"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K19">
-    <cfRule type="cellIs" dxfId="17" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="16" operator="equal">
       <formula>"Siker"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K19">
-    <cfRule type="cellIs" dxfId="16" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="17" operator="equal">
       <formula>"Nem futtatható"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K19">
-    <cfRule type="cellIs" dxfId="15" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="18" operator="equal">
       <formula>"Hiba"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K20">
-    <cfRule type="cellIs" dxfId="14" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="13" operator="equal">
       <formula>"Siker"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K20">
-    <cfRule type="cellIs" dxfId="13" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="14" operator="equal">
       <formula>"Nem futtatható"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K20">
-    <cfRule type="cellIs" dxfId="12" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="15" operator="equal">
       <formula>"Hiba"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K21">
-    <cfRule type="cellIs" dxfId="11" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="10" operator="equal">
       <formula>"Siker"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K21">
-    <cfRule type="cellIs" dxfId="10" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="11" operator="equal">
       <formula>"Nem futtatható"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K21">
-    <cfRule type="cellIs" dxfId="9" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="12" operator="equal">
       <formula>"Hiba"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K22">
-    <cfRule type="cellIs" dxfId="8" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="7" operator="equal">
       <formula>"Siker"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K22">
-    <cfRule type="cellIs" dxfId="7" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="8" operator="equal">
       <formula>"Nem futtatható"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K22">
-    <cfRule type="cellIs" dxfId="6" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="9" operator="equal">
       <formula>"Hiba"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K23">
-    <cfRule type="cellIs" dxfId="5" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="4" operator="equal">
       <formula>"Siker"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K23">
-    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="5" operator="equal">
       <formula>"Nem futtatható"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K23">
-    <cfRule type="cellIs" dxfId="3" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="6" operator="equal">
       <formula>"Hiba"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K24">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="1" operator="equal">
       <formula>"Siker"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K24">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="2" operator="equal">
       <formula>"Nem futtatható"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K24">
-    <cfRule type="cellIs" dxfId="0" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="3" operator="equal">
       <formula>"Hiba"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -12164,17 +12015,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
+      <selection pane="bottomRight" activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="20.125" customWidth="1"/>
-    <col min="2" max="5" width="22.5" customWidth="1"/>
+    <col min="2" max="2" width="28.625" customWidth="1"/>
+    <col min="3" max="3" width="25.625" customWidth="1"/>
+    <col min="4" max="5" width="22.5" customWidth="1"/>
     <col min="6" max="26" width="7.625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -12193,12 +12046,16 @@
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15.75">
+    <row r="2" spans="1:5" ht="33.75" customHeight="1">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
+      <c r="B2" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>164</v>
+      </c>
       <c r="D2" s="5"/>
       <c r="E2" s="5"/>
     </row>
@@ -12206,8 +12063,12 @@
       <c r="A3" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
+      <c r="B3" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>156</v>
+      </c>
       <c r="D3" s="5"/>
       <c r="E3" s="5"/>
     </row>
@@ -12215,8 +12076,12 @@
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="5"/>
-      <c r="C4" s="5"/>
+      <c r="B4" s="16" t="s">
+        <v>169</v>
+      </c>
+      <c r="C4" s="16" t="s">
+        <v>170</v>
+      </c>
       <c r="D4" s="5"/>
       <c r="E4" s="5"/>
     </row>
@@ -12241,8 +12106,12 @@
       <c r="A6" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
+      <c r="B6" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>105</v>
+      </c>
       <c r="D6" s="5"/>
       <c r="E6" s="5"/>
     </row>
@@ -12250,8 +12119,12 @@
       <c r="A7" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
+      <c r="B7" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="D7" s="5"/>
       <c r="E7" s="5"/>
     </row>
@@ -12259,8 +12132,12 @@
       <c r="A8" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B8" s="5"/>
-      <c r="C8" s="5"/>
+      <c r="B8" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>166</v>
+      </c>
       <c r="D8" s="5"/>
       <c r="E8" s="5"/>
     </row>
@@ -12268,8 +12145,12 @@
       <c r="A9" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
+      <c r="B9" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="C9" s="16" t="s">
+        <v>49</v>
+      </c>
       <c r="D9" s="5"/>
       <c r="E9" s="5"/>
     </row>
@@ -12277,8 +12158,12 @@
       <c r="A10" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
+      <c r="B10" s="17">
+        <v>44745</v>
+      </c>
+      <c r="C10" s="17">
+        <v>44745</v>
+      </c>
       <c r="D10" s="5"/>
       <c r="E10" s="5"/>
     </row>
@@ -12320,8 +12205,12 @@
       <c r="A13" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B13" s="5"/>
-      <c r="C13" s="5"/>
+      <c r="B13" s="16" t="s">
+        <v>167</v>
+      </c>
+      <c r="C13" s="16" t="s">
+        <v>167</v>
+      </c>
       <c r="D13" s="5"/>
       <c r="E13" s="5"/>
     </row>
@@ -12329,17 +12218,25 @@
       <c r="A14" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B14" s="5"/>
-      <c r="C14" s="5"/>
+      <c r="B14" s="16" t="s">
+        <v>81</v>
+      </c>
+      <c r="C14" s="16" t="s">
+        <v>81</v>
+      </c>
       <c r="D14" s="5"/>
       <c r="E14" s="5"/>
     </row>
-    <row r="15" spans="1:5" ht="115.5" customHeight="1">
+    <row r="15" spans="1:5" ht="84">
       <c r="A15" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B15" s="5"/>
-      <c r="C15" s="5"/>
+      <c r="B15" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="C15" s="14" t="s">
+        <v>168</v>
+      </c>
       <c r="D15" s="5"/>
       <c r="E15" s="5"/>
     </row>
@@ -18255,62 +18152,62 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B6">
-    <cfRule type="cellIs" dxfId="74" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="1" operator="equal">
       <formula>"Alacsony"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B6">
-    <cfRule type="cellIs" dxfId="73" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="2" operator="equal">
       <formula>"Normál"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B6">
-    <cfRule type="cellIs" dxfId="72" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="3" operator="equal">
       <formula>"Magas"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C6:E6">
-    <cfRule type="cellIs" dxfId="71" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="4" operator="equal">
       <formula>"Alacsony"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C6:E6">
-    <cfRule type="cellIs" dxfId="70" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="5" operator="equal">
       <formula>"Normál"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C6:E6">
-    <cfRule type="cellIs" dxfId="69" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="6" operator="equal">
       <formula>"Magas"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B7">
-    <cfRule type="cellIs" dxfId="68" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="7" operator="equal">
       <formula>"Alacsony"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B7">
-    <cfRule type="cellIs" dxfId="67" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="8" operator="equal">
       <formula>"Normál"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B7">
-    <cfRule type="cellIs" dxfId="66" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="9" operator="equal">
       <formula>"Magas"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C7:E7">
-    <cfRule type="cellIs" dxfId="65" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="10" operator="equal">
       <formula>"Alacsony"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C7:E7">
-    <cfRule type="cellIs" dxfId="64" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="11" operator="equal">
       <formula>"Normál"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C7:E7">
-    <cfRule type="cellIs" dxfId="63" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="12" operator="equal">
       <formula>"Magas"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>